<commit_message>
Se hizo la tarea de Romberg
</commit_message>
<xml_diff>
--- a/Excel/Clase del 5 de Junio 2021.xlsx
+++ b/Excel/Clase del 5 de Junio 2021.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luis\Documents\GitProjects\Clases-octave\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clases-octave\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{379743B9-7A68-4D56-9334-B615C3D0CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2D0E23-8A09-4914-B40C-F06B55F2FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D81DC6F6-5971-4AE8-B7D0-7EECBFCFDD25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D81DC6F6-5971-4AE8-B7D0-7EECBFCFDD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Romberg" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>x</t>
   </si>
@@ -226,8 +227,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Entrada de lápiz 4">
@@ -246,7 +247,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Entrada de lápiz 4">
@@ -291,8 +292,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="6" name="Entrada de lápiz 5">
@@ -311,7 +312,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="6" name="Entrada de lápiz 5">
@@ -356,8 +357,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>2460</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="14" name="Entrada de lápiz 13">
@@ -376,7 +377,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="14" name="Entrada de lápiz 13">
@@ -421,8 +422,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Entrada de lápiz 14">
@@ -441,7 +442,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="15" name="Entrada de lápiz 14">
@@ -486,8 +487,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>162060</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="29" name="Entrada de lápiz 28">
@@ -506,7 +507,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="29" name="Entrada de lápiz 28">
@@ -551,8 +552,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>17700</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="30" name="Entrada de lápiz 29">
@@ -571,7 +572,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="30" name="Entrada de lápiz 29">
@@ -616,8 +617,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>76020</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="31" name="Entrada de lápiz 30">
@@ -636,7 +637,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="31" name="Entrada de lápiz 30">
@@ -681,8 +682,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="32" name="Entrada de lápiz 31">
@@ -701,7 +702,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="32" name="Entrada de lápiz 31">
@@ -746,8 +747,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="39" name="Entrada de lápiz 38">
@@ -766,7 +767,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="39" name="Entrada de lápiz 38">
@@ -811,8 +812,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>122580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="63" name="Entrada de lápiz 62">
@@ -831,7 +832,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="63" name="Entrada de lápiz 62">
@@ -876,8 +877,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>24180</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="70" name="Entrada de lápiz 69">
@@ -896,7 +897,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="70" name="Entrada de lápiz 69">
@@ -941,8 +942,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>43740</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="78" name="Entrada de lápiz 77">
@@ -961,7 +962,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="78" name="Entrada de lápiz 77">
@@ -1006,8 +1007,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>104940</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="102" name="Entrada de lápiz 101">
@@ -1026,7 +1027,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="102" name="Entrada de lápiz 101">
@@ -1071,8 +1072,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>17880</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="109" name="Entrada de lápiz 108">
@@ -1091,7 +1092,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="109" name="Entrada de lápiz 108">
@@ -1136,8 +1137,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="114" name="Entrada de lápiz 113">
@@ -1156,7 +1157,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="114" name="Entrada de lápiz 113">
@@ -1201,8 +1202,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>182520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="115" name="Entrada de lápiz 114">
@@ -1221,7 +1222,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="115" name="Entrada de lápiz 114">
@@ -1266,8 +1267,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="124" name="Entrada de lápiz 123">
@@ -1286,7 +1287,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="124" name="Entrada de lápiz 123">
@@ -1331,8 +1332,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="125" name="Entrada de lápiz 124">
@@ -1351,7 +1352,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="125" name="Entrada de lápiz 124">
@@ -1396,8 +1397,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="126" name="Entrada de lápiz 125">
@@ -1416,7 +1417,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="126" name="Entrada de lápiz 125">
@@ -1461,8 +1462,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="127" name="Entrada de lápiz 126">
@@ -1481,7 +1482,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="127" name="Entrada de lápiz 126">
@@ -1526,8 +1527,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>133800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId42">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="131" name="Entrada de lápiz 130">
@@ -1546,7 +1547,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="131" name="Entrada de lápiz 130">
@@ -1591,8 +1592,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>161580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId44">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="134" name="Entrada de lápiz 133">
@@ -1611,7 +1612,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="134" name="Entrada de lápiz 133">
@@ -1656,8 +1657,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>39480</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="137" name="Entrada de lápiz 136">
@@ -1676,7 +1677,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="137" name="Entrada de lápiz 136">
@@ -1721,8 +1722,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>176340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId48">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="144" name="Entrada de lápiz 143">
@@ -1741,7 +1742,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="144" name="Entrada de lápiz 143">
@@ -1786,8 +1787,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>69240</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId50">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="155" name="Entrada de lápiz 154">
@@ -1806,7 +1807,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="155" name="Entrada de lápiz 154">
@@ -1851,8 +1852,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId52">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="157" name="Entrada de lápiz 156">
@@ -1871,7 +1872,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="157" name="Entrada de lápiz 156">
@@ -1916,8 +1917,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>32520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId54">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="158" name="Entrada de lápiz 157">
@@ -1936,7 +1937,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="158" name="Entrada de lápiz 157">
@@ -1981,8 +1982,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>127980</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId56">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="169" name="Entrada de lápiz 168">
@@ -2001,7 +2002,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="169" name="Entrada de lápiz 168">
@@ -2046,8 +2047,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>177900</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId58">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="170" name="Entrada de lápiz 169">
@@ -2066,7 +2067,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="170" name="Entrada de lápiz 169">
@@ -2111,8 +2112,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>176520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId60">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="173" name="Entrada de lápiz 172">
@@ -2131,7 +2132,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="173" name="Entrada de lápiz 172">
@@ -2176,8 +2177,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>98340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId62">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="183" name="Entrada de lápiz 182">
@@ -2196,7 +2197,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="183" name="Entrada de lápiz 182">
@@ -2241,8 +2242,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>124020</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId64">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="184" name="Entrada de lápiz 183">
@@ -2261,7 +2262,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="184" name="Entrada de lápiz 183">
@@ -2306,8 +2307,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>148740</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId66">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="193" name="Entrada de lápiz 192">
@@ -2326,7 +2327,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="193" name="Entrada de lápiz 192">
@@ -2371,8 +2372,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>101580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId68">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="196" name="Entrada de lápiz 195">
@@ -2391,7 +2392,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="196" name="Entrada de lápiz 195">
@@ -2436,8 +2437,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>55860</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId70">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="197" name="Entrada de lápiz 196">
@@ -2456,7 +2457,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="197" name="Entrada de lápiz 196">
@@ -2501,8 +2502,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId72">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="198" name="Entrada de lápiz 197">
@@ -2521,7 +2522,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="198" name="Entrada de lápiz 197">
@@ -2566,8 +2567,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>181020</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId74">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="199" name="Entrada de lápiz 198">
@@ -2586,7 +2587,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="199" name="Entrada de lápiz 198">
@@ -2680,8 +2681,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>93960</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Entrada de lápiz 7">
@@ -2700,7 +2701,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="8" name="Entrada de lápiz 7">
@@ -2745,8 +2746,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="10" name="Entrada de lápiz 9">
@@ -2765,7 +2766,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="10" name="Entrada de lápiz 9">
@@ -2810,8 +2811,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Entrada de lápiz 15">
@@ -2830,7 +2831,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Entrada de lápiz 15">
@@ -2875,8 +2876,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>68520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="20" name="Entrada de lápiz 19">
@@ -2895,7 +2896,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="20" name="Entrada de lápiz 19">
@@ -2940,8 +2941,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>58800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="26" name="Entrada de lápiz 25">
@@ -2960,7 +2961,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="26" name="Entrada de lápiz 25">
@@ -3005,8 +3006,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>112140</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="29" name="Entrada de lápiz 28">
@@ -3025,7 +3026,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="29" name="Entrada de lápiz 28">
@@ -3070,8 +3071,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="35" name="Entrada de lápiz 34">
@@ -3090,7 +3091,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="35" name="Entrada de lápiz 34">
@@ -3135,8 +3136,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>76380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="53" name="Entrada de lápiz 52">
@@ -3155,7 +3156,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="53" name="Entrada de lápiz 52">
@@ -3200,8 +3201,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>171480</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="54" name="Entrada de lápiz 53">
@@ -3220,7 +3221,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="54" name="Entrada de lápiz 53">
@@ -3402,8 +3403,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>104760</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="11" name="Entrada de lápiz 10">
@@ -3422,7 +3423,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="11" name="Entrada de lápiz 10">
@@ -3467,8 +3468,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>178440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="14" name="Entrada de lápiz 13">
@@ -3487,7 +3488,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="14" name="Entrada de lápiz 13">
@@ -3532,8 +3533,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>154620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Entrada de lápiz 14">
@@ -3552,7 +3553,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="15" name="Entrada de lápiz 14">
@@ -3597,8 +3598,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>159660</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Entrada de lápiz 15">
@@ -3617,7 +3618,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Entrada de lápiz 15">
@@ -3662,8 +3663,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>29580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="24" name="Entrada de lápiz 23">
@@ -3682,7 +3683,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="24" name="Entrada de lápiz 23">
@@ -3727,8 +3728,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>83340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="32" name="Entrada de lápiz 31">
@@ -3747,7 +3748,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="32" name="Entrada de lápiz 31">
@@ -3792,8 +3793,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>180900</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="36" name="Entrada de lápiz 35">
@@ -3812,7 +3813,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="36" name="Entrada de lápiz 35">
@@ -3857,8 +3858,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>162960</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="48" name="Entrada de lápiz 47">
@@ -3877,7 +3878,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="48" name="Entrada de lápiz 47">
@@ -3922,8 +3923,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>64380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="52" name="Entrada de lápiz 51">
@@ -3942,7 +3943,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="52" name="Entrada de lápiz 51">
@@ -3987,8 +3988,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>187080</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="56" name="Entrada de lápiz 55">
@@ -4007,7 +4008,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="56" name="Entrada de lápiz 55">
@@ -4052,8 +4053,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>181560</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="58" name="Entrada de lápiz 57">
@@ -4072,7 +4073,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="58" name="Entrada de lápiz 57">
@@ -4117,8 +4118,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>145620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="59" name="Entrada de lápiz 58">
@@ -4137,7 +4138,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="59" name="Entrada de lápiz 58">
@@ -4182,8 +4183,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>142740</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="66" name="Entrada de lápiz 65">
@@ -4202,7 +4203,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="66" name="Entrada de lápiz 65">
@@ -4247,8 +4248,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>165060</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="69" name="Entrada de lápiz 68">
@@ -4267,7 +4268,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="69" name="Entrada de lápiz 68">
@@ -4312,8 +4313,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>25020</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="70" name="Entrada de lápiz 69">
@@ -4332,7 +4333,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="70" name="Entrada de lápiz 69">
@@ -4377,8 +4378,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>7440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="73" name="Entrada de lápiz 72">
@@ -4397,7 +4398,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="73" name="Entrada de lápiz 72">
@@ -4442,8 +4443,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>26160</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="77" name="Entrada de lápiz 76">
@@ -4462,7 +4463,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="77" name="Entrada de lápiz 76">
@@ -4507,8 +4508,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>189300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="84" name="Entrada de lápiz 83">
@@ -4527,7 +4528,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="84" name="Entrada de lápiz 83">
@@ -4572,8 +4573,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="87" name="Entrada de lápiz 86">
@@ -4592,7 +4593,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="87" name="Entrada de lápiz 86">
@@ -4637,8 +4638,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="97" name="Entrada de lápiz 96">
@@ -4657,7 +4658,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="97" name="Entrada de lápiz 96">
@@ -4702,8 +4703,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>38580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId42">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="98" name="Entrada de lápiz 97">
@@ -4722,7 +4723,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="98" name="Entrada de lápiz 97">
@@ -4767,8 +4768,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId44">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="105" name="Entrada de lápiz 104">
@@ -4787,7 +4788,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="105" name="Entrada de lápiz 104">
@@ -4832,8 +4833,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>106080</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="106" name="Entrada de lápiz 105">
@@ -4852,7 +4853,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="106" name="Entrada de lápiz 105">
@@ -4897,8 +4898,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>116040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId48">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="107" name="Entrada de lápiz 106">
@@ -4917,7 +4918,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="107" name="Entrada de lápiz 106">
@@ -4962,8 +4963,8 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>49380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId50">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="110" name="Entrada de lápiz 109">
@@ -4982,7 +4983,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="110" name="Entrada de lápiz 109">
@@ -5027,8 +5028,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>171540</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId52">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="114" name="Entrada de lápiz 113">
@@ -5047,7 +5048,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="114" name="Entrada de lápiz 113">
@@ -5092,8 +5093,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>90840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId54">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="123" name="Entrada de lápiz 122">
@@ -5112,7 +5113,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="123" name="Entrada de lápiz 122">
@@ -5157,8 +5158,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>141600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId56">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="136" name="Entrada de lápiz 135">
@@ -5177,7 +5178,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="136" name="Entrada de lápiz 135">
@@ -5222,8 +5223,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>58440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId58">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="141" name="Entrada de lápiz 140">
@@ -5242,7 +5243,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="141" name="Entrada de lápiz 140">
@@ -5287,8 +5288,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>76380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId60">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="142" name="Entrada de lápiz 141">
@@ -5307,7 +5308,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="142" name="Entrada de lápiz 141">
@@ -5395,8 +5396,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>19860</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId61">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="168" name="Entrada de lápiz 167">
@@ -5415,7 +5416,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="168" name="Entrada de lápiz 167">
@@ -5460,8 +5461,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>128760</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId63">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="189" name="Entrada de lápiz 188">
@@ -5480,7 +5481,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="189" name="Entrada de lápiz 188">
@@ -5525,8 +5526,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>123780</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId65">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="190" name="Entrada de lápiz 189">
@@ -5545,7 +5546,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="190" name="Entrada de lápiz 189">
@@ -5590,8 +5591,8 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>143160</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId67">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="191" name="Entrada de lápiz 190">
@@ -5610,7 +5611,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="191" name="Entrada de lápiz 190">
@@ -5655,8 +5656,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>124500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId69">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="202" name="Entrada de lápiz 201">
@@ -5675,7 +5676,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="202" name="Entrada de lápiz 201">
@@ -5720,8 +5721,8 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>52440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId71">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="208" name="Entrada de lápiz 207">
@@ -5740,7 +5741,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="208" name="Entrada de lápiz 207">
@@ -5785,8 +5786,8 @@
       <xdr:row>43</xdr:row>
       <xdr:rowOff>126840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId73">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="223" name="Entrada de lápiz 222">
@@ -5805,7 +5806,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="223" name="Entrada de lápiz 222">
@@ -5850,8 +5851,8 @@
       <xdr:row>47</xdr:row>
       <xdr:rowOff>164220</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId75">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="226" name="Entrada de lápiz 225">
@@ -5870,7 +5871,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="226" name="Entrada de lápiz 225">
@@ -5915,8 +5916,8 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId77">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="236" name="Entrada de lápiz 235">
@@ -5935,7 +5936,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="236" name="Entrada de lápiz 235">
@@ -5965,6 +5966,105 @@
         </xdr:pic>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>743585</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>101046</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C16F78B4-5BEE-4CC8-91EB-71A5948F617C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="91440"/>
+          <a:ext cx="4705985" cy="558246"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{897B5A7A-672B-4FE2-A005-74AA6564D9BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2057400" y="3078480"/>
+          <a:ext cx="7543800" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6021,22 +6121,22 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">265 1350,'-1'-83,"11"-246,-5 284,2 1,2 0,1 0,3 1,25-58,-22 62,3 1,1 0,37-52,-49 80,1 0,0 0,0 1,1 0,0 0,0 1,1 1,0 0,0 0,1 1,0 0,0 1,1 1,-1 0,24-5,43 5,-56 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="823">133 821,'4'0,"6"0,7 0,8 0,5 0,2 0,4 0,10 0,1 0,2 0,-3 0,-5 0,-4 0,-5 0,-7 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1846">1535 344,'-18'1,"0"1,1 0,-1 1,1 1,-28 10,-79 39,111-47,-45 22,-65 43,97-54,1 1,1 1,1 1,-35 39,53-53,1 0,0 0,0 1,0-1,1 1,0 0,1 0,-1 0,1 1,1-1,-1 0,1 8,0 10,1 0,4 32,0-3,-3-39,0-1,1 1,0-1,1 0,1 0,1 0,0 0,0-1,1 0,1 0,0 0,1-1,0 0,1-1,1 1,0-2,0 1,1-2,0 1,0-1,18 10,-9-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3187">1615 794,'-1'-1,"1"-1,-1 1,1-1,-1 0,1 1,-1-1,0 1,0 0,0-1,0 1,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,-1-1,-36-18,25 14,-3-2,-1-1,0 2,-1 1,1 0,-1 1,0 1,-1 1,1 0,-36 1,49 3,1 1,1-1,-1 1,0 0,0 0,1 1,-1-1,1 1,0 0,-1 0,2 1,-1-1,0 1,1 0,-1 0,1 0,0 0,0 1,1-1,0 1,-1 0,0 5,-4 7,0 1,2 0,0 1,-4 31,8-44,1 0,-1 0,1 0,0 0,0 0,1 0,0 0,0 0,0 0,1-1,0 1,0 0,0-1,1 1,0-1,0 0,0 0,0 0,9 9,-2-6,-1 0,2-1,-1-1,1 0,0 0,0-1,0 0,22 6,-23-8,110 29,-107-29,-1-1,1-1,-1 0,1-1,0 0,-1-1,22-4,-30 4,0-1,0 0,1 0,-1 0,-1-1,1 1,0-1,-1 0,1 0,-1 0,0-1,0 1,0-1,0 0,-1 0,1 0,-1 0,0 0,-1 0,1 0,-1-1,1 1,-1-1,-1 1,1-1,0 1,-1-9,0 5,0-1,0 0,0 1,-1-1,0 1,-1-1,0 1,-1-1,1 1,-1 0,-1 0,0 1,0-1,-5-7,-12-8,-1 1,-34-25,34 29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4177.99">1879 0,'5'1,"1"0,-1 0,1 0,-1 1,0 0,1 0,-1 0,0 0,0 1,0 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,-1 1,1-1,-1 1,0-1,0 1,4 7,6 14,-1 0,-1 1,7 29,-11-35,-1-2,63 212,-61-192,-1 1,-2-1,-2 1,-1 42,-2 27,2-68,-2 1,-2 0,-7 41,2-60,-1-1,-1 1,-1-1,0-1,-26 37,-8 18,6-7,19-43</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7396">1032 1694,'-1'14,"0"0,-1-1,0 1,-1-1,0 0,-1 0,-10 22,-5 3,-28 41,32-56,1 0,1 1,1 0,1 1,-12 40,19-41,1 0,1 0,1 1,1-1,2 0,0 1,6 27,-3-32,1-1,1-1,1 1,0-1,17 27,-9-21</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8872">1482 2117,'-4'-3,"0"1,0-1,0 0,-1 1,1 0,0 0,-1 0,0 1,1 0,-1 0,0 0,-7-1,-66 0,54 2,14 0,0 0,0 1,0 0,0 1,1 0,-1 0,0 1,1 1,-1-1,1 1,0 1,0 0,1 0,-1 1,1 0,1 0,-1 1,-8 10,9-9,0 1,1 1,1-1,0 1,0 0,1 0,0 1,1-1,0 1,0 0,1 0,1 0,0 0,0 0,1 0,2 18,-1-25,0 1,0 0,0 0,0-1,1 1,0 0,0-1,0 0,0 1,1-1,-1 0,1 0,0 0,1-1,-1 1,1-1,-1 0,1 0,0 0,0 0,0 0,1-1,-1 0,1 0,-1 0,8 1,-5-1,0 0,1-1,-1 0,0-1,0 0,1 0,-1 0,0-1,1 0,-1 0,0-1,0 0,0 0,0-1,-1 0,1 0,8-6,-5 3,-1-1,1-1,-2 0,1 0,-1-1,0 0,-1 0,0-1,-1 0,0 0,5-12,-5 7,0-1,-1 0,-1 0,-1-1,0 0,-1 1,-1-22,-1 14</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5483.99">159 2435,'13'10,"-10"-17,-12-26,-13-32,3 0,3-1,3-1,3-1,3 1,3-1,8-127,-3 190,-1 1,1-1,0 1,0 0,1 0,-1-1,1 1,0 0,0 0,0 1,1-1,-1 0,1 1,0-1,0 1,0 0,0 0,1 0,-1 1,1-1,0 1,0 0,0 0,6-3,3 1,0 1,0 0,0 0,0 1,0 1,26 1,-16 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6417.99">1 2144,'4'0,"11"0,11 0,16 0,4 0,-1 0,-3 0,-5 5,-8 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9934">1615 2461,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11052.99">1958 1879,'4'5,"2"10,0 7,-1 9,-2 13,-1 7,-5 0,-3-4,-4-1,-5-4,0-5,2-4,8-7,15-9,8-7,8-5,-3-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11961.03">2170 1932,'1'155,"-3"162,-11-200,0 33,13-78,0-43</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13053.03">2329 1456,'4'1,"1"0,-1-1,1 2,-1-1,0 0,1 1,-1 0,0 0,0 0,0 0,0 1,3 3,43 39,-22-15,-2 1,-1 2,-2 0,-1 2,-2 0,-1 1,-2 1,-2 1,-1 0,-2 1,-1 1,8 68,-10-41,6 40,0 127,-15-215,-8 170,5-167,-1 0,-1 0,-1 0,-1 0,-1-1,-15 29,-67 104,73-125</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14275.99">80 4154,'1'0,"0"0,0-1,0 1,0-1,0 1,-1-1,1 0,0 1,0-1,0 0,0 0,-1 1,1-1,0 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1-2,9-31,-8 25,13-53,-4 0,5-74,-4 30,1 40,3 1,3 1,41-98,-28 81,-25 64,1 0,0 1,1 0,1 1,0 0,1 0,0 1,2 1,17-16,-24 23,0 1,0 0,1 1,-1-1,1 1,0 1,0-1,1 1,-1 0,1 1,-1 0,1 0,0 1,0 0,0 0,0 1,-1 0,1 0,0 1,0 0,0 0,0 1,8 2,12 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14941.99">239 3599,'0'5,"4"1,6-1,11 0,6-2,3 4,0 0,1-1,3-1,0-2,0-1,-2-1,-7-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16062.99">1191 3096,'-6'6,"2"0,-1 1,1-1,0 1,0 0,-3 7,-5 10,-27 44,-111 219,101-185,34-74,1 1,2 0,0 1,2 0,-7 35,10-12,3-1,2 1,9 105,-5-151,0 0,1 0,-1 0,1 0,1 0,-1-1,1 0,0 1,0-1,1-1,0 1,0-1,1 1,-1-2,9 7,4 2,0-1,0 0,1-1,20 7,-15-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">273 1297,'-1'-80,"12"-236,-6 273,2 1,2-1,2 1,2 1,26-56,-22 59,2 2,2-1,38-49,-51 76,1 1,1-1,-1 1,1 1,0-1,1 1,0 2,0-1,1 0,0 1,1 1,-1 0,1 1,0 0,24-4,44 4,-57 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="823">137 789,'4'0,"7"0,6 0,9 0,5 0,2 0,4 0,10 0,2 0,1 0,-2 0,-6 0,-4 0,-5 0,-7 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1846">1583 331,'-18'0,"-1"2,2 0,-2 1,2 1,-30 10,-81 36,115-44,-47 21,-67 41,100-51,2 0,0 1,1 1,-36 38,55-51,1 0,0-1,0 2,0-1,0 1,1-1,1 1,-1 0,1 0,1 0,-1 0,1 7,0 10,1 0,4 31,0-3,-3-38,0 0,1 0,0 0,2-1,0 1,1-1,0 1,0-2,1 1,2-1,-1 1,1-2,0 1,2-2,0 2,0-3,1 2,0-2,0 0,1 0,17 9,-8-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3187">1666 763,'-1'-1,"1"-1,-1 1,1-1,-1 0,1 1,-1-1,0 1,0 0,0-1,0 2,0-2,0 1,0 0,0 0,-1 0,0 0,1 0,0 0,-1 0,-1-1,-37-17,26 13,-4-2,-1 0,1 1,-2 1,2 0,-2 2,0 0,0 1,0 0,-36 1,49 3,2 1,1-1,-1 1,0 0,0 0,0 1,0-2,1 2,0 0,-1 0,2 1,-1-1,0 1,0 0,0-1,1 1,0 0,0 1,1-1,0 1,-1-1,0 6,-4 6,-1 2,3-1,0 1,-4 30,8-42,1 0,-1-1,1 1,0 0,0 0,1 0,0-1,0 1,0 0,1-1,0 0,0 1,0-1,1 1,0-1,0-1,0 1,0 0,10 8,-3-5,-1 0,3-2,-2 0,1 0,1 0,-1-1,1-1,22 7,-24-8,114 28,-111-29,-1 0,2-1,-2 0,2-1,-1 0,-1-1,23-3,-30 3,-1-1,0 0,1 0,-1 0,-1-1,1 1,0-1,0 0,0 0,-1 1,0-2,0 1,0-1,0 0,-1 0,1 0,-1 1,0-1,0 0,0 0,-1-1,1 1,-1 0,-1 0,1-1,0 1,-1-8,0 4,0-1,0 1,0 0,-1-1,0 2,-1-2,0 1,-2 0,2 0,-1 0,-1 1,0 0,0-1,-5-6,-13-8,-1 1,-34-25,34 29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4177.99">1938 0,'5'1,"2"0,-2 0,1 0,-1 1,0 0,1 0,0 0,-1-1,0 2,0 0,-1 0,1 0,-1 1,2-1,-2 1,0-1,-1 2,1-1,-1 1,0-1,0 0,5 8,5 13,-1 0,0 1,6 28,-10-34,-2-2,65 204,-63-184,-1 0,-1-1,-3 2,-1 40,-2 25,2-64,-2 0,-2 1,-8 38,3-57,-1 0,-1 0,-2-1,1-1,-27 36,-9 17,7-7,20-41</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7396">1065 1628,'-2'13,"1"1,-1-2,0 1,-1 0,0-1,-1 1,-10 21,-6 2,-29 40,34-54,1 0,0 1,2 0,0 1,-11 39,19-40,0 0,2 0,1 1,1-1,2 0,1 1,5 26,-3-31,1 0,1-2,2 1,-1-1,18 27,-10-21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8872">1529 2034,'-4'-3,"-1"1,1-1,0 0,-1 2,1-1,0 0,-1 0,-1 1,2 0,-1 0,0 0,-7-1,-69 0,56 2,15 0,0 0,-1 1,1 0,0 1,1 0,-2 0,1 1,1 1,-2-2,2 2,0 1,-1 0,2 0,-1 0,1 1,0 0,0 1,-8 9,9-8,-1 0,2 2,1-1,0 0,0 1,1-1,-1 2,2-1,0 0,0 1,1-1,1 1,0-1,0 1,1 0,2 16,-1-23,0 1,0 0,0 0,0-1,1 0,0 1,0-1,0 0,0 1,2-2,-2 1,1 0,0 0,1-1,-1 1,1-1,-1-1,1 1,1 0,-1 0,0 0,1-1,-1 0,1 0,-1 0,9 1,-6-1,0-1,1 0,0 0,-1-1,0 0,1 0,0 0,-1-1,1 0,-1 0,0 0,1-1,-1 0,0-1,-1 0,2 0,7-6,-5 4,0-2,0-1,-2 1,1-1,0-1,-1 1,-1-1,0-1,0 1,-1-1,5-11,-5 7,0-2,0 1,-2-1,-1 0,0 0,-1 0,-1-20,-1 13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5483.99">164 2340,'13'9,"-10"-16,-12-24,-13-32,2 1,3-2,4 0,3-1,2 0,4 0,8-122,-3 182,-1 1,2-1,-1 1,0 1,1-1,-1-1,1 1,0 0,0 0,0 1,1 0,-1-1,1 1,0-1,0 1,0 0,1 0,0 1,-1 0,1-1,0 1,0 0,0 0,7-3,2 1,0 1,1 1,-1-1,1 1,-1 1,27 1,-16 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6417.99">1 2060,'4'0,"12"0,10 0,18 0,3 0,0 0,-4 0,-5 5,-8 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9934">1666 2365,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11052.99">2020 1805,'4'5,"2"10,0 6,-1 9,-2 12,0 7,-7 0,-2-4,-4-1,-6-4,1-4,2-4,7-7,17-9,7-6,9-6,-3-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11961.03">2238 1856,'1'149,"-3"156,-11-193,0 32,13-74,0-43</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13053.03">2402 1399,'5'1,"0"0,-1-1,1 2,-1-1,0 0,1 1,0 0,-1-1,0 1,0 0,0 1,3 3,45 37,-23-14,-2 1,-2 2,-1-1,-1 3,-3-1,0 2,-3 1,-1 0,-2 1,-1 0,-2 2,9 64,-11-38,6 37,1 123,-16-206,-8 162,5-160,-2 0,0 1,-1-1,-1 0,-1-1,-16 28,-69 100,76-120</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14275.99">82 3991,'2'0,"-1"0,0-1,0 1,0-1,0 1,-1-1,1 0,0 1,0-1,0 0,0 0,-1 1,1 0,0-1,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1-2,9-30,-8 25,14-52,-5 0,6-70,-5 28,2 39,2 0,4 2,42-95,-29 78,-26 62,1-1,0 2,2 0,0 0,0 1,2-1,-1 2,2 1,18-16,-25 22,1 1,-1 0,1 1,-1 0,1 0,1 1,-1-1,1 1,-1 0,2 1,-2 0,1 1,0 0,1 0,-1 0,0 1,-1 0,2 0,-1 1,0 0,0 0,1 0,7 3,13 9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14941.99">247 3458,'0'5,"4"1,6-2,12 1,5-2,4 4,0-1,1 0,3-1,0-2,1-1,-3-1,-8-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16062.99">1229 2975,'-7'5,"3"1,-1 1,1-1,0 0,0 1,-4 7,-4 9,-28 42,-115 211,105-178,34-71,2 1,1-1,1 2,2 0,-8 33,11-11,3-1,2 1,9 101,-5-145,0 0,1-1,-1 1,1 0,1-1,-1 0,2 0,-1 1,0-2,1 0,0 1,0-1,1 1,0-3,8 8,5 2,-1-2,1 1,0-2,22 7,-17-7</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6064,7 +6164,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">347 291,'-21'0,"1"0,0 0,-1 1,-32 7,46-6,-1 0,1 1,0 0,-1 0,1 1,1-1,-1 2,1-1,-1 1,1 0,1 0,-11 12,3-1,2 1,0 0,0 1,2 0,0 0,1 1,1 0,1 1,-8 39,7-5,1 0,4 84,2-107,1-1,2 1,1-1,14 54,-14-72,0 0,2 1,-1-2,1 1,1-1,0 0,1 0,0-1,1 0,0-1,0 0,1 0,19 13,-13-11,1 0,0-1,0-1,1 0,35 10,-46-17,1 0,0-1,0 0,0-1,0 1,0-2,0 1,0-1,0 0,0-1,0 1,0-2,-1 1,1-1,-1 0,0-1,8-4,2-4,1-2,-2 1,0-2,-1 0,-1-1,0-1,23-35,-1-9,30-68,-53 103,-2-1,-2-1,0 0,-2 0,-1-1,5-53,-2-8,-2 32,-2-83,-5 136,-1-1,0 1,0 0,-1 0,1 0,-1 0,0 0,0 0,-1 0,0 1,0-1,0 1,0 0,0 0,-1 0,0 0,0 0,0 1,0 0,-1 0,1 0,-6-2,-12-7,-1 2,-1 1,-36-10,31 11,12 2,1 2,-1 0,0 1,0 1,0 1,0 0,-1 1,1 1,-28 4,23 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="625.96">1088 1111,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="625.95">1088 1111,'0'0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2075.96">1776 264,'-24'0,"0"1,1 2,-1 0,1 1,-31 10,44-12,1 2,0 0,0 0,0 0,1 1,0 1,0-1,0 1,0 1,1-1,0 1,0 1,1-1,0 1,-8 14,10-13,0 0,1 1,0 0,0-1,1 1,0 0,-1 21,6 74,0-61,-3-38,1 1,-1-1,1 1,1-1,-1 1,1-1,0 1,0-1,1 0,0 0,0 0,0-1,1 1,0-1,7 8,-1-5,-1 0,1-1,1 0,-1 0,1-1,0-1,18 7,-16-8,1 0,-1-1,1-1,0 0,0 0,0-1,-1-1,1-1,0 0,0 0,0-2,-1 1,1-2,-1 0,0 0,0-2,0 1,-1-2,14-8,-18 10,1-1,-1 0,0 0,-1-1,1 0,-1 0,-1-1,0 0,0 0,0 0,-1-1,0 0,-1 0,0 0,0 0,-1-1,0 0,-1 0,0 1,0-1,-1-1,0 1,-1 0,-1 0,1 0,-5-19,3 22,-1-1,0 1,-1 0,1 0,-1 0,-1 1,1-1,-1 1,0 0,-1 0,0 1,1-1,-2 2,-11-9,-1 1,0 1,-1 0,0 2,-23-7,36 13,-1 0,1 1,-1 1,0-1,0 1,1 0,-1 1,-11 1,15-1,0 1,0 0,0 0,0 0,1 1,-1-1,0 1,0 0,1 0,0 0,-1 1,1-1,0 1,0 0,0-1,0 1,-2 4,-18 27</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3344.98">1670 846,'-2'6,"1"0,-1-1,0 1,0-1,-1 0,0 0,0 0,0 0,-6 7,-4 8,-35 61,-57 107,102-180,-1 0,1 0,1 0,0 0,0 1,0-1,1 1,0-1,1 1,0 0,0-1,1 1,2 10,-1-13,0 1,0-1,1 0,0 0,0 0,0 0,1-1,0 1,0-1,1 0,-1 0,1-1,0 1,0-1,1 0,-1 0,7 3,6 3,0-1,1 0,0-2,1 0,-1-1,1-1,1 0,34 2,-45-7,0 0,0 0,1-1,-1 0,0 0,0-1,0-1,0 0,-1 0,1-1,-1 0,1-1,-1 0,-1 0,1-1,-1 0,0 0,0-1,6-8,-4 3,-1 0,-1 0,0-1,0 0,-1 0,-1 0,0-1,-1 0,-1-1,0 1,-1-1,0 1,-2-1,1 0,-2 0,0 0,-3-26,0 30,0-1,-1 1,0 0,0 0,-1 1,-1-1,0 1,-12-16,-3 0,-42-42,56 61,-1 0,-1 0,1 1,-12-6,-3 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4371.96">2225 0,'0'6,"1"-1,0 0,0 0,1 0,0 0,0-1,0 1,5 8,6 13,29 84,130 301,-157-374,-1 0,-2 1,-2 0,-2 0,7 67,4 20,-8-66,-1 1,0 80,-10-115,-1 0,-1 0,-1-1,-1 1,-1-1,-2 1,0-2,-16 35,6-23,-2 0,-1-2,-1 0,-2-2,-1 0,-44 42,56-61</inkml:trace>
@@ -6127,26 +6227,26 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">588 768,'5'6,"-1"1,1-1,-1 1,0-1,-1 1,1 0,-2 0,1 1,-1-1,0 1,2 10,0 14,2 43,-5-56,-1 4,2 0,0-1,2 0,0 0,12 34,-9-42,0-14,1-25,-4-42,-4 31,-2 26,2 0,-1 0,2 0,-1 0,1 0,1 0,0 0,0 0,1 0,5-11,-7 19,1 0,1 0,-1 0,0 0,0 0,1 1,-1-1,1 1,-1-1,1 1,0 0,0 0,-1 0,1 1,0-1,0 1,0-1,0 1,0 0,0 0,0 0,-1 1,1-1,0 1,0-1,0 1,0 0,2 1,9 2,-1 1,0 0,0 1,17 11,-23-13,-1 0,1 1,-1-1,0 1,0 1,-1-1,0 1,0 0,0 0,-1 0,6 11,-6-8,-1 1,0-1,-1 0,0 1,0 0,-1-1,-1 1,0 17,0-25,0 22,-1-1,-1 1,-1-1,-8 29,10-48,0 1,0 0,-1-1,0 1,0-1,0 1,-1-1,1 0,-1 0,0 0,0 0,-1-1,1 1,-1-1,1 0,-1 0,0 0,-1 0,1-1,0 0,-1 0,1 0,-1 0,1-1,-1 1,0-1,-5 0,-14 1,0-1,-1-2,1 0,0-1,0-2,0 0,-29-11,22 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1266">1144 1191,'0'-4,"4"-2,6 0,6 1,10 2,4 1,6 1,2 0,-2 1,-1 0,-8 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2882.99">1673 979,'-13'0,"0"0,0 1,0 1,0 0,1 0,-24 8,30-7,0 0,0 0,1 0,-1 1,1 0,0 0,0 0,1 1,-1-1,1 1,0 0,0 0,0 1,1-1,-4 10,5-12,-10 23,-14 41,23-60,2-1,-1 0,1 0,0 1,0-1,0 1,1-1,0 1,1-1,-1 0,1 1,0-1,3 8,-2-10,1 0,-1 0,1-1,0 1,1-1,-1 1,0-1,1 0,0-1,0 1,-1 0,2-1,-1 0,0 0,0 0,1-1,-1 1,1-1,6 1,0 0,1 0,0 0,0-2,0 1,-1-1,20-3,-27 2,0 0,0-1,0 1,0-1,0 1,0-1,0-1,0 1,-1 0,1-1,-1 0,0 0,1 0,-2 0,1 0,0-1,0 1,-1-1,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,0-7,2-12,-1-1,0 1,-5-47,1 38,2 2,-1 14,-5 43,-3 20,2 1,2 1,3-1,3 54,0-98,-1-1,1 1,0-1,0 1,0-1,0 0,0 1,1-1,0 0,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,1-1,0 0,0 1,0-1,0-1,0 1,0 0,0-1,1 1,-1-1,0 0,1 0,-1-1,1 1,0-1,-1 1,1-1,-1 0,1 0,0-1,-1 1,1-1,-1 0,1 0,-1 0,0 0,1-1,2-1,7-8,-6-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3790.02">456 503,'-9'0,"-29"0,0 1,1 1,-41 9,67-8,-1 0,1 0,0 1,0 1,0 0,1 0,-1 1,1 1,1 0,-1 0,1 1,0 0,-14 17,12-10,0 0,1 1,1 0,1 0,0 1,1 0,1 1,0-1,1 1,-3 25,3 12,2-1,4 64,1-63,-1-35,0 0,2 0,0-1,1 1,1-1,1 0,1 0,0 0,2-1,0 0,1-1,0 0,2 0,0-2,25 27,-26-34,0-2,0 0,1 0,-1-1,1 0,0-1,0 0,1-1,-1-1,21 3,43 10,-67-12,202 56,-185-53</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4604">1858 476,'4'2,"0"-1,0 1,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0 0,0 0,0 0,0 1,4 5,2 4,-1 0,-1 0,0 1,-1 0,0 0,6 27,15 96,-18-83,2 8,9 42,-4 1,3 177,-19-258,-1 0,-6 35,5-50,-1 0,0 0,-1 0,1-1,-1 1,-1-1,0 0,0 0,-8 9,-11 9,2-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6443">2678 1164,'3139'0,"-2889"-11,-5 0,-74 16,-2 9,265 54,-359-58,-1-2,89-3,45 4,57 37,6 1,243 30,-39-5,-427-65,-42-4,-27-2,-19-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16099.34">3472 238,'-2'200,"4"217,-2-406,0 0,1 0,0 0,1-1,0 1,1 0,0-1,0 1,8 13,-11-23,0-1,0 0,0 1,0-1,1 0,-1 1,0-1,0 1,0-1,1 0,-1 0,0 1,0-1,1 0,-1 1,0-1,0 0,1 0,-1 0,0 1,1-1,-1 0,1 0,-1 0,0 0,1 0,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 0,1 0,-1 0,0-1,1 1,-1 0,0 0,1 0,7-17,-1-24,-6 13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16997.31">3472 185,'0'5,"4"1,6 0,11-1,11-2,8-1,7-5,-1-3,2 0,-3 1,-6 2,-3 0,-5 2,-2 0,-6 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17730.33">3313 529,'4'0,"11"0,8 0,17 0,24 0,11 0,1 0,-7 0,-12 0,-15-4,-10-2,-10 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18585.31">4186 159,'-13'170,"0"-23,11-76,4 262,2-311,2-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20350.33">4451 238,'0'496,"-1"-505,2 0,-1 1,1-1,1 0,-1 0,1 0,1 1,0-1,0 1,1 0,0 0,0 0,1 0,0 1,0 0,1 0,-1 0,2 1,-1 0,1 0,0 0,0 1,0 0,1 0,0 1,0 0,0 0,1 1,-1 0,1 1,11-3,-9 4,0 0,0 1,0 0,0 1,0 0,20 5,-28-5,-1 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 1,0-1,0 1,0 0,0 0,-1 0,1-1,0 2,-1-1,1 0,-1 0,0 0,0 1,1-1,-2 1,1-1,0 1,0-1,-1 1,0-1,1 1,-1-1,0 1,0 0,0-1,-1 1,0 3,0-2,0 0,0 0,0 0,-1 1,0-1,0 0,0-1,0 1,-1 0,1-1,-1 1,0-1,0 0,0 0,-1 0,1 0,-1-1,0 1,1-1,-1 0,0 0,0 0,0-1,-1 1,1-1,0 0,-6 0,-12 3,-1-1,0-2,-43-1,52-1,-12 1,3-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21154.3">4768 80,'6'0,"0"0,0 0,0 1,-1-1,1 1,0 0,0 1,0 0,-1 0,1 0,0 0,-1 1,0 0,0 0,0 0,0 1,0 0,-1 0,0 0,1 0,-2 1,1-1,0 1,5 10,4 10,-1 1,-1 0,-1 0,-1 1,-1 0,-2 1,0 0,1 46,-3 19,-11 120,5-191,0-1,-2 0,0 0,-1 0,-1 0,-1-1,-1 0,-1 0,0-1,-16 24,3-23,22-20,-1 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 1,0-1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,1-1,-1 1,0 0,1-1,-1 1,0 0,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,0 0,-6-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21904.31">5165 476,'4'0,"7"0,5 0,5 0,3 0,2 0,1 0,1 0,4 0,1 0,0 0,3 0,0 0,-1 0,-8 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22583.33">6197 212,'0'5,"0"10,-5 20,-1 14,-4 17,-1 0,2 4,3-1,1-4,3-4,1-8,0-25,2-19</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23223.31">6197 185,'4'0,"7"0,9 0,7 0,3 0,1 0,-1-4,0-2,-2 1,0 0,-5 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24030.31">6091 609,'4'0,"7"0,5-4,5-2,3 0,2 1,1 2,1 1,4-4,1 0,0 0,-1 2,-7 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24870.3">6964 53,'-1'12,"0"0,-1-1,-1 1,1-1,-2 1,1-1,-2 0,1-1,-8 13,-11 16,-30 37,20-30,20-26,1 0,1 0,1 1,0 1,2-1,1 1,0 1,1 0,2 0,0 0,2 0,0 0,3 30,-1-22,2-1,1 1,1-1,16 58,-15-74,-4-8,0 0,0-1,1 1,0-1,0 1,1-1,0 0,-1 0,2 0,-1 0,0-1,1 1,0-1,0 0,1 0,4 4,9-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26560.31">7176 476,'-10'1,"0"1,0-1,1 1,-1 1,1 0,0 0,0 1,0 0,0 0,-12 10,-11 8,-36 32,60-47,-25 19,-34 30,62-51,-1 1,1 0,1 0,-1 0,1 0,0 0,0 1,-4 11,7-15,1-1,0 1,0-1,0 1,0 0,0-1,1 1,-1-1,1 1,0-1,0 1,0-1,0 0,0 1,0-1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0-1,0 1,0-1,0 1,1-1,-1 0,0 1,4 0,6 4,-1-1,1 0,1 0,20 4,-23-7,1-1,-1 1,0-2,1 1,-1-2,1 1,10-3,-17 2,1 0,-1 0,0 0,0-1,-1 1,1-1,0 0,0 0,-1 0,1-1,-1 1,0-1,0 0,0 0,0 0,0 0,-1-1,1 1,-1-1,2-3,10-22,-1 0,-2-1,-1 0,-1 0,-2-1,-1 0,4-50,-17 54,2 27,0 16,-4 29,1-4,1 1,-1 46,8-85,0-1,-1 1,2 0,-1-1,0 1,0 0,1-1,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,1-1,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,3 1,11 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27563.31">7335 0,'1'18,"2"0,0 0,1 0,12 34,2 10,39 284,-51-252,-9 151,1-221,-2 0,0 1,-2-1,0-1,-2 1,-11 23,8-22</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29466.31">5245 1561,'1'-7,"1"0,0 0,1 0,-1 0,1 0,1 1,0-1,-1 1,2 0,-1 0,1 0,5-5,4-6,4-6,1 2,0 0,2 1,0 1,1 1,1 1,29-16,-34 22,2 2,-1 0,1 1,1 1,-1 1,1 0,0 2,0 0,1 2,26-1,-29 4,1-1,0 2,-1 1,0 0,0 1,0 1,0 1,-1 1,19 9,-28-10,0-1,-1 1,0 0,0 0,0 1,-1 1,0-1,-1 1,1 0,-1 0,-1 1,0 0,0 0,-1 0,0 0,0 1,-1 0,0-1,2 18,0 17,-1 0,-1 0,-3 1,-11 85,6-98,-1 0,-2 0,-1 0,-1-1,-2-1,-1 0,-27 45,26-54,-2-1,-1 0,0-1,-1-1,-1-1,-1 0,-1-2,0 0,0-1,-2-2,0 0,0-1,-38 12,58-22,-1 0,1 0,0 0,-1 0,1-1,-1 1,1-1,-1 0,1 0,-1-1,1 1,-1 0,1-1,0 0,-1 0,1 0,0 0,-1-1,1 1,0-1,0 0,0 0,-3-3,3 1,0 0,0 0,0-1,1 1,-1-1,1 0,0 0,1 0,-1 0,1 0,0 0,0 0,1 0,-1 0,1-6,6-197,-5 200,0 0,0 0,1 1,-1-1,2 0,-1 1,1-1,1 1,-1 0,1 0,8-11,-9 14,1 0,0 0,0 1,0-1,0 1,0 0,1 0,0 1,-1-1,1 1,0 0,0 0,0 1,1-1,-1 1,0 0,0 1,7-1,2 0,0 1,0 0,1 1,-1 0,0 1,0 1,0 0,0 1,0 1,-1 0,0 0,0 2,0-1,-1 2,0 0,0 0,-1 1,0 0,-1 1,15 17,-16-16,0-1,1 0,0-1,1 0,0-1,0 0,1 0,-1-1,2-1,-1 0,1-1,14 4,-1-3,1-1,0-1,0-1,1-1,29-3,59-1,-87 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">610 739,'5'6,"-1"1,1-1,-1 0,0 0,0 1,0 0,-2-1,1 2,-1-1,0 1,2 9,0 14,3 41,-6-54,-1 4,2 0,0 0,2-1,0 0,13 33,-10-41,0-13,1-24,-3-40,-5 29,-2 25,2 1,-1-1,2 1,-1-1,1 0,1 1,0-1,0 0,1 1,5-11,-7 18,1 0,1 0,-1 0,1 0,-1 0,1 1,-1-1,1 1,-1-1,1 1,0 0,0 0,-1 0,2 1,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,1 1,-1-1,0 1,0 0,2 1,10 2,-2 1,1 0,-1 1,18 10,-24-12,0 0,0 0,-1 0,0 1,1 1,-2-1,0 0,0 1,0 0,-1 0,7 10,-7-7,-1 0,0 0,-1 0,0 0,0 1,-1-1,-1 0,0 17,0-24,0 21,-1-1,-1 2,-1-2,-8 28,10-46,0 0,0 1,-1-1,0 1,0-1,-1 1,0-2,1 1,-1 0,0 0,0 0,-1-1,1 1,-1-2,0 1,0 0,0 0,-1 0,1-1,0 0,-2 0,2 0,-1 0,1-1,-1 1,0-1,-6-1,-14 2,0-1,0-2,0 0,0 0,0-3,0 0,-30-11,23 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1266">1186 1147,'0'-4,"4"-2,7 0,5 1,11 2,4 2,7 0,1 0,-2 1,0 0,-9 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2882.99">1735 942,'-14'0,"1"0,-1 1,1 1,-1 0,2 0,-25 8,30-7,1 0,0 0,1-1,-2 2,2 0,0 0,0 0,1 1,-1-2,0 2,1 0,0 0,0 1,1-2,-4 11,5-12,-11 22,-14 39,24-57,2-1,-1 0,1-1,0 2,0-1,0 1,1-2,0 2,1-1,-1 0,1 0,0 0,3 8,-2-10,1-1,-1 1,1-1,1 1,0-1,-1 1,0-1,1 0,0-2,0 2,-1 0,3-1,-2 0,0 0,0 0,1-1,-1 1,2-1,5 1,0 0,2 0,-1-1,1-1,-1 1,0-1,20-2,-28 1,0 0,0-1,0 1,0-1,1 1,-1-1,0-1,0 1,-1 0,1-1,-1 0,1 1,0-1,-2 0,1 0,0-1,0 1,-1-1,0 0,0 1,0-1,0 0,-1 0,2 0,-2 0,0 0,0-6,2-12,-1-1,0 0,-5-44,1 36,2 2,-1 14,-6 41,-2 19,2 1,2 2,3-2,3 52,0-94,-1-1,1 1,0-1,0 0,0 0,0 0,0 1,1-1,0 0,0 0,0 0,0-1,0 1,0 0,2-1,-2 1,1-1,0 0,0 1,0-1,0-1,0 1,0 0,1-2,0 2,-1-1,0 0,1 0,-1-1,1 1,0-1,0 1,0-1,-1 0,1 0,0-1,-1 1,1-1,-1 0,2 0,-2 0,0 0,1 0,2-2,8-8,-7-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3790.02">473 484,'-10'0,"-29"0,0 1,0 1,-42 9,70-8,-1-1,0 1,1 1,-1 1,1 0,1 0,-2 0,2 2,0 0,0 0,1 0,-1 1,-13 16,11-9,1-1,0 1,2 1,1-1,-1 2,2-1,1 1,0 0,1 0,-4 24,4 12,2-1,4 62,1-61,-1-34,0 0,2 1,0-2,2 1,0-1,1 1,1-1,0 0,3 0,-1-1,2-1,-1 1,2-1,1-1,25 25,-26-32,-1-3,0 1,2 0,-2-1,2 0,-1-2,1 1,0-1,-1-1,23 3,43 9,-68-11,209 54,-192-51</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4604">1927 458,'4'2,"0"-1,0 1,0 0,0 0,0 0,1 1,-2-1,1 1,-1-1,0 1,0 0,0 0,0 1,5 5,1 3,-1 1,0-1,-1 2,-1-1,0 1,7 25,15 93,-19-80,2 8,10 40,-4 1,2 170,-19-248,-1 0,-6 34,5-48,-1 0,0-1,-1 1,1-1,-2 0,0 0,0 0,0-1,-9 10,-10 8,1-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6443">2777 1121,'3255'0,"-2996"-11,-5 0,-77 16,-2 9,275 51,-372-55,-1-3,92-2,47 4,58 35,7 1,252 30,-40-6,-443-62,-44-4,-28-2,-19-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16099.34">3600 229,'-2'193,"4"208,-2-390,0-1,1 1,0-1,1 0,0 1,1-1,1 0,-1 0,8 14,-11-23,0-1,0 0,0 1,0-1,1 0,-1 0,0 0,0 1,0-1,1 0,-1 0,0 1,0-1,1 0,-1 1,0-1,0 0,1 0,-1 0,0 1,1-1,-1 0,1 0,-1 0,0 0,1 0,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 0,1 0,-1 0,0-1,1 1,-1 0,0 0,2 0,6-16,-1-24,-6 14</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16997.3">3600 178,'0'5,"4"1,7-1,10 0,13-2,7-1,8-5,-2-3,3 1,-3 0,-7 2,-2 0,-6 2,-2 0,-6 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17730.32">3435 509,'4'0,"12"0,8 0,17 0,26 0,10 0,2 0,-7 0,-13 0,-16-4,-9-1,-12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18585.3">4340 153,'-13'164,"0"-23,10-72,6 251,1-299,2-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20350.32">4615 229,'0'478,"-1"-487,2 0,-1 2,1-2,1 0,-1 1,1-1,2 1,-1 0,0 0,1 0,0 0,0 1,1-1,1 1,-1 1,1-1,-1 0,2 1,0 1,0-1,0 0,0 1,1 0,0 1,0 0,1 0,-1 0,1 1,0 0,0 1,12-3,-10 5,0-1,1 1,-1 0,1 1,-1-1,21 6,-29-5,-1 0,1 0,0 0,0 0,-1 0,0 0,1 0,-1 1,0-1,0 1,0 0,0 0,-1 0,1-1,0 1,-1 0,2 0,-2 0,0 0,0 1,1-1,-2 1,1-1,0 1,0-1,-1 0,0 0,1 1,-1-1,0 1,0 0,0-1,-1 1,0 3,0-3,0 1,0 0,0 0,-1 1,0-1,-1-1,1 0,0 1,-1 0,1-1,-1 1,0-1,0 0,0-1,-1 1,0 0,0-1,0 1,1-1,-1 0,0 0,0 0,-1-1,0 1,1-1,0 0,-6 0,-13 2,-1 0,0-2,-44-1,53-1,-12 1,3-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21154.3">4944 77,'6'0,"0"0,1 0,-1 1,-1-1,1 1,0 0,1 1,-1 0,-1 0,1 0,1 0,-2 0,0 1,0 0,0 0,0 1,1 0,-2 0,0-1,1 1,-2 1,1-1,1 1,4 9,4 10,0 1,-2 0,0 0,-2 1,-1 0,-2 1,1 0,0 45,-3 17,-11 116,5-184,0 0,-3-1,1 0,-1 0,-1 0,-1 0,-2-1,0 0,0-1,-17 24,3-23,23-19,-1 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 1,0-1,1 0,-1 0,0 0,1-1,-1 1,0 0,-1 0,2 0,-1 0,1-1,-1 1,0 0,1-1,-1 1,0 0,1-1,-1 1,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,0 0,-6-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21904.31">5356 458,'4'0,"7"0,6 0,5 0,2 0,3 0,1 0,1 0,5 0,0 0,0 0,3 0,1 0,-2 0,-8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22583.33">6426 204,'0'5,"0"9,-6 20,0 13,-4 17,-1-1,1 5,4-2,1-3,3-5,1-7,0-24,2-18</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23223.31">6426 178,'4'0,"7"0,10 0,7 0,3 0,1 0,-1-4,0-2,-2 2,1-1,-7 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24030.31">6316 586,'4'0,"7"0,6-4,5-1,3-1,2 1,1 2,1 1,4-4,1 1,0-1,-1 2,-7 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24870.3">7221 51,'-1'12,"0"-1,-1 0,-1 0,1 0,-2 0,0 0,-1 0,1-2,-8 13,-12 16,-31 35,21-29,20-24,2-1,0 0,2 1,0 2,1-2,2 1,0 1,1 0,1 0,1 0,2 1,0-1,3 29,-1-21,2-1,1 0,1 0,17 56,-16-72,-4-7,0 0,0-1,2 1,-1-2,0 2,1-1,0 0,-1 0,2-1,-1 1,0-1,1 1,1-1,-1 0,1-1,4 5,10-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26560.31">7441 458,'-11'1,"1"1,0-1,0 1,0 1,1 0,-1 0,1 1,0-1,-1 1,-11 10,-13 7,-36 31,62-45,-27 18,-34 29,64-50,-2 2,2 0,1 0,-1-1,1 1,0 0,0 1,-5 10,8-14,1-1,0 1,0-1,0 1,0-1,0 0,1 1,-1-1,1 1,0-1,0 1,0-1,0 0,0 1,0-1,1 0,0-1,-1 1,1 0,0 0,-1 0,1 0,0-1,0 1,0-1,0 1,1-1,-1 0,0 1,5 0,5 3,0 0,0 0,1 0,22 4,-25-8,1 0,0 1,-1-2,2 1,-2-2,1 1,11-3,-18 2,1 1,0-1,-1 0,0-1,-1 1,1-1,0 0,0 0,0 0,0-1,-1 1,0-1,0 0,0 1,0-1,0 0,-1-1,2 1,-2-1,2-3,10-21,0 1,-3-2,0 0,-2 0,-2-1,-1 0,5-48,-19 52,3 26,0 16,-4 27,0-4,2 2,-1 44,8-82,0-2,-1 2,2 0,-1-1,0 1,0 0,1-1,-1 1,1-1,0 1,0-2,0 2,0-1,0 1,1-1,-1 0,1 0,0 0,-1 0,2 0,-1 0,0 0,0-1,3 2,12 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27563.31">7606 0,'1'17,"2"1,0-1,1 0,13 33,1 10,41 273,-52-242,-10 145,0-213,-1 0,0 1,-2-1,0-1,-3 1,-10 22,7-21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29466.31">5439 1503,'1'-7,"1"0,0 1,1-1,-1 0,1 0,1 2,0-2,-1 1,3 0,-2 0,1 1,5-6,5-5,3-6,2 1,0 1,2 1,-1 1,2 0,1 2,30-16,-35 22,1 1,0 0,1 2,1 0,-2 1,2 0,0 2,0 1,1 1,26-1,-29 4,1-1,-1 2,0 1,0-1,0 2,-1 1,1 1,-1 1,19 8,-29-9,1-1,-2 0,0 1,1 0,-1 1,-1 0,0 0,0 1,0-1,-1 1,-1 1,0 0,1-1,-2 1,0 0,0 0,-1 1,0-2,2 18,1 17,-2-1,-1 0,-3 2,-11 81,5-94,0 0,-2-1,-2 1,0-1,-2-1,-2 0,-27 43,26-52,-1-1,-2 1,0-2,0-1,-2 0,-1-1,-1-1,1-1,-1-1,-2-1,0 0,0-2,-39 12,60-21,-1 0,1 0,0 0,-2 0,2-1,-1 1,1-1,-1 0,1 0,-1-1,1 1,-2 0,2-1,0 0,-1 0,1 0,0 0,-1-1,1 1,0-1,-1 1,1-1,-3-3,3 1,0 0,0 0,0-1,1 2,-2-2,2 0,0 0,1 0,-1 1,1-1,0 0,0 0,1 0,-1 0,1-5,6-190,-5 192,0 0,0 1,1 0,-1-1,3 0,-2 2,1-2,1 1,-1 0,1 1,9-12,-10 15,1-1,0 0,0 1,0-1,0 1,1 0,0 0,0 1,-1 0,1 0,0 0,1 0,-1 1,1-1,-1 1,0 0,1 1,6-1,3 0,-1 1,1 0,0 1,0 0,-1 1,1 1,-1 0,1 1,-1 0,0 1,-1 0,1 2,-1-1,0 1,-1 1,1 0,-2 0,0 1,0 1,15 16,-17-16,0 0,2-1,-1 0,1 0,1-2,-1 1,2 0,-2-1,3-2,-2 1,2-1,14 4,-2-4,2 0,0-1,0-1,1-1,31-3,60-1,-90 2</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6235,7 +6335,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'120'6,"166"29,52 3,415 58,-29-2,-650-93,123-17,-4 1,243 13,-413 0,-1-1,0-1,37-11,-35 7,-1 2,1 1,0 1,27-1,598 4,-376 2,-152-11,-16 0,60 10,0 7,0 7,261 56,-336-57,-73-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'124'6,"170"29,55 3,427 57,-30-1,-670-93,128-17,-6 1,252 13,-426 0,-2-1,1-1,38-11,-37 7,0 2,1 1,0 1,27-1,617 4,-388 2,-156-11,-17 0,62 10,1 7,-1 7,269 56,-347-57,-74-13</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6520,7 +6620,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">349 212,'-43'0,"22"-1,0 0,1 2,-1 1,0 0,-21 6,35-6,0 1,1 0,-1 0,1 0,0 1,0-1,0 2,0-1,1 1,-1-1,1 2,0-1,1 0,-1 1,1 0,0 0,1 0,-6 13,-1 4,1 0,1 1,1 0,2 1,0-1,1 1,2 0,0 0,2 0,2 26,0-35,0-1,2 0,-1 1,2-1,0-1,0 1,1-1,1 0,1 0,0-1,1 0,0 0,1-1,0 0,1-1,0 0,14 10,-7-8,0 0,0-2,1 0,1-1,25 9,-36-16,0 0,1-1,-1 0,1 0,-1-1,1-1,-1 1,1-2,-1 1,1-1,-1-1,1 0,-1 0,13-5,-16 4,-1 0,1-1,-1 0,0 1,0-2,0 1,-1-1,1 1,-1-1,0-1,0 1,-1 0,6-12,3-9,15-48,-23 64,6-20,-2-1,10-56,-17 72,0 1,-1-1,0 0,-1 1,-1-1,0 1,-1-1,-7-19,7 20,-2 1,0-1,0 1,-1 0,-1 0,0 1,-1 0,0 0,-1 1,0 0,-1 0,0 1,-1 1,0-1,-14-8,-8-4,21 13,-1 1,-1-1,1 2,-1 0,-22-8,14 10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="425.99">879 688,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="425.98">879 688,'0'0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1258.02">1275 0,'-1'9,"0"-1,0 1,-1-1,0 0,0 0,-1 0,0 0,-5 9,-40 64,23-41,15-24,2 1,0 0,1 0,0 0,2 1,0 0,-4 30,9-44,0-1,1 0,0 1,-1-1,1 0,0 0,1 0,-1 1,1-1,-1-1,1 1,0 0,0 0,0-1,0 1,1-1,-1 1,1-1,-1 0,1 0,0 0,0 0,0-1,0 1,0-1,5 2,12 5,0-2,42 10,-46-13,23 7,40 7,-58-16</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1663.99">1619 186,'0'9,"0"17,0 12,0 9,0 11,0 3,0 1,0-1,0 2,0-4,0-9,0-8,0 3,-5 2,-1-6</inkml:trace>
 </inkml:ink>
@@ -6549,12 +6649,12 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 318,'4'0,"29"-4,36-2,19-9,17-1,18 1,11 4,9-1,34-8,-7 0,-34 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="645.99">874 106,'-5'5,"-1"10,0 16,1 12,2 17,1 11,1 8,0 30,1 6,1-8,-1-13,0-18,0-12,0-14,1-10,-1-7,0-6,0-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1182.99">451 1218,'144'-29,"2"7,0 5,165 4,-281 13,-6-1,0 2,33 5,-31 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2363.99">1403 900,'4'0,"0"-1,0 0,1 0,-1 0,0-1,0 1,5-4,10-3,85-28,-12 4,159-35,-248 66,1 0,0 1,0-1,0 1,0 0,0 0,0 0,0 1,0-1,-1 1,8 2,-9-2,0 0,-1 1,1-1,0 1,0-1,-1 1,1 0,-1 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,-1 5,5 43,-2 0,-7 99,0-47,3-66,-1 1,-1-1,-3 1,-1-1,-1 0,-2-1,-20 48,23-70,0 0,-1-1,0 0,-1 0,-1-1,1 0,-2-1,1 0,-14 9,16-13,0-1,-1 0,1 0,-1-1,0 0,0 0,0-1,-1 0,1-1,-1 0,0-1,1 0,-1 0,-13-1,21 0,0-1,0 1,-1 0,1-1,0 0,0 1,-1-1,1 0,0 0,0 0,0 0,0-1,0 1,1 0,-1-1,0 1,1-1,-1 0,0 0,-1-3,1 1,0 1,1-1,-1 0,1 0,0 0,0 0,1 0,-1 0,1-1,0-7,0 4,1 0,0 0,1 0,-1 1,2-1,-1 0,1 1,0-1,0 1,1 0,8-12,-4 12,0 0,0 0,1 1,0 0,0 1,0 0,1 0,-1 1,1 0,0 1,1 0,-1 1,0 0,19-2,5 2,-1 1,1 2,45 6,-72-5,0-1,1 1,-1 0,0 1,0-1,0 2,-1-1,1 1,-1 0,10 7,2 5,32 37,-42-43,1 1,0-1,0-1,1 0,1 0,-1-1,1 0,0-1,1-1,20 10,-23-14,0 1,0-2,1 1,-1-1,0-1,1 1,-1-2,0 1,1-1,9-3,4-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3018.99">2276 0,'9'0,"21"0,18 0,16 0,19 0,13 0,3 0,0 0,-5 0,-8 0,-16 0,-18 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3594.99">2461 318,'4'0,"16"0,17 0,21 0,13 0,9 0,13 0,-4 0,-5 0,-12 0,-8 0,-12 0,-5 0,-6 0,-10 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 306,'4'0,"31"-4,37-2,21-8,17-2,20 2,11 3,9 0,36-9,-7 1,-36 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="645.99">919 102,'-5'5,"-2"9,1 16,1 11,2 17,1 10,0 8,1 29,1 5,1-7,-1-12,0-18,0-12,0-13,2-9,-2-8,0-5,0-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1182.99">474 1171,'152'-28,"1"7,1 4,173 5,-296 12,-6-1,1 2,34 5,-33-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2363.99">1475 865,'4'0,"1"-1,-1 0,1 0,-1 0,0-1,1 1,4-3,11-4,89-27,-12 4,167-33,-261 63,1 0,1 1,-1-1,0 1,0 0,0 0,1 0,-1 1,0-1,-1 1,9 2,-10-2,0 0,-1 1,1-1,0 1,0-1,-1 1,2 0,-2-1,1 1,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,-1 4,5 42,-1 0,-9 96,1-46,3-64,-1 2,-1-2,-3 2,-2-1,0-1,-3 0,-20 46,23-68,1 1,-1-2,-1 1,0-1,-2 0,2-1,-3 0,2 0,-16 8,18-12,0-2,-2 1,2 0,-2-1,1 0,-1 0,1-2,-2 1,2-1,-2 0,1-1,0 0,0 0,-14-1,22 0,-1-1,1 1,-1 0,1-1,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0-1,0 1,1 1,-1-2,0 1,1-1,-1 0,0 0,-2-3,2 1,0 1,1-1,-1 1,1-1,0 0,0 0,1 0,-1 0,1 0,0-8,0 4,1 1,0-1,1 0,-1 2,2-2,-1 0,2 1,-1 0,0 0,1 0,9-11,-5 11,1 1,-1-1,1 1,1 0,-1 2,1-1,0 0,0 1,0 0,1 1,0 0,0 2,-1-1,21-2,5 2,-2 1,2 2,47 6,-76-5,1-2,0 2,0 0,-1 1,0-1,1 2,-2-1,1 1,0 0,10 6,1 5,35 36,-45-41,2 1,-1-2,1 0,0 0,2-1,-2 0,2 0,0-2,0 0,22 9,-25-13,1 1,-1-2,2 1,-2-1,1-1,0 1,0-2,-1 1,2-1,9-3,4-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3018.99">2393 0,'10'0,"21"0,20 0,16 0,20 0,14 0,3 0,0 0,-5 0,-9 0,-16 0,-19 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3594.99">2588 306,'4'0,"17"0,18 0,22 0,13 0,10 0,14 0,-4 0,-6 0,-12 0,-9 0,-12 0,-6 0,-6 0,-10 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6581,7 +6681,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 4,'5453'0,"-5374"-1,-39-1,0 1,73 10,-87-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 4,'5694'0,"-5612"-1,-40-1,0 1,76 10,-91-3</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6608,19 +6708,19 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 423,'-1'37,"0"-18,1 1,3 26,-2-41,0 1,1 0,-1 0,1-1,0 1,1-1,-1 1,1-1,0 0,0 0,8 9,2-1,-2 1,1-2,0 1,0-2,1 0,1 0,0-1,1-1,21 11,122 38,-156-57,0-1,0 1,1-1,-1 1,0-1,1 0,-1 1,1-1,-1-1,0 1,1 0,-1 0,0-1,1 0,-1 1,0-1,0 0,0 0,1 0,-1 0,0 0,0-1,0 1,-1-1,1 1,0-1,-1 0,1 0,-1 1,1-1,-1 0,2-3,2-6,0-1,-1 0,0 0,0 0,1-14,3-9,6-9,-6 23,-1 0,-1-1,-1 0,-1 0,3-39,-7 56,-1 0,1 0,-1 0,0-1,0 1,0 0,-1 1,0-1,0 0,0 0,-1 1,1-1,-1 1,0 0,0 0,-1 0,1 0,-1 1,0-1,0 1,0 0,0 0,-1 0,1 1,-1 0,0-1,1 2,-1-1,0 0,-7 0,-24-4,-1 1,1 3,0 0,-1 3,-46 6,70-6,6-1,0 1,1 1,-1-1,1 1,0 0,-11 5,-4 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="419">823 793</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1597.05">955 423,'0'-1,"0"0,1 0,-1-1,1 1,0 0,-1 0,1 0,0-1,0 1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,2 0,30-17,-19 12,-5 0,1 1,0 0,1 1,-1 0,1 0,0 1,20-2,-29 4,1 1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 1,1 0,0-1,-1 1,1 0,-1 0,1 0,-1 0,0 1,0-1,1 1,-1-1,0 1,0 0,0 0,-1 0,1 0,0 0,-1 0,1 1,-1-1,0 0,0 1,0-1,0 1,0-1,0 1,-1-1,1 1,-1 2,4 19,-2-1,-1 0,-1 1,0-1,-2 0,-1 0,-1 1,0-2,-2 1,-15 37,19-56,0 0,-1-1,1 1,-1-1,0 1,0-1,0 0,0 0,-1 0,1-1,-1 1,0-1,1 0,-1 0,-5 2,6-3,0 0,0 0,0 0,1-1,-1 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 0,0 1,0-1,1 0,-1-1,0 1,1 0,-1-1,-3-2,6 4,-1 0,1-1,-1 1,1 0,-1-1,1 1,0 0,-1-1,1 1,0-1,-1 1,1 0,0-1,-1 1,1-1,0 1,0-1,0 1,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1 0,0-1,1 1,-1-1,0 1,1-1,-1 1,0 0,1-1,-1 1,1 0,0-1,26-8,-16 8,0 2,0-1,0 1,-1 1,1 0,0 1,-1 0,1 0,-1 1,13 7,14 9,47 33,-44-26,-4-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7001.66">1431 529,'59'-11,"1"3,0 2,94 3,-117 3,-34 0,1 0,-1 0,0 0,0 0,0 0,0 1,0 0,0-1,0 1,0 0,0 0,0 1,0-1,-1 1,1-1,0 1,-1 0,1 0,-1 0,0 0,4 5,-4-3,0 0,-1 0,1 0,-1 0,0 1,0-1,0 1,-1-1,1 1,-1-1,0 1,-1-1,1 0,-2 8,1-6,0-1,0 1,-1-1,0 0,0 1,0-1,0 0,-1 0,0 0,0-1,0 1,-1-1,0 0,0 1,0-2,0 1,0 0,-1-1,-8 5,4-3,1-2,-1 0,0 0,0 0,-1-1,1 0,0-1,-1 0,1-1,-17-1,31 2,-1 0,1-1,0 2,0-1,0 0,-1 1,1 0,-1 0,0 1,1-1,-1 1,0 0,0 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,0 0,-1 0,1 1,-1-1,0 0,0 1,2 9,-3-11,1 0,-1 1,-1-1,1 1,0 0,-1-1,1 1,-1 0,0-1,-1 1,1 0,0-1,-1 1,0-1,0 1,0-1,0 1,-1-1,1 0,-4 6,1-6,1 1,0-1,-1-1,1 1,-1 0,0-1,0 1,0-1,0 0,0-1,0 1,-1-1,1 0,0 0,-1 0,-5 0,-20 2,0-2,1-2,-1 0,0-2,1-1,-1-1,-30-11,54 14,0 0,1 0,0 0,-1-1,1 1,0-1,1-1,-10-6,0-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7002.66">2040 343,'20'0,"1"0,1 0,0 1,0 1,39 9,-56-9,0-1,1 1,-1 1,0-1,0 1,0 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,-1 1,1-1,-1 0,0 1,0 0,0 0,0 0,-1 0,0 0,0 1,2 9,1 16,-2 0,-1 0,-1 1,-1-1,-2 1,-9 49,10-75,-1 0,1 0,-1 0,0-1,-1 1,0 0,1-1,-1 1,-1-1,1 0,-1 0,0-1,0 1,-1-1,1 1,-1-1,0-1,0 1,0-1,-1 0,1 0,-1 0,-9 2,-1-1,1 0,-1-2,0 0,0-1,0 0,0-1,0-1,-16-3,29 4,1 0,-1-1,0 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-5-4,7 5,-1-1,1 0,-1 1,0-1,1 0,0 1,-1-1,1 0,-1 0,1 0,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,-1 0,1 1,1-1,-1 0,0 0,0 0,0-1,2-1,-1 1,1-1,-1 0,1 1,0 0,0-1,0 1,0 0,1 0,-1 0,0 0,1 1,0-1,-1 1,1-1,0 1,-1 0,1 0,4-1,2 0,0 0,0 0,1 0,-1 2,0-1,0 1,1 0,15 3,-3 2,1 1,25 11,-36-12,14 3,-3-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7003.66">2649 343,'0'5,"0"6,0 14,0 8,0 11,0 8,0 4,0 1,0-5,0-6,0-7,0-5,0-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7004.66">2463 582,'9'0,"12"0,11 0,5 0,5 0,-4 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7005.66">3178 423,'5'0,"-1"-2,1 1,0 0,0-1,-1 0,1 0,6-4,-5 2,0 1,0 0,0 1,1-1,8-1,-13 4,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 1,0-1,1 0,-1 1,0-1,0 1,0 0,0-1,0 1,1 0,-1-1,0 1,-1 0,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 1,1-1,-1 0,1 2,7 21,-1 1,-1 0,-2 0,0 1,-2-1,-1 51,-2-65,-1-1,-1 1,0-1,0 0,-1 0,0 0,0 0,-1-1,-1 0,0 0,0 0,0-1,-1 0,-1 0,1 0,-1-1,0 0,-1-1,0 0,0 0,0-1,0 0,-1-1,0 0,0 0,0-1,-1 0,1-1,-1 0,-18 0,12-2,0-1,1-1,-1 0,1-2,-31-9,43 12,0-1,0 0,0 0,0 0,0-1,1 1,-1-1,1 0,0 1,0-2,0 1,-3-4,4 4,1 1,0-1,0 1,0-1,1 0,-1 1,1-1,-1 0,1 1,0-1,0 0,0 1,0-1,0 0,1 1,-1-1,1 0,0 1,0-1,0 1,2-5,0 2,0 0,1 0,0 0,0 1,1-1,-1 1,1 0,0 1,0-1,0 1,0 0,1 0,-1 0,1 1,0 0,-1 0,1 0,0 1,10-2,7 0,0 0,-1 2,45 2,-50 1,0 0,0 1,-1 0,1 1,-1 1,0 1,0 0,-1 1,0 1,24 16,-23-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7369.68">3522 767,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8358.34">3892 264,'-5'0,"-5"5,-6 6,-1 5,4 9,3 5,8-3,18-5,11-8,9-5,4-4,-1-4,-3-1,-2-1,1 0,0-1,-2 1,-6 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8864.4">4236 0,'1'70,"-4"0,-2 0,-3 0,-19 71,17-104,1 1,1 0,2 1,2-1,2 1,2 39,0-76,0 0,0 0,0 0,1 1,-1-1,0 0,1 0,0-1,-1 1,1 0,0 0,0 0,0 0,0-1,1 1,-1 0,0-1,1 1,-1-1,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,3 0,22-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10119.47">4765 291,'-33'0,"1"1,0 1,0 1,-47 12,69-12,1 0,0 0,0 1,0 1,0-1,1 1,-1 0,1 1,1 0,-1 1,1-1,0 1,0 1,1-1,0 1,0 0,1 1,0-1,-4 11,8-17,0 1,0 0,-1-1,2 1,-1 0,0-1,0 1,1 0,0 0,-1 0,1-1,0 1,0 0,1 0,-1 0,1 0,-1-1,1 1,0 0,0-1,0 1,2 3,0-3,-1-1,1 0,0 1,0-1,0 0,0-1,0 1,0 0,0-1,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,6-1,72-4,-67 2,1 1,-1 0,1 1,-1 0,1 2,26 5,-37-5,0 0,0 0,-1 0,1 1,-1 0,0 0,0 0,0 1,0-1,0 1,-1 0,1 0,-1 0,0 0,-1 1,1-1,-1 1,0 0,0-1,2 11,0-3,-2 0,0 1,0 0,-1-1,-1 1,0 0,-2 18,1-28,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1-1,-1 1,0-1,0 1,0-1,0 0,0 1,-1-1,1 0,-1-1,1 1,-1 0,0-1,1 1,-1-1,0 0,0 0,0 0,0 0,0-1,0 1,-6-1,-12 2,0-1,0-1,-32-4,12 1,-3 2,-70-4,80-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11793.02">5400 238,'-19'0,"1"1,0 0,-25 6,34-5,0 1,1 0,-1 0,1 1,0 0,0 1,0 0,-12 10,4-2,1 1,0 0,0 1,2 1,0 0,-17 29,23-32,0 1,1 0,1 0,0 1,1-1,0 1,1 0,1 0,0 27,1-14,1 0,1-1,2 1,1 0,13 48,-15-69,1 0,0 1,0-2,0 1,1 0,1-1,-1 1,1-1,0-1,0 1,0-1,1 1,0-2,0 1,0-1,1 0,-1 0,1 0,0-1,0 0,1-1,-1 1,0-1,1-1,-1 0,9 1,0 0,-1-2,1 1,-1-2,1 0,-1-1,0-1,21-5,-32 7,1-1,-1 1,-1-1,1 1,0-1,0 0,-1 0,1-1,-1 1,1-1,-1 0,0 0,0 0,-1 0,1 0,0-1,-1 1,0-1,0 0,0 0,0 0,-1 0,0 0,1 0,-2 0,1 0,0 0,-1 0,1-1,-1 1,-1-4,0 0,1 1,-2 0,1 0,-1 0,0 1,-1-1,0 0,0 1,0 0,-1-1,1 1,-1 0,-1 1,-5-6,2 3,0 1,-1 0,0 0,0 1,-1 0,1 1,-1 0,-15-5,4 3,0 2,-1 0,1 1,-1 1,0 1,0 1,0 1,-38 4,38 2,6 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 404,'-1'35,"0"-17,1 1,3 25,-2-39,0 1,1-1,-1 1,1-1,1 0,0 0,-1 1,1-1,0 0,0-1,9 10,1-2,-1 1,0-1,1 0,0-1,0-1,2 1,-1-2,2 0,22 10,127 36,-163-54,0-1,0 1,2-1,-2 1,0-1,1 0,-1 1,1-1,-1-1,0 1,1 0,0 0,-1-1,1 0,-1 1,0-1,0 0,0 0,1 0,-1 1,0-1,1-1,-1 1,-1-1,1 1,0-1,-1 0,1 0,-1 1,1-1,-1 0,2-2,3-7,-1 0,-1-1,0 1,0-1,2-13,2-8,7-9,-7 22,-1 0,0-1,-2 0,-1 0,3-37,-7 53,-1 0,1 0,-1 1,0-2,0 1,0 0,-1 2,0-2,0 0,0 0,-1 2,1-2,-2 1,1 0,0 0,-1 0,1 1,-1 0,-1-1,1 1,0 0,0 0,-1 1,0 0,0 0,0-1,1 2,-1-1,-1 0,-6 0,-26-4,-1 2,2 2,-1 0,-1 3,-48 5,74-5,5-1,1 1,1 1,-1-1,0 1,1 0,-12 5,-4 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="419">861 757</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1597.05">999 404,'0'-1,"0"0,1 0,-1-1,2 1,-1 0,-1 0,1 0,0-1,0 1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,2 1,32-18,-21 13,-4-1,0 1,1 0,0 2,0-1,0 0,1 1,20-2,-30 4,1 1,1 0,-2 0,1 0,0 0,-1 0,1 0,-1 1,1 0,1-1,-2 1,1 0,-1 0,1 0,-1 0,0 1,0-1,1 1,0-1,-1 1,0 0,0-1,-1 1,1 0,0 0,-1 0,1 1,-1-1,0 0,0 1,0-1,0 0,0 0,1 1,-2-1,1 1,-1 2,4 18,-2-1,-1 0,-1 0,0 0,-2 0,-1 0,-2 1,1-2,-2 1,-16 35,20-53,0 0,-1-1,1 1,-2-1,1 0,0 0,0 0,0 0,-1 0,1-1,-2 1,1-2,1 1,-1 0,-6 2,7-3,0 0,0 0,0 0,1-1,-1 1,0-1,-1 0,1 0,0 0,0 0,0 0,0 0,0-1,-1 0,1 1,0-1,1 0,-1-1,0 1,1 0,-1-1,-4-1,7 3,-1 0,1-1,-1 1,1 0,-1-1,1 1,0 0,-1-1,1 1,0-1,-1 1,1 0,0-1,-1 1,1-1,0 1,0-1,0 1,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1 0,0-1,1 1,-1-1,0 1,1-1,-1 1,0 0,1-1,-1 1,1 0,0 0,27-9,-16 8,0 2,-1-1,1 1,-2 1,2 0,-1 1,0-1,0 1,-1 1,15 7,13 8,50 31,-46-24,-4-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7001.66">1498 505,'61'-11,"2"4,0 1,98 3,-122 3,-36 0,1 0,-1 0,0 0,1 0,-1 0,0 1,0 0,0-1,0 1,0 0,1 0,-1 1,0-1,-1 1,1-1,0 0,-1 1,1 0,0 0,-1 0,4 5,-4-3,0-1,-1 1,1 0,-1 0,0 1,0-2,0 2,-1-1,1 1,-1-1,0 0,-1 0,1 0,-2 7,1-5,0-1,0 1,-1-2,0 1,0 1,0-1,0 0,-1-1,-1 1,1-1,0 1,-1-2,0 1,0 1,-1-2,1 1,0 0,-1-2,-9 6,5-3,0-2,0 0,0-1,-1 1,0-1,0 0,1-1,-2 0,2-1,-18-1,32 2,-1 0,1-1,1 2,-1-1,0 0,-1 1,2 0,-2-1,0 2,1-1,-1 1,0 0,1 0,-2 0,1 0,-1 0,1 0,-1 1,1 0,-1 0,-1 0,1 0,-1 0,0 0,0 1,2 8,-3-10,2 0,-2 1,-1-2,1 2,0 0,-1-1,1 1,-1 0,0-2,-1 2,1 0,0-1,-1 1,0-1,0 0,0 0,-1 1,0-1,1 0,-4 5,1-5,1 1,0-1,-2-1,2 1,-1 0,0-1,0 0,0 0,-1 0,1-1,0 1,-1-1,1 0,-1 0,0 0,-5 0,-22 2,1-2,1-2,-2 0,1-2,0-1,0-1,-32-10,57 13,0 0,0 0,1 0,-1 0,1 0,-1-1,2-1,-10-6,-1-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7002.66">2135 327,'21'0,"1"0,1 0,0 1,0 1,41 9,-59-9,0-1,2 0,-2 2,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,-1 1,1 0,-2 1,1-1,-1-1,0 2,0 0,1 0,-1-1,-1 1,0 0,0 1,2 8,1 16,-1-1,-2 1,-1 0,-1 0,-2 0,-10 48,11-73,-1 1,1 0,-1 0,0-2,-1 2,-1 0,2-1,-1 0,-1 0,1 0,-1 0,-1-2,1 2,-1-1,1 1,-1-1,-1-2,1 2,0-1,-1 0,0 0,0 0,-10 2,0-2,0 1,-1-2,1 0,-1-1,0 0,0-1,1-1,-18-3,31 4,1 0,-1-1,0 1,-1-1,2 0,-1 0,0 0,1 0,-1 0,1 0,-6-3,8 4,-1-1,1 0,-1 1,0-1,1 0,0 1,-1-1,1 0,-1 0,1 0,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,-1 0,1 1,1-1,-1 0,0 1,0-1,0-1,2-1,-1 1,1-1,-1 0,1 1,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 1,0-1,0 1,0-1,0 1,-1 0,1 0,4-1,3 1,-1-1,1 0,0 0,0 2,-1-1,0 1,2 0,15 3,-3 2,1 0,26 11,-37-11,14 3,-3-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7003.66">2772 327,'0'5,"0"6,0 12,0 9,0 10,0 8,0 3,0 1,0-4,0-6,0-7,0-4,0-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7004.66">2578 555,'9'0,"13"0,12 0,4 0,6 0,-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7005.66">3326 404,'5'0,"-1"-2,2 1,-1 0,0-1,-1 0,1 0,7-4,-6 3,1 0,-1 0,0 1,1-1,9-1,-14 4,-1 0,0 0,0 0,1 0,-1 0,1 0,0 0,-1 0,0 1,0-1,1 0,-1 1,0-1,0 1,0 0,0-1,0 1,1 0,-1-1,0 1,-1 0,1 0,0 0,0 0,1 0,-1 0,-1 0,1 0,-1 0,1 0,-1 0,1 2,7 20,-1 1,0 0,-3 0,0 1,-2-2,-1 50,-2-63,-1 0,-1 0,0 0,0-1,-2 1,1 0,0-1,-1 0,-1-1,-1 1,1-1,0 0,-2 0,0-1,1 1,-2-1,1-1,-1 0,-1 0,1 0,-1-2,1 1,-2-1,1 0,-1 0,1-2,-2 1,2-1,-1 0,-20 0,13-2,1-1,0-1,-1 0,1-2,-32-8,45 11,0-1,0 0,-1 0,1 0,0 0,1 0,-1-1,1 0,-1 1,1-2,0 1,-3-3,4 3,1 1,0-1,0 1,0-1,1 0,-2 1,2 0,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,1 2,-1-2,2 0,-1 1,0-1,0 1,2-5,0 3,0-1,1 0,0 0,1 2,0-2,-1 1,1 0,1 1,-1-1,0 2,0-1,2 0,-2 0,1 1,0 0,0 0,0 0,0 1,11-1,7-1,0 0,-1 2,47 2,-52 1,0 0,0 1,-2-1,2 2,-1 1,0 1,-1-1,0 2,0 1,24 15,-23-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7369.68">3686 732,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8358.34">4073 252,'-5'0,"-6"5,-5 5,-2 5,4 9,4 5,8-3,19-5,11-8,9-4,5-5,-1-3,-3-1,-3-1,2 0,0 0,-3 0,-6 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8864.4">4433 0,'1'67,"-4"0,-2-1,-4 1,-19 68,18-100,0 1,2 1,2 0,2-1,1 1,3 38,0-73,0-1,0 1,0 0,1 1,-1-1,0 0,2 0,-1-1,-1 1,1 0,0 0,0-1,0 1,0-1,1 1,-1 0,0-1,1 1,-1-1,1 1,-1-1,1 0,0 0,-1 0,2 0,-1 0,0 0,0 0,0-1,0 0,0 1,0-1,0 1,0-1,1 0,-1 0,3 0,23-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10119.46">4987 278,'-35'0,"2"1,-1 1,1 0,-50 13,73-12,0-1,1 1,-1 1,1 1,0-1,0 0,0 1,0 1,2 0,-1 0,0 0,1 1,0 0,0 0,1 1,0-1,1 2,-1-1,-3 10,8-16,0 0,0 1,-1-1,2 1,-1 0,0-1,0 1,1 0,0-1,-1 1,1-1,0 1,0 0,1 0,-1 0,1 0,-1-2,1 2,0 0,0-1,0 1,2 3,0-3,-1-2,1 1,1 1,-1-1,0 0,0-1,0 1,0 0,0-1,1 0,0 0,-1 0,0 0,1 0,-1-1,1 1,7-1,75-4,-71 2,2 1,-1 0,1 1,-2 0,2 2,27 4,-39-4,1 0,-1 0,-1 0,1 1,-1 0,1 0,-1 0,0 0,0 0,0 1,-1 0,2 0,-2-1,0 1,-1 1,1-1,-1 1,0-1,0 0,3 11,-1-4,-2 0,0 2,0-1,-1 0,-1 0,0 1,-2 16,1-26,0 0,0 0,0 0,0-1,0 1,0 0,-1 0,1-1,-2 1,1-1,0 1,0-2,0 1,0 1,-1-1,1 0,-1-1,1 1,-2 0,1-1,1 1,-1-1,0 0,0 0,0 0,-1-1,1 0,0 1,-6-1,-13 2,0-1,0-1,-34-4,13 2,-3 1,-73-4,84-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11793.02">5651 227,'-19'0,"0"1,0 0,-26 6,35-5,1 0,1 1,-2 0,2 1,-1 0,1 1,0-1,-13 11,4-3,1 1,1 1,-1 0,2 1,1 1,-19 27,25-31,0 1,0 1,2-1,0 1,1 0,0 0,0 0,2 1,0 25,1-14,1 1,1-1,2 1,2-1,12 47,-15-66,2-1,-1 2,0-2,0 0,1 1,1-1,0 0,0 0,0-1,0 1,1-2,0 2,0-2,0 1,1-1,0-1,-1 1,2 0,-1-1,0 0,2-1,-2 0,0 0,2-1,-2 0,10 1,-1 0,0-2,1 1,-1-2,0 0,0-1,0-1,21-4,-32 6,0-1,-1 1,-1-1,1 1,1-1,-1 0,-1 0,1-1,-1 2,1-2,0 0,-1 0,0 0,-1 0,1 0,0 0,-1 0,0-1,0 0,1 0,-1 0,-1 1,0-1,1 0,-2 0,1 0,0 1,-1-1,1-1,-1 1,-1-4,0 1,1 0,-2 1,1-1,-1 0,0 1,-2 0,1-1,0 1,0 1,-1-2,1 1,-2 0,0 2,-5-7,1 4,1 0,-1 0,-1 1,1 0,-2 0,2 1,-2 1,-15-6,4 3,0 3,-1-1,1 1,-1 1,0 1,0 1,0 1,-40 4,40 2,7 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6733,13 +6833,13 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">669 284,'-24'-1,"1"-1,-30-7,36 5,0 1,0 1,0 0,0 1,0 1,-19 2,13 3,0 0,0 1,1 1,-1 2,2 0,-1 1,2 1,-1 1,1 1,1 0,1 2,-19 18,23-20,1 1,1 1,0 0,1 1,1 0,1 0,0 1,1 0,0 1,2 0,0 0,1 1,1-1,0 1,0 25,2-15,0 9,5 74,-2-104,0 0,0 0,1 0,0 0,0 0,1 0,0-1,0 1,1-1,-1 0,2 0,-1 0,1 0,0-1,7 7,-6-9,1 0,-1-1,1 1,0-1,0 0,0-1,0 0,0 0,1-1,-1 1,1-2,-1 1,1-1,-1 0,12-2,13-2,0-1,36-12,-59 15,8-3,1 0,-1-2,0 0,-1 0,1-2,-2 0,1-1,-1 0,-1-1,0-1,0 0,15-20,4-1,27-34,-55 61,-1 0,0-1,0 0,-1 0,0 0,0 0,0-1,-1 1,2-12,40-279,-43 295,2-15,-1-1,0 1,-2-1,0 1,-3-19,3 33,-1 0,0 0,0 0,0 0,-1 0,1 1,-1-1,0 0,0 1,0-1,0 1,-1 0,0 0,1 0,-1 0,0 0,0 1,-1-1,1 1,0 0,-1 0,1 0,-1 0,0 1,0-1,0 1,1 0,-8-1,-9-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="594.52">1092 813,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3009.04">1753 46,'-32'-1,"1"-2,0-2,0 0,0-2,-32-13,59 19,0 0,0 0,0 1,0-1,0 1,0-1,0 1,0 1,0-1,0 0,0 1,0 0,0 0,0 0,0 0,0 1,1 0,-1 0,1 0,-1 0,1 0,0 0,0 1,0 0,0 0,0 0,0 0,-2 4,-7 9,2 1,0 1,0 0,-8 24,8-17,1-6,-4 7,1 1,1 1,1 0,2 0,-9 56,16-81,1 0,0-1,0 1,1 0,-1-1,1 1,-1 0,1-1,0 1,0 0,0-1,0 0,1 1,-1-1,0 0,1 1,0-1,0 0,-1 0,1 0,0 0,1-1,-1 1,0-1,0 1,1-1,3 2,7 2,0-1,0 0,1 0,19 1,16 5,202 93,-76-27,-162-70,0-1,-1 2,1 0,-1 0,-1 1,0 0,17 16,-25-20,1-1,-1 0,0 1,-1-1,1 1,-1 0,1 0,-1 0,0 0,0 0,-1 0,1 1,-1-1,0 1,0-1,-1 1,1-1,-1 1,0-1,0 1,-1-1,1 1,-1-1,0 1,0-1,-1 1,-1 4,0-4,0-1,0 0,0 0,-1-1,1 1,-1 0,0-1,0 0,0 0,0 0,0-1,-1 1,1-1,-1 0,0 0,1-1,-1 0,0 1,-10 0,-11 1,1-1,-42-1,49-1,-10-1,0-1,0-1,0-1,1-2,-1 0,1-2,-38-17,35 12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5098.75">2177 99,'106'-1,"129"4,-220-2,-1 1,1 0,-1 1,0 1,0 0,0 1,0 1,-1 0,0 0,19 14,-26-16,0 1,-1 0,1 0,-1 0,0 1,0 0,-1 0,1 0,-1 1,-1 0,1-1,-1 1,0 0,-1 0,0 1,0-1,0 1,-1-1,0 1,-1-1,0 14,0-14,0-1,-1 1,0-1,0 0,0 1,-1-1,0 0,0 0,0 0,-1 0,0-1,0 1,0-1,-1 0,0 1,0-2,0 1,-1 0,0-1,1 0,-1 0,-1 0,-9 5,5-4,6-3,0 0,0 0,0 1,1-1,-1 1,0 0,-5 6,8-8,1-1,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0-1,1 1,-1-1,0 1,1 0,20 16,-6-10,-1 1,0 1,-1 0,0 1,23 22,-31-26,1 1,-1 0,0 1,-1-1,0 1,0 0,-1 0,0 0,0 0,-1 1,0-1,2 18,-1 13,-1 0,-2 0,-8 62,7-94,-1 1,0-2,-1 1,0 0,0 0,0-1,-1 0,0 0,0 0,-1 0,0 0,0-1,0 0,0 0,-1-1,0 1,0-1,0 0,0-1,-1 1,1-1,-1-1,-7 3,-10 3,0-2,-1 0,1-1,-1-2,-36 1,-25-1,-151-14,198 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6041.43">3050 257,'62'-15,"38"6,147 6,-163 4,-80-2,0 1,0 0,0 1,0-1,0 0,0 1,0 0,0 0,0 0,0 1,-1-1,1 1,0 0,-1 0,5 3,-6-2,0 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 1,0-1,-1 0,1 1,-1-1,0 1,0-1,0 0,0 1,-2 6,-2 17,-2 1,-1-1,-1 0,-1 0,-1-1,-28 50,-100 138,-49 30,142-192</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6691.43">3129 760,'4'-9,"11"-3,8 1,8 2,21 2,7 3,-2 2,-2 1,-6 1,-7 0,-5 1,-6 0,-2-1,-3 0,-1 0,-4 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8372.61">4055 125,'-4'24,"0"0,-1 0,-1-1,-2 0,0 0,-22 42,10-23,-34 82,48-108,1 1,1 0,1 1,1-1,-1 33,7 158,-3-205,-1 1,0 0,1 0,0-1,0 1,0-1,0 1,0 0,1-1,0 0,-1 1,1-1,1 0,-1 0,0 0,1 0,-1-1,1 1,0-1,0 1,0-1,0 0,0 0,1 0,-1-1,1 1,-1-1,1 0,-1 0,8 1,8 1,2-1,-1-2,0 0,36-5,-3 2,-52 3,64-8,-63 8,0-1,1 0,-1 1,0-1,0 0,0 0,0 0,0-1,0 1,-1 0,4-3,-5 3,1 0,-1 0,1 0,-1 1,1-1,-1 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,0-1,-1-1,-1 0,1 1,0-1,-1 1,1 0,-1-1,0 1,0 0,1 1,-2-1,1 0,-6-1,-46-14,36 12,-47-17,-38-11,95 31,0 0,0 1,0 0,-1 0,1 1,0 0,0 1,0 0,-11 3,17-3,0 0,1 0,-1 0,0 1,0-1,1 1,-1 0,1-1,0 1,-1 0,1 1,0-1,0 0,0 1,1-1,-1 1,0-1,1 1,0 0,0 0,0-1,-1 5,-5 19</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">696 273,'-25'-1,"1"-1,-31-7,37 6,0 0,1 1,-1 0,0 1,1 1,-21 2,14 3,0-1,0 2,2 1,-2 2,2-1,-1 2,2 0,-1 2,2 1,0-1,1 2,-19 18,23-19,1 0,2 2,0-1,0 1,2 1,0-1,1 1,1 1,-1 0,3 0,0 1,1 0,0-1,1 2,0 23,2-14,0 8,5 72,-2-100,0-1,0 1,1 0,0-1,0 1,2 0,-1-2,0 2,1-1,-1 0,2-1,-1 1,2 0,-1-1,7 6,-5-8,0 0,-1-1,1 1,1-2,-1 1,0-1,1 0,-1 0,1-1,-1 1,2-2,-2 1,1-1,0 0,11-2,15-2,-1-1,38-11,-62 14,9-3,0 0,0-1,0-1,-2 0,2-1,-2-1,0-1,0 1,-2-2,1 0,0-1,15-19,4 0,28-34,-56 59,-2 1,0-2,0 0,-1 0,0 1,0-1,1-1,-2 2,2-13,42-267,-45 283,2-14,-1-2,0 2,-2-1,0 0,-3-17,3 31,-1 0,0 0,0 1,0-1,-1 0,0 1,0-1,0 0,0 1,0 0,0 0,-1 0,0 0,1 0,-1 0,0 0,-1 1,0-1,1 2,0-1,-1 0,1 0,-1 0,-1 1,1-1,0 1,1 0,-8-1,-10-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="594.52">1136 782,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3009.04">1823 44,'-33'-1,"0"-2,1-1,0-1,0-2,-34-12,62 18,0 0,0 0,0 1,-1-1,1 1,0-1,0 1,0 1,0-1,-1 0,1 1,0 0,0 0,0 0,0 0,0 1,0 0,0 0,1-1,-1 1,1 0,0 0,0 1,-1 0,1 0,0 0,0 0,-2 3,-8 10,3 0,0 1,-1 1,-7 22,7-16,2-6,-5 7,2 1,0 1,2 0,2 0,-10 54,17-78,1 0,0-1,0 0,1 1,-1-1,1 1,-1 0,1-1,0 1,0 0,0-1,0 0,1 0,-1 0,0 0,1 1,0-1,1 0,-2 0,1 0,0 0,1-1,-1 1,0-1,0 1,1-2,3 3,8 2,0-1,-1 0,2 0,19 1,17 4,210 90,-79-26,-169-67,1-1,-2 2,2-1,-2 1,0 1,-1-1,18 16,-26-19,2-1,-2 0,0 1,-1-1,1 1,-1-1,1 1,-1 0,0 0,1 0,-2 0,1 1,-1-2,0 2,0-1,-1 1,1-1,-1 0,0 0,0 1,-1-1,1 1,-1-1,0 0,0 0,-1 1,-2 4,1-4,0-2,0 1,0 0,-1-1,1 1,-1 0,-1-1,1-1,0 1,0 0,0-1,-1 1,0-1,0 0,0 0,1-1,-1 0,-1 1,-9 0,-12 0,1 0,-44-1,51-1,-10-1,0-1,0 0,0-2,1-2,-1 0,1-2,-40-16,37 12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5098.75">2264 95,'110'-1,"134"4,-228-2,-1 1,0 0,0 1,-1 1,1-1,-1 2,1 1,-1 0,-1 0,20 13,-26-15,-1 0,-1 1,1 0,-1 0,1 1,-1-1,-1 1,1 0,-1 1,0-1,0 0,-1 1,0 0,-1-1,0 2,0-1,0 0,-1 0,0 1,-1-1,0 13,0-13,0-2,-1 2,0-1,0 0,0 0,-1 0,0 0,0 0,0-1,-1 1,0-1,-1 1,1-1,-1-1,0 2,0-2,0 1,-1 0,-1-2,2 1,-1 0,-1 0,-10 5,6-5,6-2,-1 0,1 0,0 1,1-1,-1 1,0 0,-6 5,9-7,1-1,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0-1,1 1,-1-1,0 1,1 0,21 15,-6-9,-2 1,1 0,-2 1,1 1,23 20,-31-24,0 1,-1 0,0 0,-1 0,0 1,1-1,-2 1,0 0,0-1,-1 2,0-1,2 17,-1 12,-1 1,-2-1,-8 60,7-90,-1 1,0-3,-1 2,0 0,0 0,-1-2,0 1,0 0,0 0,-1 0,0-1,-1 0,1 0,0 0,-1-1,0 0,-1 0,1 0,0-1,-1 1,0-1,0-1,-8 2,-9 4,-1-2,-1 0,1-2,-1-1,-38 1,-25-1,-158-14,207 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6041.42">3172 247,'64'-14,"40"5,153 6,-170 4,-82-2,-1 1,0 0,0 1,0-1,0 0,1 1,-1 0,0 0,0 0,0 1,-1-1,1 1,1 0,-2 0,5 2,-6-1,0 0,0 0,-1 0,1 0,-1 0,2 0,-2-1,0 1,0 1,0-1,-1 0,1 1,-1-1,0 1,0-2,0 1,0 1,-2 6,-3 16,-1 1,-1-1,-1 0,-2-1,0 0,-30 49,-103 131,-52 30,149-185</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6691.42">3254 731,'4'-9,"12"-3,8 2,8 1,22 2,7 4,-2 1,-1 1,-7 1,-8 0,-4 1,-7 0,-2-1,-3 0,-1 0,-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8372.61">4217 120,'-4'23,"0"0,-2 0,0-1,-2 1,-1-1,-22 40,10-21,-35 78,50-104,1 2,1-1,1 1,0 0,0 31,8 152,-4-198,-1 2,0 0,1 0,0-1,0 1,0-1,0 0,0 1,1-1,0 0,-1 1,1-1,1 0,-1 0,0-1,1 1,0-1,0 1,0-1,0 1,0-1,0 0,0 0,1 0,0-1,0 0,-1 0,1 0,-1 0,9 1,7 1,3-1,-1-2,0 0,37-5,-3 2,-54 3,67-7,-66 7,0-1,1 0,-1 1,0-1,0 0,0 0,0 0,0-1,1 1,-2 0,4-3,-5 3,1 0,-1 0,1 0,-1 1,1-1,-1 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,0-1,-1-1,-1 1,1 0,-1-1,0 1,1 0,-1-1,0 1,0 0,1 1,-2-1,1 0,-7-1,-47-13,37 11,-48-16,-41-11,100 31,0-1,-1 1,1 0,-1 0,0 1,1 0,0 1,-1 0,-11 2,18-2,0 0,1 0,-1 0,0 1,0-1,1 1,-2 0,2-1,0 1,-1 0,1 1,0-1,0 0,0 0,1 0,-1 1,0-1,1 1,0 0,0 0,0-1,-2 5,-4 18</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6766,7 +6866,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 302,'0'-1,"0"0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 1,0-1,0 0,0 1,0-1,1 0,29-12,-24 10,54-17,1 2,97-15,136-3,654-14,9 52,-405 3,-155-4,903-2,-395-53,4 0,-782 57,-62-1,116-9,-150 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 302,'0'-1,"0"0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 1,1-1,-1 0,0 1,0-1,1 0,30-12,-24 10,56-17,1 2,101-15,143-3,686-14,10 52,-426 3,-161-4,945-2,-413-53,4 0,-820 57,-64-1,120-9,-156 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7107,7 +7207,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">430 370,'-1'-1,"1"1,-1-1,1 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 0,0 1,1-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 1,0 0,0 0,0-1,0 1,-2 0,-27-4,23 4,-1 0,1 0,0 1,-1 0,1 0,0 1,0 0,0 0,0 0,0 1,0 0,1 1,-1 0,-8 6,7-3,-1 1,1-1,1 2,0-1,0 1,1 0,0 0,0 1,-5 12,6-10,-1 0,2 1,0 0,1 0,0 0,1 0,0 0,1 1,1-1,0 0,0 1,2-1,0 0,0 1,1-1,8 21,-6-24,1 0,1 0,-1-1,2 1,-1-1,1-1,1 0,-1 0,1 0,1-1,17 10,-22-14,0 0,0 0,0-1,0 0,1 0,-1 0,0-1,1 1,-1-1,1-1,0 1,-1-1,1 0,0 0,-1 0,1-1,-1 0,1 0,-1-1,1 1,-1-1,0-1,0 1,0 0,9-7,-3 0,-1-2,0 1,-1-1,0 0,0-1,-1 0,8-19,4-9,15-48,-31 75,0 0,0-1,-1 1,-1-1,-1 1,1-1,-3-25,1 32,-1 1,0-1,0 1,-1-1,0 1,0 0,-1 0,1 0,-1 0,0 0,-1 1,1-1,-1 1,-1 0,1 0,-1 1,1-1,-8-4,-3-2,-1 2,0 0,-1 1,-20-8,28 13,0 0,1 1,-2 0,1 0,0 1,0 0,0 1,-1 0,1 0,-12 2,19-1,0-1,-1 1,1 0,0 0,-1 0,1 0,0 0,0 0,0 1,0-1,0 1,0-1,1 1,-1 0,0 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 1,0-1,1 0,-1 1,1-1,-1 0,1 1,0-1,0 1,0-1,0 1,0-1,1 0,0 5,4 15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="441.99">933 820,'0'5,"-5"1,-6 4,0 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="441.98">933 820,'0'5,"-5"1,-6 4,0 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1753.99">1012 370,'0'-4,"1"0,0 0,0 0,0 0,0 0,1 0,0 0,-1 0,2 0,-1 1,0-1,1 1,-1 0,1-1,0 1,0 1,0-1,1 0,-1 1,1-1,-1 1,1 0,7-3,-3 1,1 1,-1 0,0 0,1 1,0 0,-1 0,1 1,0 1,0-1,13 2,-17 0,0 0,1 1,-1 0,0 0,0 0,0 1,0 0,-1 0,1 0,-1 0,1 1,-1 0,0 0,-1 0,1 0,-1 0,0 1,0 0,0 0,0-1,3 12,3 8,-1 1,0 0,4 34,-11-53,7 37,-2 0,-1 0,-3 0,-1 0,-3 1,-8 56,9-94,0-1,0 0,0 0,-1 0,0-1,0 1,0 0,0-1,-1 1,0-1,0 0,0 1,0-2,-1 1,-5 4,4-5,1 0,-1-1,-1 0,1 0,0 0,0 0,-1-1,1 0,-1 0,1-1,-1 0,1 1,-1-2,-5 0,2 0,-1 0,1-1,0 0,0-1,1 0,-1 0,0-1,1 0,-10-7,15 10,1 0,0-1,0 1,-1-1,1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1-1,0 1,0-1,0 1,0-1,0 1,0-1,1 1,-1-1,1 0,0 0,-1 1,1-1,1 0,-1 1,0-1,1 0,-1 1,1-1,0 1,0-1,0 0,0 1,2-3,-1 2,1 0,-1 0,1 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,1 1,-1-1,1 1,-1 0,1 0,0 0,-1 1,8-1,75 0,-66 2,8 1,-1 2,0 1,0 1,0 1,36 16,-45-17</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7138.99">351 0,'-3'1,"0"-1,0 1,0 0,0 0,0 0,0 0,0 1,1-1,-1 1,1 0,-1-1,1 1,0 0,-4 4,-32 38,27-29,2-4,-39 46,-69 107,105-144,1 0,1 0,1 1,1 0,0 1,2 0,1 0,0 0,2 1,-1 24,3-18,0-6,0 0,4 23,-3-42,0-1,0 1,1 0,0 0,0-1,0 1,0-1,1 1,-1-1,1 1,0-1,0 0,0 0,0 0,1 0,-1 0,1 0,0-1,3 3,10 2</inkml:trace>
 </inkml:ink>
@@ -7166,22 +7266,22 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2788 1244,'0'5,"-5"10,-6 11,0 16,-9 8,-4 11,-3-2,3-5,5-9,2-6,4-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1560">3634 371,'-6'15,"1"-1,0 1,1-1,-3 24,-7 31,-12 1,-55 109,55-129,2 0,2 2,3 0,-21 90,39-135,0 0,0 1,1-1,0 0,0 1,1-1,0 1,0-1,1 0,0 0,0 0,0 0,1 0,4 7,-5-11,1 0,-1 0,0 0,1 0,-1-1,1 1,0-1,0 0,0 0,0 0,1 0,-1-1,0 1,1-1,-1 0,1 0,-1 0,1 0,-1 0,1-1,0 0,0 0,-1 0,1 0,0-1,-1 1,1-1,-1 0,1 0,3-1,2-2,0 0,0-1,0 0,0 0,-1-1,0 0,0 0,0-1,-1 0,0 0,-1-1,8-11,10-15,30-59,-49 82,8-18,-1 0,-2-1,-1 0,-2-1,5-37,3-9,-8 44,-1 0,-1 0,-3 0,0-1,-2 1,-2-1,-6-40,7 69,0 1,0 0,0 0,-1 0,0 0,1 0,-1 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,0-1,0 1,-1 1,1-1,-1 1,0-1,1 1,-1 0,0 0,-8-2,-10-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2114">4005 1059,'4'0,"6"0,2 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3557">4693 397,'-9'1,"1"0,0 0,0 1,0 0,0 0,0 0,1 1,-1 1,1-1,0 1,0 1,0-1,0 1,1 0,0 0,0 1,0 0,1 0,0 1,0-1,0 1,-6 13,3-4,0 1,1 0,0 0,1 0,2 1,-1 0,2 0,1 0,-1 23,3-18,1 1,1-1,1 0,1 0,1 0,1 0,11 28,-14-44,0 0,1-1,0 1,0-1,1 0,-1 0,1 0,1 0,-1-1,1 0,9 7,-10-9,0-1,1 0,-1 1,0-2,1 1,-1 0,1-1,0 0,0-1,-1 1,1-1,0 0,0-1,-1 1,1-1,0 0,6-2,-7 1,0 0,0 0,0-1,0 1,0-1,0 0,-1 0,0-1,1 1,-1-1,0 0,-1 0,1-1,-1 1,0-1,4-6,-5 7,0 1,-1-1,1 1,-1-1,0 0,0 1,0-1,0 0,-1 0,0 0,1 0,-1 1,-1-1,1 0,-1 0,1 0,-1 0,0 1,0-1,-1 0,1 1,-1-1,0 1,-2-5,0 5,1 0,0-1,-1 2,0-1,1 0,-1 1,0 0,-1-1,1 2,0-1,0 0,-6 0,-55-11,65 13,-30-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4438">4878 159,'2'1,"1"1,-1-1,1 0,-1 1,1-1,-1 1,0 0,1 0,-1-1,0 2,0-1,-1 0,1 0,0 1,-1-1,1 1,-1-1,0 1,2 4,3 5,25 43,-4 1,-1 2,-3 0,-3 2,-2 0,-3 1,-3 1,-2 0,-3 0,-3 1,-6 102,0-147,0 0,-2 0,0-1,-1 1,0-1,-2 0,0 0,-1-1,0 0,-2-1,-13 20,5-16</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5608">274 0,'-1'1,"0"-1,0 1,0-1,0 1,0-1,0 1,0 0,1-1,-1 1,0 0,0 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 2,-4 36,3-32,-10 117,-12 222,19-265,-24 135,14-125,7-12,3 0,7 83,0-29,-3-118,-1 4,2 0,0 0,4 20,-4-35,-1 0,1 0,0 0,1 0,-1-1,1 1,0 0,0-1,0 1,0-1,0 1,1-1,0 0,-1 0,1 0,1-1,-1 1,0-1,0 1,5 1,18 6,1-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7436">988 2593,'-2'3,"0"0,0 0,0 0,-1 0,1-1,0 1,-1-1,0 0,0 0,-3 2,-3 3,1 0,0 0,0 1,0-1,1 1,0 1,1 0,0 0,0 0,1 0,0 1,1 0,0 0,0 0,1 0,0 1,1 0,1-1,-2 22,8 192,-4-219,-1 1,1 0,1-1,-1 1,1-1,0 1,0-1,0 0,1 0,0 0,0 0,0 0,1 0,-1-1,8 7,-3-5,0 0,0 0,0-1,1 0,0 0,0-1,0-1,15 5,2-2,0-1,1-2,0 0,-1-2,52-3,-62-1,0 0,0-1,0-1,0 0,-1-1,0-1,0 0,0-1,-1-1,0 0,-1-1,0 0,-1-1,0-1,0 0,-1 0,-1-1,0 0,-1-1,14-27,-14 21,-1 1,1 0,-2-1,-1 1,5-26,-10 39,0 1,-1-1,0 0,0 0,0 0,-1 0,0 1,0-1,0 0,-1 0,0 1,0-1,0 1,-1 0,1 0,-1 0,-1 0,1 0,-7-7,-11-9,-1 2,-1 0,0 2,-2 0,-51-26,57 34,-1 0,0 1,0 1,-1 1,0 1,0 1,0 1,-40-2,58 6,-1-1,1 0,0 1,0-1,0 1,0 0,0 0,1 0,-1 1,0-1,0 1,1-1,-1 1,1 0,-1 0,1 0,0 0,0 0,-4 5,-5 11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8791">2205 2276,'-5'2,"0"0,0 0,0 0,1 0,-1 1,1-1,0 1,-1 1,2-1,-1 0,0 1,-4 5,-5 4,-45 43,3 2,2 3,3 3,-72 116,115-166,0 1,1-1,1 1,0 0,0 0,2 0,0 0,1 1,0 0,1-1,1 1,3 24,-2-23,2 0,0 1,1-1,1-1,0 1,2-1,-1 0,2 0,0 0,20 26,-24-37,0 0,1 0,0 0,-1-1,1 0,1 0,-1 0,0-1,1 0,0 0,0 0,0-1,0 0,0 0,0 0,1-1,-1 0,0 0,1-1,-1 1,1-1,-1-1,1 1,-1-1,0-1,1 1,-1-1,0 0,8-4,-12 6,-1-1,1 0,0 0,-1-1,1 1,-1 0,0 0,1-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 0,-1 1,1-1,0 0,-1 0,1 0,-1 1,0-5,0 2,0 0,-1-1,1 1,-1 0,0 0,0-1,-1 1,1 0,-5-7,2 3,-1 1,0-1,-1 1,1 0,-1 0,-1 0,1 1,-1 0,-10-7,-12 1,3 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9292">1703 3255,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10130">3052 3017,'0'5,"0"5,-5 6,-5 9,-6 5,-1 7,-5 18,-5 6,-1 0,-10 0,2-6,2-4,3-11,2-11,1-7,6-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11468.02">4110 2382,'-13'0,"0"1,1 0,-1 0,1 1,-1 1,1 0,0 1,0 0,0 1,1 0,-1 1,-18 12,18-10,-1-1,1 2,1 0,-1 0,2 1,-1 1,1-1,1 2,0-1,0 1,1 1,1-1,0 1,1 1,0-1,-4 17,-6 21,-37 140,47-162,1 1,1-1,2 1,2 48,0-74,0 0,1 0,0 0,0 1,0-1,0 0,1 0,0-1,-1 1,1 0,1 0,-1-1,0 1,1-1,0 0,0 0,0 0,0 0,0 0,1-1,-1 0,1 1,-1-1,1 0,0-1,0 1,0-1,0 1,0-1,0-1,1 1,7 0,1 0,-1-1,1 0,0-1,-1-1,1 0,-1 0,1-2,-1 1,21-10,-20 6,-1 0,1-1,-1 0,0-1,-1-1,0 0,-1 0,0-1,0 0,-1-1,-1 0,0-1,0 1,-1-1,-1-1,-1 1,1-1,-2 0,0-1,2-19,5-34,3-132,-14 188,1-4,-2 0,0 0,-5-21,5 32,0 1,-1-1,1 0,-1 1,-1-1,1 1,0 0,-1-1,0 1,0 0,0 1,-1-1,1 1,-1-1,-4-2,-12-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12647">4825 2302,'-21'37,"-35"47,-6 10,59-89,-10 17,0 1,2 0,0 1,-11 41,21-60,0 0,0 0,0 0,1 1,0-1,0 0,0 0,1 1,-1-1,1 0,1 0,2 9,-2-11,0 1,0-1,1 0,-1 0,1 0,0 0,0 0,0 0,0-1,0 1,0-1,1 0,-1 0,1 0,0-1,-1 1,1-1,8 2,-4-1,1 0,-1 0,1-1,0 0,-1-1,1 0,0 0,-1-1,1 0,0 0,-1-1,1 0,-1-1,0 0,1 0,-2-1,1 0,0 0,11-9,-11 6,0 0,0-1,-1-1,0 1,0-1,-1 0,0-1,-1 1,0-1,0-1,-1 1,0 0,-1-1,3-20,-1 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14191">4851 2752,'-17'0,"-2"0,1 0,-1 1,0 1,-27 6,40-6,1-1,0 1,0 0,0 1,0-1,1 1,-1 0,1 0,-1 1,1 0,0-1,0 1,1 0,-1 1,1-1,0 1,0-1,0 1,1 0,-2 5,-1 2,1 0,1 0,0 0,0 0,2 0,-1 1,2-1,-1 1,2-1,0 1,0-1,1 0,1 1,4 14,-4-19,0 0,1 0,0 0,0-1,1 1,0-1,0 0,1 0,-1-1,2 0,-1 0,1 0,-1-1,1 0,1 0,-1-1,1 1,0-2,0 1,16 3,-11-3,0-1,0-1,1-1,-1 0,1 0,0-2,-1 1,16-4,-23 3,-1 0,1-1,-1 1,1-1,-1 0,0 0,0-1,0 0,0 0,-1 0,1 0,-1-1,1 1,-1-1,0 0,-1-1,1 1,-1-1,0 1,0-1,0 0,2-6,0-3,-1 0,0 0,-1 0,0-1,-1 1,-1-1,0 0,-1 0,0 1,-5-27,3 33,-1-1,1 0,-1 0,-1 1,0 0,0 0,0 0,-1 0,0 0,-1 1,0 0,0 0,0 1,-1 0,0 0,0 0,0 1,-14-8,-34-9,31 13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15181.03">4798 2223,'4'0,"2"5,0 10,3 16,0 7,-1 2,-2-1,2-3,0-4,-1-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16212">5010 1905,'7'1,"0"0,0 1,0 0,0 0,0 0,0 1,-1 0,1 0,-1 1,0-1,0 2,0-1,0 1,7 7,10 11,36 47,-55-64,140 194,-123-166,-1 1,-3 0,0 1,14 49,-14-19,19 135,-26-59,-11 226,-4-337,-1-1,-1 0,-1 0,-2-1,-1 0,-1-1,-2 0,-19 29,31-54,0 0,0 0,-1 0,1 0,-1-1,0 1,1-1,-1 0,0 1,0-2,-1 1,1 0,0 0,-1-1,1 0,-1 0,-5 1,-38 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17138">591 2143,'-8'2,"1"0,1 0,-1 0,0 1,1 0,-1 0,1 1,0 0,0 0,0 0,0 1,1 0,-8 9,2-4,-58 56,3 3,3 2,-70 104,110-140,1 1,1 1,-24 63,36-75,1 1,1 0,1 0,2 1,1-1,-1 49,4-55,0 0,2 0,0 1,1-1,1-1,1 1,1 0,15 34,-2-18,1 0,2-2,1 0,1-2,2-1,39 37,-49-53</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2878 1201,'0'5,"-5"9,-7 12,1 14,-10 8,-3 11,-4-2,3-5,5-8,3-6,3-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1560">3751 358,'-6'15,"1"-2,0 2,1-2,-4 24,-6 30,-13 0,-56 106,56-125,2 1,2 1,4 0,-23 87,41-130,0 0,0 0,1 0,0 0,0 1,1-2,0 2,0-1,1 0,0-1,0 1,1 0,0 0,4 6,-5-10,1 0,-1 0,0 0,1 0,-1-1,1 0,0 0,1 0,-1 0,0 0,1 0,-1-1,0 1,1-1,-1 0,1 0,0 0,0 0,-1 0,1-1,0 0,0 0,-1 0,1 0,1-1,-2 1,1-1,-1 0,1 0,3-1,3-2,-1 0,0-1,0 1,1-1,-2-1,0 0,0 0,1 0,-2-1,0 0,-1-1,9-10,10-15,30-57,-50 80,9-18,-2 0,-1-1,-2 0,-2-1,6-36,2-8,-8 42,-1 0,0 0,-4 0,0 0,-2 0,-2-1,-7-39,8 68,0 0,0 0,0 0,-1 0,0 0,1 0,-1 1,-1-1,1 0,-1 1,1-1,-1 1,0 0,-1-1,1 2,-1 0,1-1,-1 1,0-1,1 1,-1 0,-1 0,-7-2,-11-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2114">4134 1023,'4'0,"7"0,1 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3557">4844 383,'-9'1,"1"0,0 0,-1 1,1 0,0 0,0 0,0 1,0 1,1-1,0 0,-1 2,1-1,0 1,1 0,0 0,-1 0,1 1,1 0,0 1,0-1,0 0,-7 14,4-5,0 2,0-1,1 0,1 1,2 0,-1 1,2-1,1 0,-1 23,3-18,1 1,1-1,1 1,1-1,1 0,1 0,12 28,-15-44,0 1,1-1,0 1,0-2,1 1,0 0,0 0,1 0,-1-2,1 1,10 7,-11-9,0-1,1 0,-1 0,1-1,0 1,-1 0,1-1,0 0,1-1,-2 1,1-1,0 0,0-1,-1 1,2-1,-1 0,6-2,-7 1,1 1,-1-1,0-1,0 1,0-1,0 0,0 0,-1-1,1 1,-1-1,0 1,-1-1,1-1,-1 1,0-1,5-5,-6 6,0 1,-1-1,1 1,-1-1,0 0,0 1,0 0,0-1,-1 0,0 0,1 0,-1 1,-1-1,1 1,-1-1,1 0,-1 0,0 1,0-1,-1 0,1 1,-1 0,0 0,-2-5,-1 5,2 0,0-1,-1 2,0-1,1 1,-1 0,0 0,-1-1,0 2,1-1,0 0,-6 0,-57-11,67 13,-31-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4438">5035 154,'3'0,"0"2,-1-1,1 0,-1 1,1-1,-1 1,0 0,1 0,-1-1,0 2,0-1,-1 0,1 0,1 1,-2-1,1 0,-1 0,0 1,2 4,3 5,26 41,-4 1,-1 2,-4 0,-2 2,-2 0,-4 1,-2 0,-3 1,-3 0,-3 1,-6 98,0-141,0-1,-2 0,0 0,-1 0,-1 0,-1-1,0 0,-1 0,-1-1,-1 0,-14 19,6-16</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5608">283 0,'-1'1,"0"-1,0 1,0-1,0 1,0-1,0 1,0 0,1-1,-1 1,-1 0,1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1-1,1 1,0 0,0 0,-1 0,1 0,0 0,0 2,-4 35,3-31,-10 112,-13 215,20-255,-25 129,15-120,6-12,4 1,7 79,0-28,-3-113,-1 3,2 1,0-1,5 20,-5-35,-1 1,1 0,0 0,1 0,-1-1,1 1,0 0,0-2,0 2,0-1,0 1,1-1,0 0,-1 0,2 0,0-1,-1 0,0 0,0 1,5 1,19 6,1-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7436">1020 2504,'-2'3,"0"0,0-1,0 1,-1 0,0-1,1 1,-1-1,0 0,0 0,-3 2,-3 2,0 1,1 0,0 1,0-2,0 2,1 1,1 0,0-1,0 1,0 0,1 0,1 1,0 0,0-1,1 1,0 1,1-1,1 0,-3 21,10 185,-5-211,-1 1,1-1,1 0,-1 1,1-1,0 1,0-2,0 1,1 0,0 0,0 0,0 0,2-1,-2 0,8 7,-3-5,1-1,-1 1,0-1,1 0,1 0,-1-1,0-1,16 4,2-1,0-1,1-2,-1 0,0-2,54-3,-65-1,1 0,-1-1,1-1,-1 0,0 0,-1-2,1 0,-1-1,0 0,-1-1,0-1,-1 1,-1-2,1-1,-1 1,0-1,-2 0,0-1,-1 0,15-27,-15 21,0 0,0 1,-2-1,-1 0,6-24,-11 37,0 1,-1 0,0-1,0 0,0 0,-1 0,0 2,0-2,0 0,-1 0,0 1,0 0,-1 0,0 0,1 0,-1 0,-1 0,1 1,-7-8,-12-8,-1 1,0 1,-1 2,-2-1,-52-24,58 32,-1 0,1 2,-1 0,-1 1,1 1,-1 1,0 1,-41-1,60 5,-1-1,1 0,0 1,0-1,0 1,0-1,0 1,0 0,0 1,0-1,0 1,1-1,-1 1,1 0,-1 0,1 0,0 0,0 0,-5 5,-4 10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8791">2276 2198,'-5'2,"0"-1,0 1,0 0,0 0,0 1,1-1,0 1,-1 1,2-1,-1 0,-1 1,-3 4,-5 5,-47 41,3 2,2 3,4 3,-75 111,119-159,-1 0,2 0,1 0,0 1,0-1,2 1,0-1,0 2,1-1,1 0,1 0,3 24,-2-23,3 1,-1 0,1-1,1 0,0 0,2 0,0-1,1 1,0-1,21 26,-25-37,0 1,1 0,1 0,-2-1,1 0,1-1,-1 1,0-1,2 0,-1 0,0 0,0-1,0 0,1 0,-1 0,1-1,-1 0,0 0,2-1,-2 1,1-1,-1-1,1 1,0-1,-1-1,1 1,-1-1,0 0,9-4,-13 6,-1-1,1 0,0 0,-1-1,1 1,-1 0,0 0,1-1,-1 1,0-1,0 1,0 0,0 0,0-1,1 0,-2 1,1-1,0 0,-1 0,1 0,-1 1,0-5,0 2,0 1,-1-2,1 1,-1 0,0 0,-1-1,0 1,1 1,-5-8,2 3,-1 1,0 0,-1 0,0 0,0 0,-1 1,1 0,-1 0,-11-6,-12 0,3 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9292">1758 3143,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10130">3150 2913,'0'5,"0"5,-5 5,-5 9,-7 5,0 7,-6 17,-5 6,-1 0,-10 0,2-6,2-4,3-10,2-11,1-7,6-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11468.02">4243 2300,'-14'0,"1"1,0 0,0 0,1 1,-2 1,2 0,-1 0,1 1,0 1,0 0,0 1,-19 11,19-9,-2-1,2 1,0 1,0 0,2 0,-2 2,2-1,1 1,-1 0,1 0,1 2,1-1,-1 0,2 2,0-2,-4 17,-7 20,-38 136,49-157,1 1,1-1,2 1,2 46,0-71,0 0,1 0,0 0,0 0,0 0,0 0,1 0,0-1,-1 1,1 0,1-1,-1 0,1 1,0-1,0 0,0 0,0 0,0 0,0 0,1-2,-1 1,1 1,0-1,0 0,0-1,0 1,0-1,0 1,0-1,0-1,2 1,6 0,1 0,0-1,0 0,1-1,-2-1,1 0,0 0,0-2,0 1,21-9,-21 5,0 0,0 0,-1-1,1-1,-2-1,0 1,0-1,-1 0,0-1,0-1,-2 1,0-2,0 2,0-2,-2 0,-1 0,1-1,-2 1,1-2,1-17,5-34,4-127,-15 181,1-3,-2-1,-1 1,-4-21,5 31,0 1,-1 0,1-1,-1 1,-1-1,1 1,0 0,-1 0,0 0,0 0,-1 1,0-1,1 1,-1-1,-4-1,-13-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12647">4981 2223,'-22'35,"-36"47,-6 8,61-85,-10 16,-1 2,3-1,0 1,-12 40,22-58,0-1,0 1,0 0,1 1,0-1,0 0,0-1,1 2,-1-1,1 0,1 0,2 8,-2-10,0 1,0-1,1 0,-1 0,1-1,1 1,-1 0,0 0,0-1,0 1,0-1,1 0,-1 0,1 0,1-1,-2 1,1-1,8 1,-4 0,2 0,-2 0,1-1,1 0,-2-1,1 0,0 0,0-1,0 0,0 0,-1-1,2 0,-2 0,0-1,2 0,-3-1,1 0,0 0,12-8,-12 5,0 0,1-1,-2 0,0 0,0-1,0 1,-1-2,-1 1,0 0,0-2,-1 1,1 1,-2-2,3-19,-1 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14191">5008 2657,'-18'0,"-2"0,2 0,-2 1,1 1,-29 6,42-6,1-1,0 1,-1 0,1 1,0-2,1 2,-1 0,1 0,-1 1,0 0,1-1,0 1,1-1,-1 2,1-1,0 1,0-1,0 1,0 0,-1 4,-1 3,1-1,1 1,0 0,0-1,2 1,-1 0,2 0,-1 0,2 0,0 1,0-2,1 1,1 0,4 14,-4-18,0 0,1-1,1 1,-1-1,1 1,0-2,0 1,1 0,0-1,1 0,-1-1,1 1,-1-1,2 0,0 0,-1-2,1 2,1-2,-1 1,17 3,-12-3,0-1,1-1,0-2,0 1,0 0,1-2,-2 1,17-3,-24 2,-1 0,2-1,-2 1,1-1,-1 0,0 0,0-1,1 0,-1 0,-1 0,1 0,-1 0,1 0,-1-1,1 0,-2-1,1 1,-1-1,0 2,0-2,0 0,2-6,1-2,-2-1,0 1,-1-1,0 0,-1 0,-1 0,0-1,-1 1,0 0,-5-25,3 31,-1-1,1 1,-1-1,-2 1,1 0,0 1,0-1,-1 0,0 1,-1 0,-1 0,1 0,0 2,-1-1,0 0,-1 0,1 1,-15-7,-34-9,31 12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15181.03">4953 2146,'4'0,"2"5,0 10,4 15,-1 6,-1 3,-2-1,3-4,-1-3,-1-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16212">5172 1839,'7'1,"0"0,0 1,1 0,-1 0,0 0,0 1,-1 0,2 0,-2 1,0-1,0 1,0 0,1 1,6 7,11 10,37 45,-57-61,145 187,-128-160,0 1,-4 0,1 0,14 49,-15-20,21 131,-28-57,-11 219,-4-326,-1-1,-2 0,0 0,-2-1,-2 0,0-1,-2 0,-20 28,31-52,1 0,0-1,-1 1,1 0,-1-1,0 1,1-1,-1 0,0 1,0-2,-2 1,2 0,0 0,-1-1,1 0,-1-1,-5 2,-40 9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17138">610 2069,'-8'2,"1"0,0 0,0 0,0 1,1 0,-2 0,2 0,0 1,0 0,0 0,0 1,0 0,-7 8,2-3,-61 54,4 2,3 3,-72 100,113-135,1 0,2 2,-26 61,38-73,1 1,1 0,0 0,3 1,1-1,-1 48,4-54,0 0,2 1,0 0,1-1,1 0,2 0,0 0,15 33,-1-17,1 0,1-2,2-1,1-1,2-1,40 36,-51-52</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7383,12 +7483,12 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 133,'0'-4,"9"-2,16 0,22-3,17 0,15 1,8 2,2 3,0-8,3-2,-10 1,-15 3,-18 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="708.96">345 0,'-2'2,"1"-1,-1 1,1-1,0 1,0-1,0 1,0 0,0-1,0 1,0 0,0 0,1 0,-1 0,1-1,-1 1,1 0,0 0,0 0,0 3,-2 1,-33 305,29-215,-31 158,26-182,10-52</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1343.96">107 953,'4'0,"6"0,11 0,1-4,11-2,4 0,0 1,-1 2,-3 1,-2 1,-2 0,-7 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2271.96">1006 847,'2'-16,"1"-1,0 0,2 1,0-1,0 1,2 0,0 1,1 0,15-23,-23 37,1 0,-1 0,1 0,-1 1,1-1,0 0,0 0,-1 0,1 0,0 0,0 1,0-1,-1 0,1 1,0-1,0 1,0-1,0 1,0-1,2 1,-2 0,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 0,1 1,-1 0,1-1,-1 1,1-1,-1 1,0 0,1-1,-1 1,0 0,1-1,-1 1,0 0,0 0,8 54,-8-53,27 711,-26-657</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4681.97">1773 1244,'0'5,"0"10,0 11,0 16,-9 27,-12 15,-16 7,-24 11,-2-8,1-11,11-15,46-37,23-23</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5608.49">2117 821,'-1'-1,"0"0,0-1,0 1,1 0,-1-1,0 1,1-1,-1 0,1 1,0-1,0 1,-1-1,1 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 0,0-1,15-36,-12 29,32-60,3 0,3 3,4 1,101-113,-142 173,0 0,1 1,-1 0,1 0,0 0,0 1,9-5,-14 8,0 1,0-1,0 1,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 1,0-1,1 2,0-1,-1 1,1 0,0 0,-1 0,0 1,1-1,-1 0,0 1,0-1,0 0,0 1,-1-1,1 1,0 2,8 66,-3 0,-3 0,-7 95,0-68,0 30,-1 125,9-216,1-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 127,'0'-4,"10"-1,16-1,24-3,19 1,15 0,9 2,2 3,0-7,3-3,-11 2,-15 2,-20 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="708.95">368 0,'-2'2,"1"-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 0,0 1,0 0,0 0,1 0,-1 0,1-1,-1 1,1 0,0 0,0 0,0 2,-2 2,-36 292,32-207,-33 152,27-174,11-50</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1343.96">114 912,'4'0,"7"0,11 0,2-4,11-2,5 0,-1 2,-1 1,-2 1,-3 1,-2 0,-8 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2271.96">1073 810,'2'-15,"2"-1,-1-1,2 2,0-1,1 1,1-1,1 2,0 0,17-23,-25 36,1 0,-1 0,1 0,-1 1,1-1,0 1,0-1,-1 0,1 0,0 0,0 1,0-1,-1 0,1 1,0-1,1 1,-1-1,0 1,0-1,2 1,-2 0,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 0,1 1,-1 0,1-1,-1 1,2-1,-2 1,0 0,1-1,-1 1,0-1,1 0,-1 1,0 0,0 0,8 52,-8-51,29 680,-28-628</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4681.96">1891 1190,'0'5,"0"9,0 11,0 15,-9 26,-14 15,-16 6,-26 10,-2-7,1-10,11-15,50-36,24-21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5608.49">2258 785,'-1'-1,"0"1,0-2,0 1,1 0,-1-1,0 1,1-1,-1 0,1 1,0-1,0 1,-1-1,1 1,0-1,0 0,1 2,-1-2,0 1,0-1,1 0,0-1,16-34,-13 27,35-57,2 0,4 3,4 1,108-108,-151 165,-1 0,1 1,0 1,0-1,0 0,1 1,9-4,-15 7,0 1,0-1,0 1,0 0,0 0,0-1,0 1,1 0,0 0,-1 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 1,0-1,2 2,-1-2,-1 2,1 0,0 0,-1 0,0 1,1-1,-1 0,0 1,0-1,1 0,-1 0,-1 0,1 1,0 2,8 63,-2 0,-4 0,-7 91,-1-66,1 30,-1 119,9-207,1-8</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7415,12 +7515,12 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 211,'4'0,"15"0,19 0,15 0,12 0,23 0,5 0,-5 0,-3 0,-7 0,-13 0,-12 0,-7 0,-6 0,-6 0,-4 0,-3 0,-5 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="715.99">318 316,'8'185,"45"261,-38-347,-11-54,-3 83,-2-73,1-23</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1347.99">80 1216,'0'-4,"4"-2,7 1,9 0,12 2,3 1,2 1,-2 0,2 1,0 0,7 1,0 3,-3 2,-3 0,-9-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3664.99">742 899,'22'0,"0"0,0 2,0 0,0 1,-1 1,1 2,-1 0,0 1,-1 1,1 1,34 21,-17-8,-14-9,-1 2,0 0,22 21,-39-31,-1 1,1 0,-1 0,0 1,0-1,-1 1,0 0,0 0,0 1,-1-1,0 1,-1-1,0 1,0 0,1 8,0 25,-1 1,-3-1,-1 1,-1-1,-12 50,12-83,0-1,0 1,-1-1,1 0,-1 0,-1 0,0-1,0 1,0-1,0-1,-1 1,0-1,0 0,-1 0,0 0,1-1,-12 5,5-3,1 0,-1-1,0-1,-1 0,1-1,-1-1,1 0,-1 0,-19-1,31-1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,1-1,-1 1,0-1,0 0,1 1,-1-1,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,-2-1,3 2,0-1,-1 1,1-1,0 1,0-1,0 1,0-1,1 1,-1 0,0-1,0 1,1-1,-1 1,1-1,0 1,-1 0,1-1,0 1,0 0,1-2,4-5,1 1,-1 1,1-1,0 1,0 0,1 1,10-7,-2 5,0 1,0 0,0 1,1 0,0 2,0 0,0 1,0 1,0 0,0 1,0 1,1 1,-1 0,32 9,-19-1,0 1,0 2,-1 0,-1 2,-1 1,0 2,27 21,10 8,-39-32</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4357.99">2329 1242,'-9'5,"-3"6,-4 0,1 4,-7 8,-3 9,2 4,5 0,6-2,0-1,-2 6,-3 1,1-1,3-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5400.99">2541 528,'91'-107,"-27"28,57-76,-1 1,-119 153,31-28,-31 29,-1-1,1 1,0 0,0-1,0 1,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,0 0,0 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,0 0,-1-1,1 1,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,0-1,0 1,1 1,5 18,-1 1,-1-1,0 1,-2 0,0 0,-2 0,-2 27,2 33,37 223,1 37,-25-230,-2-17,-10-73</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 203,'4'0,"16"0,20 0,16 0,13 0,24 0,5 0,-5 0,-4 0,-7 0,-13 0,-13 0,-8 0,-5 0,-8 0,-3 0,-3 0,-6 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="715.99">335 304,'9'178,"47"252,-40-335,-12-52,-3 80,-2-70,1-22</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1347.99">84 1171,'0'-4,"5"-2,6 1,10 0,13 2,3 2,2 0,-2 0,2 1,0 0,7 1,1 2,-4 3,-3 0,-9-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3664.99">783 865,'23'0,"0"0,0 2,0 0,1 1,-2 1,1 2,-1 0,0 0,-1 2,1 1,37 20,-19-8,-15-9,-1 3,0-1,24 21,-42-30,-1 0,2 1,-2 0,0 1,1-2,-2 2,0 0,0 0,1 0,-2 0,0 1,-1-1,0 0,0 1,1 7,0 25,0 0,-4 0,-2 0,0 0,-13 47,13-79,0-1,0 0,-1 0,1 0,-2 0,0-1,0 0,0 1,-1-1,1-2,-1 2,-1-1,1 0,-1 0,-1-1,2 0,-13 5,5-3,2 0,-2-2,0 0,-1 0,2-1,-2-1,1 0,-1 0,-19-1,31-1,1 0,1 0,-1 0,0 0,0 0,0 0,0 0,1-1,-1 1,0-1,-1 0,2 1,-1-1,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,-3-1,4 2,0-1,-1 1,1-1,0 2,0-2,0 1,0-1,1 1,-1 0,0-1,0 1,1-1,-1 1,2-1,-1 1,-1 0,1-1,0 1,0 0,1-2,4-4,2 0,-2 1,1-1,1 2,-1-1,1 1,11-6,-2 4,0 1,0 0,0 1,1 1,0 1,0 0,0 1,0 1,0 0,-1 1,1 1,1 1,-1 0,34 8,-20 0,-1 1,1 1,-1 1,-2 1,0 1,-1 3,29 19,10 9,-40-32</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4357.99">2456 1196,'-9'4,"-4"7,-4 0,2 3,-9 8,-2 9,2 4,5-1,6-1,0-1,-1 5,-4 2,1-2,3-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5400.99">2680 508,'96'-103,"-28"27,59-73,0 1,-126 147,33-27,-33 28,-1-1,1 1,0 0,0-1,0 1,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,1 0,-1 1,0-1,0 0,0 1,-1-1,1 1,0-1,0 1,-1-1,1 1,0 0,-1-1,1 1,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1-1,0 0,0 1,1 1,6 18,-2 0,-1-1,0 1,-2 1,1-1,-3 0,-3 26,3 32,39 215,2 35,-28-221,-1-17,-11-69</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7562,13 +7662,13 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1668 86,'0'-1,"1"0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 1,-1 0,0 0,1-1,2 1,37-6,-37 6,319-5,-179 7,-59 3,-47 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="774">1853 324,'4'0,"15"0,19 0,19 0,10 0,7 0,0 0,-8 0,-11 0,-11 0,-11 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2622.01">1 748,'0'5,"4"1,15-5,19-11,6-9,0-6,-6 6,-11 16,-9 21,-9 17,-4 7,-5 5,-1-1,-1-3,5-5,6-5,1-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2092.01">556 801,'0'5,"0"10,0 7,-5 13,-1 11,-8 5,-3-1,3-5,2-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-785">821 827,'1'-2,"1"-1,0 0,0 1,0 0,0-1,0 1,0 0,1 0,-1 0,1 0,0 1,4-3,2-2,78-52,-79 54,-1-1,2 2,-1-1,0 1,1 0,-1 1,1 0,0 0,14 0,-20 2,-1 1,0-1,0 1,0-1,0 1,0 0,0 0,-1 0,1 0,0 0,0 0,-1 1,1-1,-1 0,1 1,-1 0,1-1,-1 1,0 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,0 0,1 0,-1 3,2 10,-1 1,0 0,-2 17,0-17,1 30,1-14,-2 0,-1-1,-8 37,8-59,0 1,-1-1,0 0,-1 0,0 0,-1 0,1-1,-2 1,1-1,-1-1,0 1,-1-1,0 0,-12 9,7-7,1-1,-2-1,1 0,-1-1,0 0,-1-1,-14 4,25-8,-1 0,1 0,-1 0,1-1,-1 1,1-1,-1 0,1 0,-1 0,1 0,-1-1,0 1,1-1,0 0,-1 0,1 0,-1-1,1 1,0-1,0 0,0 0,0 0,0 0,1 0,-1 0,0-1,1 0,0 1,0-1,-1 0,2 0,-1 0,-2-5,3 5,1-1,-1 0,1 1,-1-1,1 1,0-1,1 0,-1 1,1-1,-1 1,1-1,0 1,0-1,1 1,-1 0,1-1,-1 1,1 0,0 0,0 0,1 1,-1-1,4-3,2-3,0 1,1 0,0 1,0 0,1 0,11-6,-9 8,0 0,1 1,0 0,0 1,0 0,0 1,0 0,24 1,-29 1,1 0,-1 1,1 0,-1 0,1 1,-1 0,0 0,0 1,0 0,0 1,0 0,-1 0,1 0,10 10,-6-1,0 0,14 24,-16-23,0 0,0-1,15 14,-23-25,1 0,-1 0,1 0,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0 0,6-1,24-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2439">3282 139,'388'-1,"422"3,-626 11,285 56,107 9,-264-34,-133-13,240 30,397 51,255-44,-1-66,-555-5,2132 3,-2626 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29569.13">8124 113,'0'-2,"2"0,-1-1,0 1,0 0,1-1,-1 1,1 0,-1 0,1 0,0 0,0 1,0-1,4-2,-1-1,6-3,1-1,0 2,0-1,0 2,1-1,0 2,0 0,1 0,-1 1,1 1,0 1,20-2,13 1,0 3,66 7,-107-6,0-1,-1 1,1 0,-1 1,1-1,-1 1,1 0,-1 1,0-1,0 1,0 0,0 1,-1-1,1 1,5 5,-5-3,0 1,-1-1,0 1,0 0,0 0,-1 0,0 1,0-1,3 16,-2 10,-1-1,-1 1,-2-1,-5 46,3-49,1-13,0 0,-2 1,0-1,0 0,-2 0,0-1,-1 0,-14 29,14-35,0 0,-1-1,0 1,0-1,-1-1,0 1,0-2,-1 1,0-1,0 0,0 0,-1-1,0-1,-16 6,15-6,-1 0,-1-1,1 0,0-1,-1-1,-15 0,24-1,1 0,-1 0,1 0,0-1,-1 0,1 1,0-1,-1-1,1 1,0 0,0-1,0 0,0 1,0-1,1 0,-1-1,1 1,-1 0,1-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-3-6,2 1,-1-1,1 1,0-1,1 0,0 0,0 0,1 0,0 0,1 0,0 0,0 1,4-14,-4 19,1-1,-1 1,1 0,0-1,0 1,0 0,0 0,1 0,-1 0,1 1,-1-1,1 1,0-1,0 1,0 0,1 0,-1 1,0-1,1 0,-1 1,1 0,-1 0,1 0,0 0,-1 1,1 0,0-1,0 1,-1 0,1 1,5 0,11 2,0 2,-1 0,0 1,1 1,-2 0,1 2,-1 0,27 19,-26-18,1-1,0 0,24 6,19 8,-46-16</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1734 83,'0'-1,"1"0,0 0,-1 0,1 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 1,-1 0,0 0,1-1,2 1,39-6,-39 6,332-5,-186 7,-62 3,-48 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="774">1927 313,'4'0,"16"0,19 0,20 0,11 0,7 0,0 0,-8 0,-12 0,-11 0,-12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2622.01">1 724,'0'4,"4"2,16-5,19-11,7-8,0-6,-7 6,-10 15,-11 20,-8 17,-5 7,-5 4,-1-1,-1-2,5-5,6-5,2-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2092.02">578 775,'0'5,"0"9,0 7,-5 13,-1 11,-9 4,-3-1,4-4,1-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-785">854 800,'1'-2,"1"-1,0 0,0 1,0 0,0-1,0 2,0-1,1 0,-1 0,2 0,-1 1,4-3,2-2,82-50,-83 52,-1-1,3 2,-2 0,0 0,2 0,-2 1,1 0,1 0,14 0,-21 2,-1 1,0-1,0 1,0-1,0 1,0 0,0 0,-1 0,1 0,1 0,-1 0,-1 1,1-1,-1 0,1 1,-1-1,1 0,-1 1,0 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,0 0,1 0,-1 2,2 11,0 0,-1 1,-2 16,-1-17,2 30,2-14,-4 0,0-1,-8 35,8-56,0 1,-1-1,0-1,-2 1,1 0,-1-1,1 0,-2 1,0-1,0-2,0 2,-1-1,-1 0,-11 8,6-6,2-1,-3-2,2 1,-2-1,1 0,-2-2,-14 5,26-8,-1 0,1 0,-1 0,0-1,0 1,1-1,-1 0,1 0,-1 0,1 0,-2-1,1 1,1-1,0 0,-1 0,1 0,-1-1,0 1,1-1,0 0,0 0,0 1,0-1,1 0,-1 0,0-1,0 0,1 1,0-1,-1 0,2 0,-1 0,-2-4,3 4,1-1,-1 0,1 1,-1-1,1 1,0-1,1 1,-1 0,1-1,-1 1,1-1,0 1,0-1,1 1,-1 1,1-2,-1 1,1 0,0 0,0 0,2 1,-2-1,4-3,2-2,1 0,0 0,0 1,1 1,0-1,12-6,-10 8,1 1,0 0,1 0,-1 1,1 0,-1 1,1 0,24 1,-29 1,0 0,-1 1,2 0,-2 0,1 1,0 0,-1 0,0 1,1 0,-1 1,0 0,0-1,0 1,11 10,-7-2,1 1,14 23,-17-23,0 1,1-2,15 15,-24-26,1 1,-1 0,1 0,-1-1,1 1,1-1,-1 0,0 1,0-1,0 0,0-1,0 1,0-1,0 1,1-1,-1 0,0 0,0 0,6-1,26-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2439">3413 134,'403'0,"439"1,-650 12,295 54,112 8,-274-32,-139-13,249 29,414 49,265-42,-2-64,-576-5,2216 3,-2730 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29569.12">8447 109,'0'-2,"2"0,0 0,-1 0,0 0,1-1,-1 1,1 0,-1 0,1 0,0 0,0 1,0-1,4-2,0 0,5-4,2-1,-1 2,0 0,1 1,0-1,1 2,0 0,0 0,0 2,0 0,1 1,20-2,14 1,0 3,68 7,-110-6,-1-1,-1 1,1 0,-1 1,2-1,-2 1,1-1,-1 2,0-1,1 1,-1 0,0 1,-1-1,1 1,6 4,-6-2,0 1,-1-1,1 1,-1-1,0 1,-1 0,0 1,0-2,3 17,-1 9,-2-1,-1 0,-2 0,-5 45,3-48,1-13,-1 1,-1 0,0 0,0-1,-2 1,0-2,-2 1,-13 27,13-33,1 0,-1-2,0 2,-1-1,0-1,0 0,-1-1,0 1,0-1,-1 0,1-1,-1 0,-1-1,-16 6,16-6,-2-1,0 0,0 0,1-1,-2-1,-15 0,25-1,1 0,-1 0,1 0,-1-1,0 0,1 1,0-1,-1-1,1 1,0 0,0-1,-1 1,1 0,0-1,1 0,-1-1,1 1,-1 0,1-1,0 1,0-1,-1 0,1 0,0 0,0 1,1-1,-3-6,2 1,-1 0,1 0,0-1,1 0,0 1,0-1,1 0,0 1,1-1,0 0,0 1,4-13,-4 18,1-1,-1 1,1 1,0-2,0 1,0 0,0 0,2 0,-2 0,1 1,-1-1,1 1,0-1,0 2,0-1,1 0,0 1,-1-1,1 0,-1 1,1 0,-1 0,1 0,1 0,-2 1,1 0,0-1,0 1,-1 0,1 1,6 0,11 2,-1 2,0 0,0 0,1 2,-3 0,2 2,-1-1,28 19,-28-17,2-1,0-1,25 7,19 7,-47-15</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7622,12 +7722,12 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1033,'5'-9,"0"0,1 0,0 0,1 1,0-1,1 2,12-12,-18 17,-1 1,1 0,-1-1,1 1,0 0,-1 0,1 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 1,0-1,0 1,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 1,0-1,1 1,-1-1,0 1,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0 2,5 15,0 0,-2 1,0 0,-1 0,-1 0,0 0,-2 0,-1 0,-3 28,1-17,2 0,1 0,5 32,15 90,-19-129</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2650.99">821 583,'1016'0,"-964"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3877.99">2647 1535,'5051'0,"-4990"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9547.06">2541 27,'9'0,"25"-4,12-2,11 1,10 0,-2 2,1 1,12 1,24 0,13 1,14 0,3 1,-8-1,-20 0,-24 0,-20 0,-16 0,-16 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10618.06">3176 27,'16'393,"-4"-205,-14 202,-14-299,11-67</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11152.06">2779 1139,'779'0,"-750"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 991,'5'-9,"0"0,2 1,-1-1,1 1,0 0,1 1,13-11,-19 16,-1 1,1 0,-1-1,1 1,0 0,-1 0,2 0,-1 0,0 1,-1-1,1 0,0 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 1,-2-1,1 1,0-1,0 1,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 1,0-1,1 1,-1-1,0 1,0-1,0 1,0 0,0-2,1 2,-1 0,0 0,0 2,5 14,0 0,-2 2,0-1,-1 0,-1 0,0 0,-2 1,-1-1,-3 27,1-16,2-1,1 1,5 30,16 87,-20-124</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2650.99">848 559,'1049'0,"-995"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3877.99">2734 1472,'5216'0,"-5153"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9547.06">2624 26,'9'0,"27"-4,11-2,12 2,10-1,-2 2,1 1,13 1,24 0,14 1,14 0,4 1,-9-1,-21 0,-24 0,-21 0,-17 0,-16 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10618.06">3280 26,'16'377,"-3"-197,-15 194,-15-287,12-64</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11152.06">2870 1092,'804'0,"-774"0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7854,15 +7954,15 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 582,'4'5,"11"1,11 4,20 1,11-2,0-3,0-1,-6 2,-7 0,-6 3,-5 5,-4 0,-7 1,-7 3,-10-1,-7-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1001">133 0,'-3'34,"0"0,-2 0,-2 0,-16 48,-8 40,30-117,0-1,1 1,-1-1,1 1,0 0,0-1,0 1,1 0,-1-1,1 1,0-1,0 1,1-1,0 1,-1-1,2 0,-1 0,0 0,1 0,2 4,3-1,1 0,-1 0,1 0,0-1,1-1,-1 1,17 5,-11-4,1 0,0-2,1 0,-1 0,1-2,18 2,-7-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1600">583 106,'0'9,"0"8,0 14,0 15,0 18,0 12,0 11,0-1,0 3,0 1,-5-7,-1-8,1-4,0-9,2-10,1-10,1-8,0-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2216">1430 212,'0'-4,"4"-2,11 1,21-5,12 1,18-3,14-9,8 0,1 3,5 0,-10 3,-19 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2724.99">1774 53,'-5'0,"-1"14,0 22,1 14,2 12,1 9,1 2,0-3,1-5,1-8,-1-10,0-8,0-6,0-4,1-3,-1-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3225">1535 900,'18'-4,"28"-6,21-2,11 1,-2 4,-10 1,-8 3,-8 2,-9 0,-6 1,-10 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4319">2118 768,'2'-3,"1"-1,-1 0,1 1,0-1,1 1,-1 0,1 0,-1 0,1 0,6-3,49-23,-32 17,35-22,-41 21,1 0,0 2,1 1,0 0,1 2,29-7,-50 15,-1 0,1-1,-1 1,1 0,-1 0,1 1,-1-1,1 0,-1 1,1 0,-1-1,1 1,-1 0,0 0,0 1,1-1,-1 0,0 1,0-1,2 3,-1 0,0-1,-1 1,1 0,-1 0,0 0,0 0,0 0,-1 0,1 1,0 7,0 2,0 1,-1-1,-1 0,-1 1,0-1,-4 20,0-15,0-1,-1 0,-1-1,-1 0,0 0,-13 19,-71 89,87-119,-25 23,14-21,16-8,-1 0,1 0,0-1,-1 1,1 0,0 0,-1 0,1-1,0 1,-1 0,1 0,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,1 0,-1-1,0 0,1-2,0-1,0 0,0 1,0-1,1 1,-1-1,1 1,0 0,0 0,0 0,1 0,-1 0,1 0,0 0,-1 1,1 0,0-1,0 1,1 0,-1 0,0 1,1-1,-1 1,1 0,-1-1,1 2,0-1,0 0,-1 1,7-1,4 1,1-1,-1 2,1 0,-1 1,0 0,24 8,-6-1,-3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4791.99">3070 953,'4'0,"2"9,-13 12,-11 7,-7 8,2 6,-1-3,0-5,-1-3,5-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5833.99">3414 609,'32'-20,"0"-1,-1-2,-1-2,43-44,-4 4,-45 43,54-42,-77 63,0 0,0 0,0 0,0 0,1 0,-1 1,0-1,1 0,-1 1,0 0,1-1,-1 1,1 0,-1-1,0 1,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,0 1,3 0,-2 1,0-1,-1 1,1 0,-1 0,1-1,-1 1,0 0,1 0,-1 1,0-1,0 0,-1 0,1 0,0 4,3 12,-2 1,0-1,-1 26,-1-32,-5 356,-2-66,8-265,-1-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 551,'4'5,"12"1,11 3,21 2,12-3,-1-2,1-1,-7 1,-7 1,-6 2,-6 6,-4-1,-7 1,-7 3,-11-1,-7-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1001">139 0,'-3'32,"0"0,-3 1,-1-1,-17 46,-8 37,31-110,0-1,1 0,-1 0,1 1,0 0,0-2,0 2,1 0,-1-1,1 0,0 0,0 1,1-1,0 1,-1-2,2 1,-1 0,0 0,1-1,3 5,2-1,1-1,0 1,0 0,1-2,0 0,-1 1,19 4,-13-3,2-1,0-1,0 0,0 0,1-3,18 3,-6-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1600">609 100,'0'9,"0"7,0 13,0 15,0 17,0 11,0 10,0 0,0 2,0 1,-5-6,-2-8,2-4,0-8,2-10,1-9,1-8,0-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2216">1494 201,'0'-4,"4"-2,11 2,23-6,12 2,19-4,15-8,7 0,2 3,6 0,-12 3,-19 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2724.99">1853 50,'-5'0,"-2"13,1 22,1 12,2 12,1 8,1 2,0-3,1-4,1-8,-1-9,0-8,0-6,0-4,1-2,-1-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3225">1603 853,'19'-4,"29"-6,22-1,11 1,-1 3,-11 1,-9 4,-7 1,-11 0,-5 1,-11 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4319">2212 728,'2'-3,"1"-1,-1 0,2 1,-1 0,1 0,-1 0,1 0,-1 0,1 0,7-2,51-23,-34 17,36-21,-42 19,1 1,0 2,1 0,0 1,1 1,31-6,-53 14,-1 0,1-1,-1 1,1 0,-1 0,2 1,-2-1,1 0,-1 1,1 0,-1-1,1 1,-1 0,0 0,1 0,0 0,-1 0,0 1,0-1,2 3,-1 0,0-1,-1 0,2 1,-2 0,0 0,0 0,0-1,-1 1,1 1,0 6,0 3,0 0,-1-1,-1 0,-1 2,0-2,-4 19,0-14,0-1,-2 0,0-1,-1 0,-1 0,-13 19,-74 83,91-112,-26 21,14-19,17-8,-1 0,1 0,0-1,-1 1,1 0,0 0,-1 0,1-1,0 1,-1 0,1 0,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,1 0,-1-1,0 0,1-1,0-2,0 0,0 1,0-1,1 2,-1-2,1 1,0 0,0 0,1 0,0 1,-1-1,1 0,0 0,-1 1,1 0,0-1,1 1,0 1,-1-1,0 1,1-1,-1 1,1 0,0-1,0 2,0-1,0 0,-1 1,8-1,3 1,2-1,-1 2,0 0,0 1,0 0,24 7,-5 0,-4-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4791.99">3206 903,'5'0,"1"8,-13 12,-12 7,-7 7,2 6,-1-3,-1-5,0-3,5-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5833.99">3566 577,'33'-19,"1"-1,-2-2,-1-1,45-43,-3 5,-48 40,56-40,-80 60,0 0,0 0,0 0,0 1,1-1,-1 1,0-1,2 0,-2 1,0 0,1-1,-1 1,1 0,-1-1,0 1,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 1,2 0,-2 1,0-2,-1 2,1 0,-1 0,1-1,-1 1,0 0,1 0,-1 1,0-1,0-1,-1 1,2 0,-1 4,3 11,-2 1,0-1,-1 25,-1-31,-5 338,-3-63,9-251,-1-4</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -7948,7 +8048,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2,'481'-2,"552"6,-300 51,-159-6,17-46,-332-6,672 2,-904 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2,'499'-2,"572"6,-311 51,-165-6,17-46,-343-6,696 2,-937 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8031,8 +8131,8 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'329'0,"1364"24,-1490-21,-180-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1586.99">742 238,'27'-1,"53"-10,5-1,-51 10,0 1,0 1,-1 2,1 2,60 14,-84-15,1 0,0 1,-1 1,0 0,0 0,-1 1,1 1,-1-1,10 11,-14-12,0 1,0 0,0 1,-1-1,0 1,0 0,-1 0,0 0,0 0,-1 0,1 1,-2-1,1 1,0 13,-1-15,-1 0,0 0,-1 0,0 0,0 0,0 0,0 0,-1 0,0-1,0 1,0 0,-1-1,0 0,0 0,-1 0,1 0,-1 0,0-1,0 1,0-1,-1 0,0-1,1 1,-1-1,-1 0,1 0,0 0,-1-1,1 0,-1 0,0 0,0-1,0 1,1-2,-10 2,15-3,-1 1,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,0 0,-1 1,1-1,0 0,0 0,-1 1,1-1,0 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0 0,16 12,44 17,-44-23,-15-6,17 7,-1 1,1 1,30 24,-43-30,0 1,-1 0,1 1,-1-1,0 1,0-1,-1 1,0 0,0 0,0 1,-1-1,0 1,0-1,-1 1,2 8,-2-9,0 0,-1 1,1-1,-1 1,0-1,-1 1,0-1,0 1,0-1,-1 0,-2 8,2-11,0 0,0 0,0-1,0 1,0-1,-1 0,1 0,-1 1,1-2,-1 1,0 0,0 0,0-1,0 0,0 1,0-1,0 0,-1-1,1 1,0 0,0-1,-1 0,-5 0,-286-6,270 3,0-1,1-2,-45-14,50 14,-4-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'354'0,"1467"23,-1603-20,-193-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1586.99">798 227,'29'-1,"57"-10,6 0,-56 9,1 1,-1 1,0 2,0 2,65 13,-90-14,1 0,0 0,-1 2,-1 0,1 0,-1 0,1 2,-2-1,12 10,-16-11,0 0,1 1,-1 1,-1-1,1 0,-1 1,-1 0,1-1,-1 1,-1 0,1 0,-2 0,1 0,0 13,0-14,-2 0,0 0,-2-1,1 1,0 0,0-1,0 1,-1 0,0-1,0 0,0 1,-2-1,1 0,0-1,-1 1,0 0,0 0,0-2,-1 2,1-1,-1 0,-1-1,2 1,-1-2,-2 1,2 0,0 0,-2-1,2 0,-2 0,1 0,-1-1,1 0,1-1,-12 2,17-3,-1 1,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,0 0,-1 1,1-1,0 0,0 0,-1 1,1-1,0 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0 0,17 11,47 17,-47-22,-15-6,17 6,-1 2,2 0,31 24,-45-30,-1 2,-1 0,2 1,-2-2,0 2,1-1,-2 1,0-1,0 1,0 1,0-2,-1 2,0-1,-1 1,2 7,-2-8,0-1,-1 2,1-1,-1 0,0 0,-1 1,0-2,0 2,0-1,-1 0,-2 7,2-10,-1 0,1-1,0 0,0 1,0-1,-1 0,0 0,0 1,1-2,-1 1,0 0,-1-1,1 0,0 0,0 1,-1-1,1 0,-1-1,1 1,-1 0,1-1,-1 0,-6 0,-307-6,290 3,0 0,1-3,-48-13,54 13,-5 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8121,17 +8221,17 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 741,'257'-1,"273"3,-274 21,-222-21</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="996.99">54 1032,'1'-1,"0"0,1-1,-1 1,1 0,-1 0,1-1,-1 1,1 1,0-1,0 0,-1 0,1 1,0-1,0 1,0-1,0 1,0 0,3 0,-2-1,78-8,1 3,129 7,-77 2,472-3,-576 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3845.98">2092 53,'8'0,"9"0,14 0,24 0,30 0,18 0,29 0,-5 0,-15 0,-21 0,-18 0,-16 0,-14 0,-10 0,-5 0,-8 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4896.96">2435 0,'4'0,"7"5,0 14,0 14,1 19,0 36,-4 17,-1 0,-4-9,-1-12,-1-12,-1-12,-1-13,1-6,-1-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5512.96">2224 1005,'4'0,"6"0,11 0,15 0,6 0,4 0,0 0,0 0,6 0,4 0,0 0,1 0,-6 0,-11 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6237.96">3176 953,'1'1,"-1"-1,1 0,0 1,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,-1 0,1-1,0 1,-1 0,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 1,1 34,-1-34,-4 51,-14 62,10-68,1 0,0 57,9 51,-2-132</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7729.96">3123 1085,'130'-78,"-96"55,1 1,1 2,59-23,-67 32,-14 5,0 1,1 0,-1 1,1 1,19-2,-30 4,-1 1,1 0,-1 1,0-1,1 1,-1-1,0 1,1 0,-1 0,0 0,0 1,0-1,0 1,0 0,0-1,-1 1,1 1,0-1,-1 0,0 1,1-1,-1 1,0-1,0 1,-1 0,1 0,-1 0,1 0,0 4,5 16,-2 0,-1 1,-1-1,0 1,-2 0,-1 0,-1 0,-1 0,-1-1,-6 26,7-44,0 1,0-1,0 0,-1 0,1 0,-1 0,-1 0,1-1,-1 1,1-1,-1 0,0 0,-1-1,1 1,-1-1,1 0,-1 0,0 0,0 0,0-1,-1 0,1 0,-1-1,-10 2,-11 2,-1-3,1 0,-53-3,46-1,-120-1,182 3,-1 1,1 1,50 11,-66-10,0 1,-1 0,0 0,1 1,-1 1,-1 0,1 1,-1 0,0 0,-1 1,12 12,0 3,-4-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8292.96">3785 1455,'4'0,"6"0,2 14,-1 13,-4 7,-1 6,-3 6,3-6,0-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8688.96">3864 1244,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9635.96">4155 1482,'-56'-20,"51"20,0 1,0 0,0 0,0 0,0 0,1 1,-1 0,0 0,1 0,-1 0,1 1,0 0,0-1,0 2,0-1,0 0,1 1,-1 0,1 0,0 0,0 0,1 0,-1 0,1 1,0 0,-3 8,3-8,0-1,1 1,-1-1,1 1,0-1,0 1,0 0,1 0,-1-1,1 1,1 0,-1 0,1-1,-1 1,1 0,0-1,1 1,-1 0,1-1,0 0,0 1,1-1,-1 0,1 0,0 0,0-1,0 1,6 4,8 4,0-2,29 14,-38-21,-1 0,1 0,0-1,0 0,0 0,0-1,0 0,0 0,11-1,3-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11008.97">4446 847,'2'1,"1"-1,0 1,0 0,0 0,-1 0,1 0,-1 0,1 0,-1 1,1 0,-1-1,0 1,0 0,1 0,-1 0,-1 0,1 0,0 1,0-1,-1 0,0 1,1-1,-1 1,0 0,0-1,1 6,3 9,-1-1,0 1,1 18,-5-33,10 132,-10 189,-4-153,3-3,1-188,1 0,1-1,0 1,2 0,1 0,7-21,-10 35,0 1,0 0,1 1,0-1,1 0,-1 1,1 0,0-1,0 1,0 1,1-1,0 1,0 0,0 0,0 0,1 1,0 0,-1 0,1 0,0 0,0 1,1 0,-1 1,11-2,-15 3,1-1,-1 1,1 0,-1 0,1 1,-1-1,1 0,0 1,-1 0,0-1,1 1,-1 0,1 0,-1 1,0-1,0 0,0 1,0-1,4 4,-3-1,1 1,-1-1,0 0,-1 1,1 0,-1 0,0 0,0 0,1 6,2 11,-1 1,-1 0,0 34,-3-51,0 77,-2-52</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 715,'266'-1,"283"3,-284 21,-230-22</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="996.99">56 996,'1'-1,"0"0,1-1,-1 2,1-1,-1 0,1-1,-1 1,1 1,0-1,0 0,0 0,0 1,0-1,0 1,0-1,0 1,0 0,3 0,-2-1,81-8,1 3,134 7,-81 2,490-3,-597 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3845.98">2167 51,'8'0,"9"0,16 0,23 0,33 0,17 0,31 0,-6 0,-15 0,-21 0,-20 0,-16 0,-14 0,-11 0,-5 0,-8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4896.96">2522 0,'4'0,"7"5,1 13,-1 14,2 18,-1 35,-4 17,-1-1,-3-8,-2-12,-1-12,-1-11,-1-12,1-7,-1-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5512.96">2303 970,'4'0,"7"0,10 0,17 0,5 0,5 0,0 0,-1 0,7 0,4 0,0 0,1 0,-6 0,-12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6237.96">3289 920,'1'1,"-1"-1,1 0,0 1,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,-1 0,2-1,-1 1,-1 0,1 0,-1-1,1 1,-1 0,0 0,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 1,1 33,-1-33,-4 49,-15 60,11-66,0 1,1 54,9 50,-2-128</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7729.96">3234 1048,'135'-76,"-100"54,1 1,2 1,60-21,-69 30,-14 6,-1 0,2 0,-2 1,2 1,19-2,-31 4,-1 1,1 0,-1 1,0-1,2 1,-2-1,0 1,1 0,-1 0,0 0,0 1,0-1,0 1,1 0,-1-1,-1 1,1 1,0-1,-1 0,0 0,1 0,-1 1,0-1,0 1,-1 0,2 0,-2 0,1 0,0 3,5 17,-2-1,-1 1,-1-1,1 1,-3 1,-1-1,-1 0,-2 0,0-1,-6 26,7-44,0 2,0-1,0 0,-1 0,1-1,-2 1,0 0,1-1,-1 1,1-1,-1 0,0-1,-2 0,2 1,-1-1,1 0,-1 0,0 0,-1 0,1-1,-1 0,1-1,-1 0,-11 2,-11 2,-1-3,1 0,-55-3,48-1,-124-1,188 3,-1 1,1 1,51 11,-67-10,-1 0,0 1,-1 0,1 1,0 1,-2 0,2 0,-2 1,0 0,0 1,11 11,1 3,-4-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8292.95">3920 1405,'4'0,"6"0,3 13,-2 13,-4 7,0 6,-4 5,3-5,0-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8688.95">4002 1201,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9635.95">4303 1431,'-58'-20,"53"20,0 1,0 0,-1 0,1 0,0 0,1 1,-1 0,0 0,0 0,0 0,1 1,0 0,0-1,0 2,-1-2,1 1,1 1,-1 0,1 0,0 0,0 0,1 0,-1-1,1 2,-1 0,-2 8,3-9,0 0,1 1,-1-1,1 1,0-1,0 0,0 1,1 0,-1-1,1 1,1 0,-1-1,1 0,-1 1,1 0,0-1,1 1,-1-1,1 0,0 0,0 1,1-1,-1 0,2 0,-1-1,0 0,0 1,6 4,9 4,-1-3,31 14,-40-20,0 0,0 0,0-1,0 0,1 0,-1-1,0 0,1 0,10-1,4-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11008.97">4604 818,'3'1,"0"-1,0 1,0 0,0 0,-1 0,1 0,-1-1,1 1,-1 1,1 0,0-1,-1 1,0 0,1 0,-1 0,-1 0,1 0,0 1,0-1,-1 0,0 1,1-2,-1 2,0 0,0-1,1 6,4 8,-2 0,0 0,1 18,-5-32,10 127,-10 183,-4-148,3-3,1-181,1 0,1-1,0 0,3 1,0 0,7-21,-10 35,0 0,0 0,2 1,-1-1,1 1,-1 0,1 0,0-1,0 1,0 1,2 0,-1 0,0 0,0 0,0 0,2 1,-1 0,-1 0,1 1,0-1,1 1,0 0,-1 1,12-2,-16 3,1-1,-1 1,1 0,-1 0,1 1,-1-1,1 0,0 1,0 0,-1-1,1 1,-1 0,1 0,-1 1,0-1,0 0,0 1,0-1,4 3,-2 0,0 1,-1-1,0 0,-1 1,1-1,-1 1,0 0,0 0,1 6,3 10,-2 1,-1 0,0 33,-3-49,0 74,-2-50</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8158,9 +8258,9 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 952,'0'-1,"1"-1,0 0,0 0,0 0,0 1,0-1,0 1,0-1,1 1,-1-1,0 1,1 0,0-1,-1 1,1 0,2-1,4-4,35-30,2 1,61-35,-87 59,0 1,1 1,0 1,0 1,0 0,1 2,0 0,1 2,24-2,-42 5,33-2,0 2,44 6,-78-5,1 1,0-1,0 1,0-1,-1 1,1 0,-1 1,1-1,-1 1,0-1,0 1,0 0,0 0,-1 0,1 0,-1 1,0-1,0 1,0 0,0-1,-1 1,1 0,-1 0,0 0,1 6,2 14,0-1,-2 1,0 28,-2-33,-1 20,-1 1,-2-1,-2 0,-1-1,-2 1,-2-2,-1 1,-2-2,-2 1,-1-2,-1 0,-2-2,-2 0,-1-1,-1-1,-36 35,46-53,0-1,-1 0,-25 16,35-25,-1 0,1 0,-1-1,1 1,-1-1,0 0,0-1,0 1,0-1,0-1,0 1,0-1,0 0,-10-1,15 1,-1 0,1-1,0 1,-1 0,1-1,0 1,0-1,-1 1,1-1,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,1-1,-1 1,1 0,0-1,0 1,-1 0,1-1,0 1,0-1,0 1,1 0,-1-1,0 1,0 0,1-3,1 1,-1-1,0 1,1-1,0 1,0 0,0 0,0 0,0 0,0 0,1 0,0 0,-1 1,1-1,4-1,1 0,0 0,1 1,-1 0,1 0,-1 1,1 0,0 1,12-1,78 3,-57 1,131 1,-137-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4410.84">1404 0,'24'28,"-1"1,-2 0,-1 2,-1 0,-1 2,-2 0,-2 0,19 63,-30-86,0 0,-1 0,0 1,0-1,-1 13,-1-21,0-1,0 1,0 0,0-1,0 1,0 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,-1-1,1 1,-1 0,0-1,1 1,-1-1,1 1,-1-1,0 0,1 1,-1-1,0 0,0 0,-1-1,-15-2,1 0,0-2,1 0,-1 0,1-2,0 0,-29-18,-5-2,45 25,0 1,0-1,0 1,0 0,0 0,0 0,0 1,-1 0,1 0,0 0,0 1,0-1,-1 1,1 0,0 1,0-1,0 1,1 0,-8 4,-7 5,-1 1,2 1,-21 18,31-25,-17 15,1 1,1 1,1 1,1 1,2 1,0 0,2 2,0 0,2 1,2 0,0 1,-16 61,28-86,0 1,0-1,0 1,0-1,1 1,0-1,0 1,1-1,0 1,-1-1,2 1,-1-1,1 0,0 0,0 1,0-1,1-1,4 8,-4-8,1-1,0 0,0 0,0 0,0-1,0 1,1-1,-1 0,1 0,-1-1,1 1,0-1,0 0,-1 0,1-1,0 1,0-1,0 0,0-1,0 1,8-3,22-3,0-2,0-2,-1-1,0-1,43-24,-1-5,78-57,-142 90,0 0,-1-1,0 0,0-1,9-12,-17 18,0 0,0-1,0 1,-1-1,0 0,0 0,0 0,0 0,-1 0,0 0,0 0,0 0,-1-1,0 1,0 0,0 0,-1-6,-2-4,0-1,0 1,-2 0,0 0,-12-26,1 15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5194.84">2435 105,'-4'0,"0"1,1-1,-1 0,0 1,1 0,-1 0,1 0,-1 0,1 0,0 1,-1 0,-5 4,-7 2,-70 46,1 3,3 4,3 4,3 3,-84 96,131-131,-41 59,63-83,2 0,-1 0,1 1,0-1,1 1,1 0,-1 1,2-1,-1 0,1 1,1 0,-1 11,3-18,0 0,0-1,0 1,0 0,0-1,1 1,-1-1,1 1,0-1,0 0,1 0,-1 0,1 0,-1 0,1 0,0-1,0 0,0 1,0-1,0 0,1 0,-1-1,1 1,-1-1,5 2,1 0,0-1,-1 1,1-2,0 1,0-1,1-1,-1 1,0-2,18-1,12-8,1-2,-1-1,-1-2,71-39,-31 8,85-67,-148 103,-1-1,0 0,-1-1,0 0,0-1,-1-1,-1 0,14-23,-10 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 916,'0'-1,"1"-1,0 0,0 0,0 0,0 1,0 0,0 0,1-1,0 1,-1-1,0 1,1 0,0-1,-1 1,1 0,3-1,3-4,38-28,2 0,66-33,-94 56,0 1,2 2,-1 0,0 1,1 1,0 1,1 0,0 2,26-2,-44 5,34-2,1 2,46 6,-83-5,2 1,-1-1,0 1,1-1,-2 1,1 0,-1 1,2-1,-2 0,0 0,0 1,0 0,1 0,-2 0,1 0,-1 1,0-2,0 2,0 0,1-1,-2 1,1 0,-1 0,0-1,1 7,2 13,1-1,-3 1,0 27,-2-31,-1 18,-1 2,-3-2,-1 1,-1-2,-3 2,-2-2,-1 0,-2-1,-2 0,-1-1,-1 0,-3-3,-1 1,-2-1,0-1,-39 33,49-50,0-2,-1 1,-27 15,37-24,0 0,1 0,-2-2,2 2,-1-1,-1 0,1-1,-1 1,1-1,-1-1,1 1,0-1,-1 0,-10-1,16 1,-1 0,1-1,0 1,-1 0,1-1,0 1,-1-1,0 1,1-1,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 1,0-1,-1 0,2 0,-1-1,0 1,1 0,-1 0,1-1,-1 1,1 0,0-1,0 1,-1 0,1-1,0 1,0-1,0 1,1 0,-1-1,0 2,0-1,1-3,1 1,-1-1,1 1,0-1,0 1,0 0,0 1,0-1,0 0,1 0,0 0,0 0,-1 1,1-1,5-1,0 1,1-1,0 1,0 0,1 0,-2 1,2 0,-1 1,14-1,83 3,-61 1,140 1,-147-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4410.84">1501 0,'26'27,"-2"1,-1 0,-2 2,-1-1,0 3,-3 0,-2 0,20 60,-32-82,0-1,-1 1,1 1,-1-2,-1 13,-1-20,0-1,0 1,0 0,0-1,0 1,0 0,-1-1,1 1,-1 0,1-1,-1 1,1-2,-1 2,-1-1,1 1,0-1,0 1,0-1,0 0,0 0,0 1,-1-1,1 0,0 0,-1 0,1 0,-2-1,2 1,-1 0,0-1,1 1,-1-1,1 1,-1-1,-1 0,2 1,-1-1,0 0,0 0,-1-1,-16-2,0 0,1-2,1 0,-1 0,1-1,0-1,-31-17,-6-2,49 24,-1 1,1-1,0 1,-1 0,1 0,0 0,-1 1,0 0,1 0,-1 0,1 1,0-1,-2 1,2 0,-1 1,1-1,0 1,1 0,-9 4,-8 4,0 2,2 0,-23 18,33-24,-17 14,0 1,2 1,0 2,2 0,1 1,1 0,2 2,0 0,2 0,2 1,0 1,-17 59,30-83,0 0,0 0,-1 1,1-1,1 1,0-2,0 2,1-1,1 1,-2-1,2 0,-1 0,1 0,0 0,0 0,0 0,1-1,5 8,-5-8,1-2,1 1,-1 0,0 0,1-1,-1 1,1-1,-1 0,2 0,-2-1,1 1,1-1,-1-1,-1 1,2-1,-1 1,0-1,1 0,-1-1,0 1,9-2,24-4,-1-2,1-2,-2 0,0-2,47-22,-2-6,84-54,-153 86,1 1,-1-2,0 0,-1 0,11-13,-19 19,0-1,0-1,1 1,-2-1,0 0,0 1,0-1,0 0,-1 0,1 0,-1 1,0-1,-1-1,0 1,0 0,0 1,-1-7,-3-3,1-2,0 2,-2-1,-1 1,-12-26,1 15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5194.84">2603 101,'-4'0,"0"1,0-1,0 0,0 1,1 0,-2 0,2 0,-1 0,1 0,-1 1,0 0,-5 3,-9 3,-73 44,0 3,3 4,4 3,2 4,-89 91,140-125,-44 57,68-81,2 1,-2 0,2 0,-1 0,2 1,1-1,-1 2,2-2,-2 1,2 1,1-1,-1 11,3-17,0 0,0-1,0 1,0 0,0-1,2 0,-2 0,1 1,0-1,0 0,1 0,-1 0,2 0,-2-1,1 1,0-1,0 0,1 1,-1-1,0 0,1 0,-1-1,2 1,-2-1,5 2,2-1,0 0,-2 1,2-2,0 1,-1-1,2-1,-2 1,1-2,19-1,13-7,0-3,0 0,-1-3,75-37,-32 8,90-65,-158 100,-1-2,0 0,-1 0,0-1,0 0,-2-2,0 1,15-23,-11 3</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8242,35 +8342,35 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 931,'8'0,"9"0,18 0,62 0,47 0,20 0,19 0,5 0,-7 0,-20 0,-21 0,-28 0,-30 0,-28 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1031.51">556 905,'3'0,"1"1,-1-1,1 0,0 1,-1 0,1 0,-1 0,1 0,-1 1,0-1,0 1,1 0,-1 0,0 0,0 0,3 4,-1-1,-1 0,0 1,0 0,0 0,-1 0,1 0,-1 0,2 8,2 12,0 1,-2 0,3 40,-7-57,10 525,-14-313,3-181</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2007.52">344 1963,'560'0,"-509"5,-28 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6378.51">1429 2016,'0'-5,"1"-1,-1 1,1 0,1-1,-1 1,1 0,0 0,0 0,1 0,-1 0,1 0,0 1,0-1,7-6,-9 10,0 0,1-1,-1 1,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,-1 1,1-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 1,0 0,-1-1,1 1,0 0,-1 0,1 0,0 1,-1-1,0 0,1 0,-1 1,0-1,1 1,-1-1,0 1,1 3,2 2,0-1,0 1,-1 1,0-1,-1 0,0 1,0-1,0 1,-1 0,1 9,-2 86,-1-65,-3 53,1-51,2-1,1 1,9 59,-3-76</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7279.51">2091 2227,'0'9,"0"8,0 10,0 4,0 2,-9 9,-3 1,-4 3,-4-2,-3 1,-2-8,3-6,1-3,5-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9715.51">2408 1831,'0'0,"0"-1,0 0,0 1,0-1,1 1,-1-1,0 0,1 1,-1-1,0 1,1-1,-1 1,1-1,-1 1,0-1,1 1,-1-1,1 1,0 0,-1-1,1 1,-1 0,1-1,0 1,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 0,1 0,0 1,31 9,122 81,-149-88,0 0,-1 0,0 0,1 1,-1 0,-1-1,1 1,0 1,-1-1,0 0,0 1,0 0,-1 0,1 0,-1 0,0 0,-1 0,2 6,-3-8,1 0,-1 0,0 0,1 0,-2 0,1 1,0-1,-1 0,1 0,-1 0,0-1,0 1,0 0,0 0,0 0,-1-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 0,-1 0,1 0,0 0,-1-1,0 1,1-1,-1 1,0-1,0 0,-3 1,-2 0,1-1,-1 1,0-2,1 1,-9-1,2 1,40 10,-7-4,0 0,-1 1,0 1,0 1,0 0,-2 2,26 20,-37-27,0 0,-1 0,0 0,1 0,-2 1,1-1,-1 1,0 0,0 0,0 1,-1-1,0 0,0 1,-1-1,0 1,0 0,0 0,-1-1,0 1,0 0,-1-1,0 1,0 0,0-1,-1 1,-3 6,4-7,-1-1,0 0,-1 1,1-1,-1 0,0 0,0-1,0 1,-1-1,0 1,0-1,-7 6,7-8,0 0,1-1,-1 1,0-1,0 0,0 0,0 0,0 0,0-1,0 0,0 0,0 0,0 0,-1 0,1-1,0 0,0 0,-5-2,-25-9,1-1,-35-20,24 12,16 5,4-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11615.51">3572 1487,'4'5,"16"1,21-1,19 0,15-2,10-1,-1-1,-10 0,-14-1,-12-1,-9 1,-8 0,-4 0,-2 0,-6-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12380.51">3652 1804,'13'6,"1"0,0-2,0 0,0 0,0-1,1-1,17 1,110-5,-68 0,-48 2,0 2,0 1,27 7,-31-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13605.52">4895 1804,'3752'0,"-1927"99,-569-35,4-63,-725-5,309 3,-820 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14979.51">5901 322,'0'1,"1"0,0-1,0 1,-1-1,1 1,0 0,-1 0,1-1,0 1,-1 0,1 0,-1 0,1 0,-1 0,0-1,1 1,-1 0,0 0,0 0,0 0,0 0,0 2,5 29,-5-26,4 36,-3 0,-1 0,-11 72,-38 122,46-229,1 1,1-1,-1 1,1-1,1 1,0 14,0-20,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1-1,0 1,1-1,-1 1,1-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 0,3 1,25 7,-1 1,40 18,-41-15,0-1,45 10,-70-20,0 0,0-1,0 1,0-1,0 0,0 0,0 0,1-1,-1 1,0-1,0 1,0-1,4-2,7-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15723.51">6377 534,'1'97,"-5"136,1-196,-2-1,-1 0,-2 0,-17 48,16-56,2 1,1 0,1 1,2-1,1 1,2 48,1-42</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17268.55">6615 5,'47'-2,"-33"1,-1 0,0 0,1 1,-1 1,1 0,-1 1,0 0,22 8,-31-7,1 0,-1 0,0 1,-1 0,1 0,-1 0,1 0,-1 0,0 1,-1-1,1 1,-1 0,0 0,0 0,0 0,-1 0,0 0,0 0,0 1,0 8,0 6,0-1,-2 0,0 1,-5 26,4-39,0-1,0 0,-1 1,1-1,-1 0,-1 0,1 0,-1-1,0 1,0-1,-1 0,1 0,-1 0,0-1,-1 0,1 0,-1 0,0 0,0-1,0 0,-11 3,3 0,-1-2,-1 0,1-1,0 0,-1-1,1-1,-1-1,-23-1,36 1,0-1,1 1,-1-1,0 1,1-1,-1 0,1 0,-1 0,1 0,-1 0,1-1,-1 1,1-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1-1,1 1,-1 0,1-1,0 1,0-1,0 1,0-1,0-4,1 5,0-1,0 1,0 0,1 0,-1 0,0 0,1-1,0 1,0 0,0 0,-1 0,2 0,-1 1,0-1,0 0,1 0,-1 1,1-1,-1 0,1 1,0 0,-1-1,1 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,1 1,-1 0,0-1,0 1,0 0,4 0,3 0,1 0,-1 1,1 0,-1 0,1 1,-1 0,0 1,0 0,15 7,6 5,41 29,-49-30,0 0,0-1,29 11,25 0,-54-18</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18831.51">7779 296,'9'0,"16"0,9 0,30 0,17 0,5 0,0 0,0 0,-11 0,-4 0,-1 0,-8 0,-10-9,-9-3,-12 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19784.52">8229 243,'-2'1,"1"0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 1,0-1,-1 1,1-1,0 1,0 2,0 0,-10 87,5 1,7 104,0-92,-12 132,-7 94,17-307</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20599.51">7568 1407,'44'11,"-8"-1,65-1,166-9,-122-2,42-11,-36 1,116 8,-227 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39593.66">10399 1063,'4'-3,"1"0,0 0,0 0,0 1,0-1,0 1,1 0,-1 1,1 0,-1-1,1 2,0-1,5 0,76 2,-80-1,-1 0,1 1,0-1,-1 1,0 1,1-1,-1 1,0 0,0 1,0-1,0 1,0 1,0-1,-1 1,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0 1,-1-1,1 1,-1 0,0-1,-1 1,1 1,-1-1,-1 0,1 1,-1-1,0 0,0 1,-1-1,0 9,1 34,0 2,-2 1,-10 63,8-105,0 0,0 0,-1-1,-1 0,1 1,-2-1,1-1,-1 1,0-1,-1 0,0 0,-15 12,1-3,0-1,-1-1,-44 23,57-34,0 0,0-1,0 0,0-1,0 0,0 0,-1-1,1-1,-1 1,1-1,-18-3,24 3,0-1,1 1,-1-1,0 0,0 0,0 0,0 0,0 0,1-1,-1 1,1-1,-1 0,1 0,-1 0,1 0,0 0,0 0,0 0,0-1,1 1,-1-1,1 0,-1 1,1-1,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,2-3,-1-1,1 1,0-1,0 1,0 0,1 0,0 0,0 1,1-1,-1 1,1-1,0 1,1 0,-1 1,1-1,0 1,0 0,0 0,1 0,0 1,-1 0,1 0,0 0,0 1,1 0,-1 0,0 1,12-2,-7 2,1 0,0 1,-1 0,1 0,0 1,-1 1,1 0,-1 1,0 0,0 1,0 0,0 1,0 0,19 12,79 51,-88-57</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41901.66">11378 931,'646'0,"-618"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43910.66">14182 1989,'185'-13,"3"-1,164-16,-262 19,83-1,201 10,-168 5,929-3,-1111 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="46712.66">13097 270,'4'0,"25"0,20 0,7 0,7 0,-3 0,-2 0,-7 0,-7 0,-3 0,1 0,-1 0,0 0,2 0,4 0,-3 0,-8 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="47565.66">13521 270,'0'798,"-3"-754,-11 67,2-29,11-72,0 1,-1 0,0-1,-1 1,0-1,-1 0,0 0,0 0,-1-1,-8 13,-7 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48212.66">12965 1487,'162'-13,"-11"-1,194 14,-319 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="50926.66">13838 1354,'1'-4,"1"-1,0 1,0-1,1 1,0 0,-1 0,1 0,1 0,-1 0,0 1,1-1,0 1,5-4,-2 1,1-1,-1 0,1 1,0 0,1 0,-1 1,19-8,-25 12,0 1,0-1,0 1,0-1,1 1,-1 0,0-1,0 1,1 0,-1 1,0-1,0 0,0 1,1-1,-1 1,0 0,0-1,0 1,0 0,0 0,0 0,0 1,0-1,-1 0,1 1,0 0,-1-1,1 1,-1 0,0-1,1 1,-1 0,0 0,0 0,0 0,1 4,3 7,-1 0,0 1,0 0,-1 0,-1 0,0 24,-6 93,0-53,3 16,1-69</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51681.67">14473 1672,'4'0,"2"9,-4 8,-4 5,-5 3,-1 2,0 2,2-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56574.66">14791 1196,'40'-2,"1"-2,0-3,-1 0,-1-3,59-22,-14 6,-61 19,1 2,0 1,0 0,0 2,0 1,0 1,37 4,-57-3,0 0,1 0,-1 0,0 1,-1 0,1-1,0 1,0 1,-1-1,1 1,-1-1,0 1,0 0,0 0,0 0,0 1,-1-1,1 0,-1 1,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,0 0,0 6,2 15,-1-1,-1 0,-4 46,1-39,1-13,0 0,-1 1,0-1,-2-1,0 1,-1 0,-1-1,0 0,-1 0,-1-1,-1 0,0 0,-1-1,-1 0,0-1,-21 20,20-22,-1-2,1 0,-2 0,1-1,-1-1,-1 0,-24 9,29-13,-1-1,1 0,-1-1,1 0,-1 0,0-1,0-1,1 0,-1 0,0-1,0-1,-15-3,24 5,1-1,-1 1,0 0,1-1,-1 0,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,0-1,0 1,1-1,-1 1,0-3,0 1,1 0,1 1,-1-1,0 1,0-1,1 1,0-1,-1 1,1-1,0 1,0 0,0 0,1-1,1-2,3-3,0 1,0-1,0 1,1 0,0 0,1 1,11-7,-10 8,-1 1,1 0,1 0,-1 1,0 1,1-1,0 1,-1 1,1 0,0 1,0-1,0 2,-1-1,19 5,5 3,-1 2,63 27,12 4,-79-31,-7-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65000.19">8996 2360,'-1'1,"0"-1,0 0,1 1,-1-1,0 0,0 1,1-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1 0,1-1,-1 1,1 0,0 0,0-1,-1 1,1 0,0 1,-6 26,5-20,-11 38,-1 0,-3-1,-2 0,-1-2,-49 80,67-121,-1 0,1 0,0 0,0 0,0 1,0-1,0 0,0 1,0-1,1 0,0 1,-1-1,1 1,0-1,0 1,0-1,0 0,1 1,-1-1,1 1,-1-1,1 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 0,1 0,-1-1,1 1,0 0,-1 0,1-1,0 1,0-1,0 0,0 1,1-1,-1 0,0 0,4 1,13 5,0-1,0-1,0 0,28 3,-28-5,48 8,239 46,-275-51,-3-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65892.2">9631 2360,'0'82,"-3"0,-4-1,-31 146,-5-62,-51 241,75-305,15-78</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="68809.21">10028 2227,'19'-1,"-1"-1,1 0,0-2,21-7,-1 1,66-15,1 5,121-9,-221 29,-1-1,0 1,1 0,-1 1,0-1,0 1,1 0,-1 1,0-1,0 1,0 0,-1 0,10 6,-11-5,0-1,-1 1,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,-1-1,0 1,0 0,0-1,0 1,0 0,-1-1,1 1,-1 0,0 7,0 1,0 1,-1 0,0-1,-1 1,0-1,-1 1,0-1,-1 0,0 0,-1-1,-1 1,1-1,-2 0,0 0,0-1,-1 0,-9 9,-15 11,0-2,-3-1,-59 36,73-50,-1 0,-1-2,0-1,-29 10,44-18,1 0,0 0,0-1,-1 0,1 0,-1-1,1 0,-1 0,1-1,0 0,-1 0,1-1,0 0,0 0,0-1,0 1,0-2,1 1,-8-5,12 7,0 0,0-1,0 1,1 0,-1-1,0 1,0-1,1 0,-1 1,1-1,0 0,-1 0,1 0,0 0,0 0,0 0,1 0,-1-1,0 1,1 0,-1 0,1-1,0 1,0 0,0 0,0-1,0 1,0 0,1-1,-1 1,1 0,-1 0,1 0,0-1,0 1,0 0,0 0,0 0,1 0,-1 1,3-4,1 0,0 0,0 1,0-1,0 1,1 0,-1 1,1-1,0 1,0 0,1 1,-1-1,1 1,6-1,-5 2,0 1,0-1,1 2,-1-1,0 1,0 0,0 1,0 0,15 5,2 4,39 23,-9-4,8 6,-45-25,1 0,24 10,29 19,-57-31,0 0,0-1,25 10,-13-10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="69454.2">11060 2968,'165'-2,"178"5,-169 23,-91-15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70751.2">12409 2942,'-2'0,"1"0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-1-1,1 1,0 0,-1 0,1-1,0-1,-5-41,5 39,1-25,1-1,2 1,1 0,1 0,1 0,2 1,20-46,-29 74,0 1,0 0,0-1,0 1,1-1,-1 1,0-1,0 1,0 0,0-1,0 1,1-1,-1 1,0 0,0-1,1 1,-1-1,0 1,1 0,-1 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1 0,-1 0,0-1,1 1,-1 0,1 0,0 0,4 16,-2 35,-3-48,-2 824,6-752,2-51</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 892,'8'0,"10"0,18 0,65 0,49 0,21 0,19 0,6 0,-8 0,-21 0,-21 0,-30 0,-30 0,-30 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1031.51">578 867,'3'0,"2"1,-2-1,1 0,0 1,-1 0,1 0,-1 0,2 0,-2 1,0-1,0 1,1 0,-1 0,0-1,0 1,4 4,-2-1,-1 0,0 0,0 1,1 0,-2 0,1-1,-1 1,2 8,2 11,1 0,-3 1,3 38,-7-54,11 503,-15-301,3-172</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2007.52">358 1881,'582'0,"-529"5,-29 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6378.51">1486 1932,'0'-5,"1"-1,-1 1,1 1,2-2,-2 1,1 0,0 1,0-1,1 0,-1 0,1 0,0 2,0-2,8-6,-10 10,0 0,1-1,-1 1,1 0,-1 0,1 1,0-1,-1 0,1 0,0 0,1 0,-2 1,1-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,1 1,-1-1,0 1,0 0,-1-1,1 1,0 0,-1 0,1-1,0 2,-1-1,0 0,1 0,-1 1,0-1,2 1,-2-1,0 1,1 3,2 1,0 0,0 1,-1 1,0-2,-1 1,1 1,-1-2,0 2,-1 0,1 8,-2 83,-1-63,-3 51,1-48,1-2,2 1,10 57,-4-73</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7279.51">2175 2134,'0'9,"0"7,0 10,0 3,0 3,-9 8,-4 2,-4 2,-3-2,-4 1,-2-8,3-5,1-3,5-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9715.51">2505 1754,'0'0,"0"0,0-1,0 1,0-1,1 1,-1-1,0 0,1 1,-1-1,0 1,1-1,-1 1,1-1,-1 1,0-1,1 1,-1-1,1 1,0 0,-1-1,1 1,-1 0,1-1,0 1,-1 0,1 0,0 0,-1-1,1 1,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 0,1 0,0 1,33 9,126 77,-155-84,0-1,0 1,-1 0,1 1,-1 0,-1-1,1 1,0 0,0 0,-1 0,0 1,0 0,-1-1,1 1,-1 0,0 0,-1 0,2 5,-3-7,2 0,-2 0,0 0,1 0,-2-1,1 2,0-1,-2 0,2 0,-1 0,0-1,0 1,0-1,0 1,0 0,-1-1,0 1,1-1,-1 1,0-1,0 1,0-2,0 1,-1 0,0 0,1 0,-1-1,0 1,1-1,-1 1,0-1,0 0,-4 1,-1 0,1-1,-1 0,-1-1,2 1,-10-1,3 1,41 10,-7-4,-1-1,0 2,0 1,-1 0,1 1,-2 1,27 20,-39-26,0 0,-1-1,0 1,1 0,-1 1,0-2,-1 2,0 0,0 0,0 0,-1 0,0 0,0 1,-1-2,1 2,-1 0,0-1,-1 0,0 1,0 0,-1-2,0 2,-1 0,1-1,-1 0,-3 7,4-8,-1 0,0 0,-1 1,1-1,-1-1,0 1,-1-1,1 1,-1-1,0 0,0 0,-8 6,8-8,0 0,1-1,-1 1,0-1,-1-1,1 1,0 0,0 0,0-1,0 0,-1 0,1 0,0 0,-1 0,1-1,0 0,-1 0,-4-1,-26-10,0 0,-35-20,24 12,17 5,4-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11615.51">3715 1425,'5'5,"15"0,23 0,19 0,16-2,11-1,-2-1,-10 0,-14-1,-13-1,-10 1,-8 0,-4 0,-2 0,-6-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12380.51">3799 1729,'13'5,"2"1,-1-2,1 0,-1 0,1-2,1 0,17 1,115-5,-71 0,-50 2,0 2,0 1,28 7,-32-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13605.52">5092 1729,'3902'0,"-2004"94,-591-32,4-61,-755-5,322 3,-853 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14979.51">6138 309,'0'1,"1"-1,0 0,0 1,-1-1,1 1,0 0,-1 0,1-1,0 1,-1 0,1 0,-1 0,1 0,-1 0,0-1,1 1,-1 0,0 0,0 0,0 0,0 0,0 2,6 27,-6-24,4 34,-3 1,-1-1,-12 69,-39 117,48-219,1 1,1-2,-1 2,1-1,1 0,0 14,0-19,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1-1,0 0,1 0,0 1,0-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1-1,-1 0,3 1,26 6,-1 2,42 17,-43-15,0 0,47 9,-73-19,0 0,0-1,1 1,-1-1,0 0,0 0,0 0,1-1,-1 1,0-1,1 1,-1-1,4-2,8-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15723.51">6633 512,'1'93,"-5"130,1-188,-2 0,-2-1,-1 1,-18 45,17-53,1 1,2 0,1 0,2 0,1 1,2 46,1-41</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17268.55">6881 5,'48'-2,"-33"1,-1 0,-1 0,2 1,-2 1,2 0,-2 1,1 0,22 7,-32-6,2 0,-2 0,0 1,-1 0,1-1,-1 1,1 0,0 0,-1 1,-1-1,1 0,-1 1,0 0,0 0,0 0,-1-1,0 1,0 0,0 1,0 7,0 6,0-1,-2 1,0 0,-5 25,4-37,0-2,0 1,-1 1,1-1,-1-1,-2 1,2 0,-1-1,0 0,0 0,-1 0,0 0,0 0,0-2,-1 1,1 0,-2 0,1 0,0-1,0-1,-12 4,3 0,0-2,-2 0,2-2,-1 1,-1-1,2-1,-2-1,-23-1,36 1,1-1,1 1,-1-1,0 1,1-1,-1 0,1 0,-1 0,0 1,0-1,1-1,-1 1,1-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-2-1,2 2,-1-1,1-1,0 1,0-1,0 1,0-1,0-4,1 6,0-2,0 1,0 0,1 0,-1 0,0 0,1-1,0 1,0 0,0 0,-1 1,2-1,-1 1,0-1,1 0,0 0,-1 1,1-1,-1 0,1 1,0 0,-1-1,1 1,0 0,0 0,0 0,0 1,0-1,1 0,-1 1,0-1,1 1,-1 0,0-1,0 1,0 0,4 0,4 0,0 0,-1 1,2 0,-2 0,2 0,-2 1,0 1,1 0,15 7,6 4,43 28,-51-28,0-1,-1 0,31 10,26 0,-56-18</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18831.5">8091 284,'10'0,"16"0,9 0,32 0,17 0,5 0,1 0,-1 0,-11 0,-4 0,-1 0,-9 0,-9-9,-11-2,-12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19784.52">8559 233,'-2'1,"1"0,0 0,0 0,0 0,0 0,0 1,0-2,0 1,0 0,0 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 1,0-1,-1 1,1-1,0 1,0 1,0 1,-11 83,6 2,7 98,0-87,-12 126,-8 90,18-293</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20599.5">7872 1348,'46'11,"-9"-2,68 0,173-9,-127-2,43-10,-37 0,121 8,-236 4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39593.65">10817 1019,'4'-3,"1"0,0 0,0 0,1 1,-1-1,0 1,1 0,-1 2,2-1,-2-1,1 2,0-1,6 0,78 2,-83-1,0 0,0 1,0-1,0 1,-1 1,1-2,-1 2,1 0,-1 1,0-1,0 1,1 1,-1-1,-1 1,0-1,0 1,1 0,-1 1,-1-1,1 0,-1 1,0 1,0-1,0 0,-1 1,0-1,-1 1,1 0,-1 0,-1 0,1 1,-1-2,0 1,0 1,-1-1,0 8,2 33,-1 2,-2 1,-11 60,9-101,0 1,0 0,-1-2,-2 1,2 0,-2 0,1-1,-1 0,-1 0,0 0,0-1,-16 13,1-4,0-1,-1 0,-45 21,58-32,1 0,0-2,-1 1,1-1,-1 0,1 0,-1-1,0-1,0 1,1-1,-20-3,26 3,0-1,1 1,-1-1,0 0,0 0,0 0,0 0,-1 0,2 0,-1 0,1-1,-1 0,1 0,-1 0,1 0,0 0,0 0,-1 0,1-1,1 1,-1 0,1-1,-1 1,1-1,0 0,0 0,0 0,0 0,1 1,-1-1,1 0,0 0,0 0,0 0,0 0,0 0,1 1,-1-1,2-3,-1-1,1 1,0 0,0 0,0 0,2 0,-1 1,0 0,1-1,-1 1,1 0,0 0,2 0,-2 1,1-1,0 2,0-1,1 0,0 0,0 1,-1 0,1 0,1 1,-1 0,1 0,-1 0,1 1,11-2,-6 2,0 0,1 1,-2 0,2 0,-1 1,0 1,0 0,0 1,-1 0,0 0,1 1,-1 1,1 0,19 11,82 49,-91-54</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41901.65">11835 892,'672'0,"-643"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43910.66">14751 1906,'193'-13,"2"0,172-16,-274 19,87-2,209 10,-175 5,967-3,-1156 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="46712.66">13623 259,'4'0,"26"0,21 0,7 0,8 0,-4 0,-1 0,-8 0,-7 0,-4 0,2 0,-2 0,1 0,2 0,4 0,-3 0,-9 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="47565.66">14064 259,'0'764,"-3"-721,-12 63,3-28,11-68,0 1,-1-1,0 0,-2 0,1 0,-1-1,0 1,0 0,-1-2,-9 13,-7 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48212.66">13486 1425,'168'-13,"-11"0,202 13,-332 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="50926.66">14394 1297,'1'-3,"1"-2,0 1,0-1,1 1,0 1,-1-1,1 0,2 0,-2 0,0 1,1-1,0 2,5-5,-1 1,0-1,-1 1,2 0,-1 0,1 0,0 2,19-9,-26 12,0 1,0-1,0 1,0-1,1 1,-1 0,0-1,1 1,0 0,-1 1,0-1,0 0,0 1,1-1,-1 1,0 0,0-1,0 1,0 0,1 0,-1 0,0 1,0-1,-1 0,1 1,0 0,-1-1,1 1,-1 0,0-2,1 2,-1 0,0 0,0 0,0 0,2 4,2 6,-1 1,0 0,0 1,-1-1,-1 0,0 24,-6 88,0-50,3 15,1-66</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51681.67">15054 1602,'4'0,"3"9,-5 7,-4 5,-6 3,0 2,0 2,1-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56574.66">15385 1146,'42'-2,"0"-2,1-2,-2-1,0-3,61-20,-15 5,-63 18,1 2,0 1,0 1,0 1,0 1,0 1,38 3,-58-2,-1 0,1 0,-1 0,0 1,-1 0,2-1,-1 1,0 1,-1-1,1 1,-1-1,0 0,1 1,-1 0,0 0,0 1,-1-1,1 0,-1 1,0-1,0 1,0 0,-1 0,2 0,-2 0,0-1,0 1,0 6,2 14,-1-1,-1 0,-4 44,1-37,1-13,0 0,-1 1,-1-1,-1 0,0 0,-1 0,-1 0,-1-1,0 0,-1-1,-1 1,-1-1,0-1,-2 1,1-2,-22 20,20-22,0-1,0 0,-1-1,0 0,-1-2,0 1,-26 8,31-12,-2-1,2 0,-1-1,0 0,0 0,-1-1,1-1,0 0,0 0,0-1,-1-1,-15-3,25 5,1-1,-1 1,0 0,1-1,-1 0,1 1,-1-1,1 0,0 0,-2 0,2 0,0 0,-1 0,1 0,0 0,0 1,0-2,0 1,0 0,0-1,0 1,1-1,-1 1,0-3,0 1,1 0,1 1,-1 0,0 0,0-1,1 1,0-1,-1 1,1-1,0 1,0 0,0 0,1 0,1-3,4-3,-1 1,0 0,0 0,2 0,-1 1,1 0,12-7,-11 9,0 0,0 0,1 0,0 1,-1 1,1-1,1 2,-2 0,2 0,-1 1,0-1,1 2,-2-1,20 4,6 4,-2 2,66 25,12 4,-82-29,-7-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65000.18">9357 2261,'-1'1,"0"-1,0 0,1 1,-1-1,0 0,0 1,1-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1 0,1-1,-1 1,1 0,0 0,0-1,-1 1,1 0,0 1,-7 25,6-20,-11 37,-2 0,-2-1,-3 1,-1-3,-51 77,70-116,-1-1,1 1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,1 0,0 1,-1-2,1 2,0-1,0 1,0-1,0 0,1 1,-1-1,1 1,-1-1,1-1,0 2,0-1,0 0,0 0,0 1,1-1,-1 0,2 0,-2-1,1 1,0-1,-1 1,1-1,0 1,0-1,0 0,0 1,1-1,-1 0,0 0,5 1,12 5,1-2,0 0,0 0,29 3,-30-6,51 9,248 44,-285-50,-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="65892.2">10018 2261,'0'79,"-3"0,-5-2,-31 141,-6-60,-53 231,79-292,14-75</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="68809.2">10431 2134,'19'-1,"0"-1,1 0,0-2,21-6,0 0,68-14,1 5,126-9,-229 28,-2-1,0 1,1 0,0 1,-1-1,0 1,1 0,-1 1,1-1,-1 1,0 0,-1 0,11 5,-12-4,0-1,-1 1,1 0,-1 0,0 0,0 1,0-2,1 1,-1 1,-1-1,0 1,0 0,0-1,0 0,0 1,-1-1,1 1,-1 0,0 6,0 2,0 0,-1 1,0-2,-1 2,0-2,-1 2,-1-2,0 1,0-1,-1 0,-1 0,0 0,-1-1,0 1,0-2,-2 1,-8 8,-17 11,1-2,-3-1,-62 34,76-48,-1 1,-1-3,0 0,-30 9,46-17,1 0,-1 0,1-1,-1 0,0 0,0-1,1 0,-2 0,2-1,0 0,-1 0,0-1,1 0,0 0,-1-1,1 1,0-1,1 0,-9-5,13 7,0 0,0-1,0 1,1 0,-1-1,0 1,0 0,0-1,0 1,1-1,0 0,-1 0,1 0,0 0,0 0,0 0,1 0,-1-1,0 2,1-1,-1 0,1-1,0 1,0 0,0 0,0-1,0 1,0 0,1-1,-1 2,1-1,-1 0,1 0,0-1,0 1,0 0,0 0,0 0,1 0,-1 1,4-3,0-1,0 0,0 1,0-1,1 2,0-1,-1 1,1-1,0 1,1 0,0 1,-1-1,2 2,5-2,-5 2,1 1,-1-1,1 2,0-1,-1 1,0 0,1 1,-1-1,16 6,2 4,40 21,-8-3,7 6,-46-25,1 1,24 9,31 18,-59-29,0-1,-1 0,27 9,-14-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="69454.2">11504 2844,'172'-2,"184"5,-175 22,-94-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70751.2">12907 2819,'-2'0,"1"0,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 0,0 0,1 0,-2 0,2 0,0 0,-1-1,1 1,0 0,-1 0,1-1,0-1,-5-39,5 37,1-23,1-2,2 1,2 0,0 1,1-1,3 1,20-44,-30 71,0 1,0 0,0-1,0 1,1-1,-1 1,0-1,0 1,0 0,0-1,0 1,1-1,-1 1,0 0,0-1,1 1,-1 0,0 0,1 0,-1 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1 0,-1 0,0-1,1 1,-1 0,1 0,0 0,4 15,-2 34,-3-46,-2 789,7-720,1-49</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8408,11 +8508,11 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 514,'121'-2,"131"5,-250-3,0 0,-1 0,1 0,0 1,-1-1,1 0,0 1,-1-1,1 1,0 0,-1-1,1 1,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 1,1-1,-1 0,0 1,0-1,1 4,-1-3,-1 1,1 0,-1-1,0 1,0 0,0 0,0-1,0 1,-1 0,1-1,-1 1,0 0,0-1,-1 4,-3 3,1 0,-1 0,0-1,-1 1,0-1,-1 0,-12 12,17-20,1 1,0 0,0 0,-1 0,1 1,0-1,0 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,1-1,-1 1,1-1,-1 3,1-2,1-1,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,1 0,8 4,-1-1,1 0,0 0,17 3,-14-3,2-1,-1 1,0 1,0 0,0 1,23 15,-33-18,1 1,-1 0,0 0,0 0,-1 0,1 1,-1 0,0 0,0 0,0 0,-1 0,0 0,0 1,0-1,-1 1,0-1,0 1,0 7,0-6,0 0,0 0,-1 1,0-1,-1 0,1 0,-1 0,-1 0,1 0,-1 0,-1 0,1 0,-1-1,0 1,-1-1,1 0,-1 0,-1 0,1 0,-1-1,0 0,0 0,0 0,-1 0,0-1,0 0,0 0,0-1,-1 0,1 0,-10 3,12-5,-35 9,-51 6,78-15,1 0,-1-1,1 0,-1 0,1-2,-1 1,1-1,0-1,-15-5,3-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="806">1165 223,'-7'1,"1"1,-1-1,1 1,0 0,0 0,0 1,0 0,0 0,0 0,1 1,0 0,-1 0,2 0,-1 1,-5 5,-13 15,-30 43,45-56,-30 38,3 2,2 2,3 1,-28 68,57-120,0-1,0 1,0-1,1 1,-1 0,1-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,1-1,0 1,-1-1,1 1,1-1,1 4,-1-2,1-1,0 0,0 0,1 0,-1 0,0-1,1 1,0-1,-1 0,1 0,7 2,8 2,1-1,0 0,-1-2,31 2,314-1,-297-5,-43 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1424">1351 223,'4'0,"2"9,0 21,-2 19,-1 28,-1 19,-1 12,0 22,-1 4,0-13,4-18,1-21,1-21,-2-16,-1-11,-1-7,-1-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2214">1668 12,'2'-1,"0"0,0-1,0 1,0 0,0 0,1 0,-1 0,0 1,1-1,-1 0,1 1,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,1 0,-1 0,0 0,0 0,0 0,0 1,0-1,0 1,2 1,9 6,-2 1,1 0,-2 1,11 12,5 11,-1 1,-2 1,24 50,48 127,-69-149,-3 1,-3 2,-3 0,-3 0,-3 2,-2 0,-4 0,-4 80,-3-112,-1 0,-2 0,-2 0,-1-1,-2 0,-1-1,-2 0,-2-1,0 0,-24 34,12-24</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2874">2541 673,'338'14,"7"1,-165-16,-98 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 494,'127'-2,"137"5,-262-3,0 0,0 0,0 0,0 1,-1-1,1 0,0 1,-1-1,1 1,0 0,-1-1,1 1,-1 0,2 0,-2 0,1 0,-1 0,0 0,0 1,1-1,-1 0,0 1,0-1,1 3,-1-2,-1 1,1 0,-1-1,0 1,0 0,0 0,0-1,0 0,-1 1,1-1,-1 1,0 0,0-1,-1 4,-3 2,1 1,-2 0,1-2,-1 2,-1-1,0-1,-13 13,18-20,1 1,0 0,0 0,-1-1,1 2,0-1,0 0,0 0,0 1,0-1,-1 0,2 1,-1-1,0 1,1-1,-1 1,1-1,-1 3,1-2,1-1,-1-1,0 1,1 0,-1 0,0 0,1 0,-1 0,1 0,1 0,-2 0,1 0,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,1 0,8 4,0-1,0-1,1 1,17 3,-14-3,2-1,-2 1,1 0,0 1,-1 1,25 14,-35-17,2 1,-2 0,0 0,0-1,-1 1,2 1,-2 0,0 0,0-1,0 1,-1 0,0 0,0 1,0-2,0 2,-1-1,0 1,0 6,0-5,0 0,0 0,-1 0,0 0,-1 0,1-1,-1 1,-1 0,1 0,-2-1,0 1,1 0,-1-1,0 0,-1 0,1 0,-2 0,0-1,1 1,-1-1,-1 0,1 0,0-1,-1 1,-1-1,1 0,0 0,0-1,-2-1,2 1,-11 3,13-5,-37 9,-53 5,81-14,1 0,0-1,0 0,0 0,0-2,0 1,0-1,1-1,-17-4,4-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="806">1222 214,'-7'1,"0"1,0-1,1 1,0 0,-1 0,1 1,0 0,-1 0,1 0,1 0,0 1,-2 0,3 0,-1 1,-6 4,-13 15,-31 42,46-55,-31 37,4 2,1 2,4 1,-30 66,60-117,0 0,0 1,0-1,1 1,-2 0,2-1,0 1,0 0,0-1,0 0,0 1,0-1,2 1,-2 0,1-1,0 1,-1-1,1 1,1-1,1 3,-1-1,1-1,0 0,0 0,2 0,-2 0,0-1,1 0,0 0,-1 0,2 0,6 2,9 2,1-1,0-1,-1-1,32 2,330-1,-311-5,-46 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1424">1417 214,'4'0,"3"9,-1 20,-2 18,-1 27,-1 18,-1 12,1 21,-2 4,0-12,4-18,1-21,1-19,-2-16,0-10,-2-7,-1-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2214">1750 12,'2'-1,"0"0,0-1,0 1,0 0,0 0,2 0,-2 0,0 1,1-1,-1 0,1 1,-1 0,0 0,1 0,0 0,0 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,2 0,-2 0,0 0,0 0,0 0,0 1,0-1,0 1,2 0,10 7,-2 1,0-1,-1 2,11 11,5 11,-1 0,-2 2,26 48,49 121,-71-142,-4 0,-3 3,-3-1,-4 1,-2 1,-3 0,-4 1,-4 76,-3-107,-1-1,-2 1,-2-1,-2 0,-1 0,-2-2,-1 1,-3-1,0-1,-25 34,13-24</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2874">2666 647,'354'14,"8"0,-173-15,-103 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8439,20 +8539,20 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">187 688,'4'0,"2"14,-1 18,0 12,-2 12,-1 11,-1 6,0 1,-1-4,0 0,-1-7,1-11,0-8,4-9,2-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1941.99">848 556,'-1'51,"-2"-1,-2-1,-3 1,-1-1,-3 0,-2-1,-24 58,22-68,2 0,2 1,2 0,-11 78,20-104,1 0,0 1,1-1,0 1,1-1,1 0,0 0,6 15,-6-19,1-1,0 0,1 0,0-1,0 1,1-1,0 0,0 0,1-1,-1 0,1 0,1 0,9 5,-14-9,0 0,1 1,-1-2,0 1,0 0,1-1,-1 1,1-1,0 0,-1-1,1 1,0 0,-1-1,1 0,0 0,-1 0,1 0,0-1,-1 1,1-1,0 0,-1 0,1 0,-1-1,1 1,-1-1,0 0,0 0,0 0,0 0,0-1,0 1,0-1,-1 1,1-1,-1 0,0 0,0 0,0 0,0-1,-1 1,3-6,5-11,-1 0,0 0,-2 0,0-1,-1 0,-1 0,1-33,-5 51,0-1,0 1,-1 0,1-1,-1 1,0 0,0-1,0 1,-1 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 1,-5-5,1 2,0 0,-1 1,0 0,1 0,-1 1,0 0,-13-4,-6 1,1 0,-2 2,-41-2,33 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3027">1933 291,'0'112,"-5"-1,-22 130,-37 183,60-408,2 1,0-1,1 1,0 0,2 0,0-1,1 1,0 0,1-1,1 1,1-1,0 0,1-1,1 1,1-1,0-1,18 26,25 24,-28-38</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24747">10267 741,'10'-15,"0"1,1 0,1 0,25-22,-5 6,499-460,-518 479,-7 4,2 0,-1 0,1 1,0 0,1 1,-1-1,1 1,0 1,1 0,-1 0,12-2,-19 6,0 0,0 0,1 0,-1 0,0 0,0 1,0-1,0 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 1,-1-1,1 1,-1-1,1 1,-1 0,0-1,0 1,0 0,0 0,0 0,0 0,1 4,1 5,0 0,-1 1,0-1,1 18,2 175,-23 204,9-261,4-59,-10 257,15-305</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25107.99">11511 1244,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27020">11828 291,'96'-1,"106"3,-191-1,-1 1,0-1,1 2,-1-1,0 2,-1-1,1 1,-1 1,1 0,-1 0,-1 1,1 0,11 10,-16-12,-1-1,0 0,0 1,0 0,-1 0,1-1,-1 2,0-1,0 0,0 0,-1 1,1-1,-1 1,0-1,0 1,-1-1,1 1,-1 0,0-1,-1 1,1 0,-1-1,0 1,0-1,0 1,0-1,-1 0,0 1,0-1,0 0,0 0,-5 5,-1 1,0 0,-1-1,0 0,0-1,-1 0,-1 0,1-1,-1-1,-13 7,8-4,15-9,0 1,0-1,0 0,0 1,0-1,0 1,1-1,-1 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1-1,1 1,0 0,-1-1,1 1,0 0,0-1,0 1,-1-1,3 2,8 5,1 1,0-1,18 7,-4-1,-9-3,0 1,-1 0,0 1,-1 0,-1 2,0 0,0 0,-1 1,-1 1,-1 0,0 1,-2 0,1 0,-2 1,0 0,8 33,-6-5,-2 0,-2 0,-2 1,-2-1,-7 87,5-130,-1 0,1 1,-1-1,0 0,0 0,0 0,0 0,0 1,-1-2,1 1,-1 0,0 0,0 0,0-1,0 1,-1-1,1 0,-1 0,1 1,-1-2,0 1,1 0,-1 0,0-1,0 0,0 1,-6 0,-5 1,-1-1,0 0,1-1,-31-1,16-1,-290-6,273 6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28650">13389 0,'-9'1,"1"0,0 0,0 1,0-1,0 2,0-1,1 1,-1 0,1 1,-1 0,1 0,0 1,1 0,-1 0,-7 8,-8 9,1 2,-29 42,32-42,-32 44,3 2,-45 89,79-131,0 0,2 1,1 0,1 1,2 0,1 1,1 0,2-1,1 42,4-46,2 0,1 0,13 44,-8-37,7 50,-15-69,-1 0,2 0,-1 0,2 0,0 0,1-1,0 0,1 1,1-2,0 1,0-1,1 0,1-1,0 0,0 0,1-1,14 11,-4-2,-13-13,-1 0,1 0,0-1,0 1,8 3,-13-8,0 0,0 0,0-1,0 1,0 0,0-1,0 0,1 1,-1-1,0 0,0 0,0 0,1 0,-1-1,0 1,0-1,0 1,0-1,0 0,0 0,0 1,0-2,0 1,0 0,2-2,12-12,0-2,-1 0,0 0,-2-2,0 0,-1 0,17-39,-27 53,0 1,0 0,-1-1,0 0,0 1,0-1,-1 1,1-1,-1 0,0 1,0-1,-1 0,1 1,-1-1,0 0,-3-7,0 4,1 1,-1-1,-1 1,0 0,0 0,0 0,0 1,-13-11,6 7,-1 0,0 0,-1 2,0-1,0 2,-1 0,0 1,0 0,-24-5,15 8,-1 1,0 1,-26 2,35 0,-12 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29833">13971 186,'0'0,"0"-1,0 0,0 0,1 0,-1 1,0-1,1 0,-1 0,0 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,0 1,-1-1,1 1,0 0,0-1,-1 1,1-1,0 1,0 0,-1 0,1-1,1 1,27-4,-22 3,167-3,22-3,-189 6,0 0,0 1,0-1,0 1,0 1,0-1,10 3,-14-2,-1 0,1 1,-1-1,0 0,0 1,1-1,-1 1,0 0,0 0,-1-1,1 1,0 0,-1 1,1-1,-1 0,1 0,-1 1,0-1,0 1,0-1,0 1,-1-1,1 4,1 8,0 0,-1 0,-1 0,0 0,-1-1,-1 1,0 0,-1 0,-5 15,-49 126,42-118,-33 68,-104 165,62-118,51-71,28-50</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30349.99">13971 688,'4'-4,"7"-2,9 1,21 0,11 2,11 1,8 1,-4 0,-8 1,-10 0,-9 1,-6-1,-1 0,4 0,-1 0,-6 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30994">15003 212,'-6'3,"0"1,0-1,1 1,-1 0,1 0,0 0,0 1,1 0,0 0,-8 11,3-5,-53 71,5 1,-67 131,124-214,-5 9,0-1,1 1,1 0,-1 0,-2 16,5-23,1 0,0 1,0-1,0 0,0 1,0-1,1 0,-1 1,0-1,1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1-1,0 1,0-1,-1 1,1-1,0 1,4 0,8 5,-1-2,1 0,0 0,0-1,1-1,-1-1,18 2,109-2,-95-2,98-2,-115 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31646.02">15268 239,'0'5,"0"28,0 31,0 31,0 55,0 18,0 4,-5-9,-1-19,-4-30,-1-25,2-23,3-14,-3-11,1-8,1-6,2-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33540.99">1 1932,'113'1,"725"-27,21-69,-380 41,578-15,1505 72,30 0,-981 42,-2 105,-1501-135,498 63,11-43,2027-42,-2444 7,-126 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34584.99">6934 2117,'0'5,"0"28,0 13,0 12,0 10,0 7,0 0,0 4,0-1,0-10,0-7,4-10,2-9,0-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36293">8309 2276,'-1'-1,"1"-1,0 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 1,0-1,0 1,0-1,-1 1,1-1,0 1,-1 0,1-1,-1 1,1 0,-4-1,-44-20,31 16,-120-44,120 45,-1 0,0 2,0 0,0 1,-33 0,46 3,0 1,0-1,0 1,0 1,0-1,1 1,-1 0,1 0,-1 0,1 1,0 0,1 0,-1 0,1 0,0 1,0 0,0 0,0 0,1 0,0 1,-4 8,-1 4,0 0,1 1,1 1,0-1,-3 28,7-39,1 1,0 0,1 0,0-1,0 1,3 15,-3-22,1 1,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0-1,0 1,0 0,0-1,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,1-1,-1 1,0-1,6 1,28 1,1-1,0-1,0-3,47-8,-51 5,0 2,1 1,-1 1,1 3,46 5,-72-5,0 0,-1 1,1 0,-1 1,0 0,0 0,0 0,0 1,0 0,-1 0,0 1,0 0,0 0,0 0,-1 1,0 0,0 0,0 0,4 8,-4-1,1 0,-2 0,1 0,-2 1,0-1,-1 1,0 0,-1 0,0 24,-1-7,0-14,0 1,-1-1,0 0,-7 25,7-36,-1-1,0 0,-1 0,1 0,-1 0,0 0,0 0,0-1,-1 0,0 1,0-1,0 0,0-1,0 1,-1-1,0 0,-9 5,2-3,0 0,0-1,-1-1,1 0,-1 0,0-1,-19 0,-99-5,55-1,56 4,5 1,-1-1,1 0,0-1,0-1,0 0,0-1,0-1,1 0,-28-13,14 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">194 664,'4'0,"2"13,-1 18,1 12,-3 11,-1 10,-1 7,0 0,-1-3,0-1,-1-6,1-11,0-8,4-8,2-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1941.99">879 536,'-1'50,"-2"-2,-2-1,-3 1,-2 0,-2-1,-2-1,-26 56,24-65,1 0,3 0,1 1,-11 75,21-101,1 1,0 0,1 0,0 0,2 0,0 0,0-1,6 15,-6-18,1-2,0 1,2 0,-1-1,0 0,1 0,0 0,1 0,0-2,-1 1,1 0,2 0,8 4,-14-8,1 0,0 1,-1-2,0 1,0 0,1-1,-1 1,1-1,1 0,-2-1,1 1,0 0,-1-1,1 0,0 0,0 0,0 0,0-1,-1 1,1-1,0 0,-1 0,2 0,-2-1,1 1,-1-1,0 0,0 0,0 0,0 0,0-1,1 2,-1-2,-1 1,1-1,-1 0,0 0,0 0,0 0,0-1,-1 2,3-7,6-10,-2-1,0 1,-1 0,-1-2,-1 1,-1 0,1-32,-5 49,0-1,0 1,-1 0,1-1,-1 1,0 1,0-2,0 1,-1 0,1 0,-1 0,0 0,0 0,0 0,0 1,0 0,-6-5,2 2,0 0,-1 1,-1 1,2-1,-1 1,0 0,-14-4,-6 1,1 1,-2 1,-43-2,35 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3027">2005 281,'0'108,"-5"-1,-23 125,-39 177,63-393,2 0,0 0,1 0,0 0,2 1,0-2,1 2,0-1,1-1,1 2,1-2,1 1,0-2,1 2,1-2,1 0,18 24,26 24,-30-37</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24747">10648 715,'11'-15,"-1"2,1-1,2 1,25-22,-5 6,518-444,-537 463,-8 3,2 0,-1 1,2 0,-1 0,1 1,0-1,0 2,0 0,2 0,-2 0,13-2,-20 6,0 0,0 0,1 0,-1 0,0 0,0 1,0-1,0 1,0-1,1 1,-1 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 1,-1-1,1 1,-1-1,1 1,-1 0,0-2,0 2,0 0,1 0,-1 0,0 0,1 4,1 5,0-1,-1 2,0-2,1 18,2 169,-23 197,8-252,5-58,-10 249,15-294</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25107.99">11938 1200,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27020">12267 281,'100'-1,"109"3,-197-1,-2 1,0-1,2 1,-2 0,1 2,-2-1,1 1,0 1,0 0,-1-1,0 2,0 0,12 9,-17-11,-1-1,0 0,0 1,0 0,-1 0,1-1,0 1,-1 0,0 0,0 0,-1 1,1-1,-1 0,0 0,0 1,-1-1,1 1,-1 0,0-1,-1 0,1 1,-1-1,0 1,0-1,0 1,0-2,-1 1,0 1,0-1,-1 0,1 0,-5 4,-1 2,0 0,-2-2,1 1,0-1,-2-1,0 1,0-1,0-1,-14 6,8-3,16-9,0 1,0-1,0 0,0 1,0-1,0 1,1-1,-1 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1 0,-1 0,1-1,-1 0,1 1,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1-1,1 1,0 0,-1-1,1 1,0 0,0-1,0 0,-1 0,3 2,9 5,0 1,1-1,18 6,-4 0,-10-4,1 2,-1 0,-1 0,0 1,-2 1,1 1,-1-1,0 2,-2 0,0 1,-1 0,-2 0,2 1,-3 0,0 0,9 33,-7-6,-1 0,-3 1,-2 0,-2 0,-7 83,5-125,-1 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 1,-1-2,1 1,-2 0,1-1,0 1,0-1,0 1,-1-1,1 0,-1 0,1 1,-1-2,0 1,0 0,0 0,0-1,0-1,0 2,-6 0,-6 1,0-1,-1 0,2-1,-33-1,17-1,-301-6,283 6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28650">13886 0,'-9'1,"0"0,1 0,0 1,0-1,-1 2,1-1,1 1,-2-1,2 2,-1 0,1 0,-1 1,2 0,-1-1,-8 9,-7 8,0 2,-30 41,33-41,-33 43,4 1,-48 87,83-127,-1 0,3 1,0 0,2 1,2 0,1 0,0 1,3-1,1 41,4-45,3 0,0 0,13 43,-7-37,6 49,-15-66,-1-1,3 1,-2-1,2 1,0-1,1 0,0 0,2 0,0-1,0 0,0 0,2-1,0 0,0 0,1-1,0 0,15 10,-4-2,-14-12,-1 0,1 0,1-1,-1 0,8 4,-12-8,-1 0,0 0,0-1,0 1,0 0,0-1,0 0,1 1,-1-1,0 0,0 0,0 0,2 0,-2-1,0 1,0-1,0 1,0-1,0 0,0 0,0 1,0-2,0 1,0 0,3-2,11-11,1-3,-2 1,1 0,-3-3,1 1,-2 0,18-38,-28 51,0 1,1 0,-2-1,0 0,0 2,0-2,-1 1,1-1,-1 0,0 1,0 0,-1-1,1 1,-1-1,0 0,-4-6,1 3,1 1,-1 0,-1 0,0 0,0 0,-1 0,1 2,-14-12,7 8,-1-1,-1 0,0 3,-1-2,1 2,-2 0,0 2,1-1,-26-5,17 8,-2 1,0 1,-27 2,36 0,-12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29833">14490 179,'0'0,"0"-1,0 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,0 1,-1-1,1 1,0 0,0-1,-1 1,1-1,0 1,0 0,-1 0,1-1,1 1,28-4,-22 3,172-3,23-2,-195 5,-1 0,0 1,0-1,1 1,-1 1,0-1,11 3,-15-3,-1 1,1 1,-1-1,0 0,0 1,1-1,0 1,-1 0,0 0,-1-1,1 1,0 0,-1 1,1-1,-1 0,1 0,-1 0,0 0,0 1,0-1,0 1,-1-1,1 4,1 7,0 1,0-1,-2 1,0-1,-2 0,0 0,0 1,-1-1,-5 15,-51 122,43-114,-34 65,-107 159,63-113,54-69,29-48</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30349.99">14490 664,'4'-4,"7"-2,10 1,22 0,10 3,13 0,7 1,-3 0,-9 1,-10 0,-10 1,-5-1,-2 0,4 0,0 0,-7 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30994">15560 205,'-6'2,"0"2,-1-1,2 1,-1 0,1 0,0 0,-1 0,2 1,0 0,-8 10,2-4,-54 68,5 1,-70 127,129-207,-5 8,0 0,1 1,1-1,-1 1,-3 15,6-22,1 0,0 1,0-1,0 0,0 1,0-1,1 0,-1 1,0-2,1 1,0 1,0-1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1-1,0 0,0 0,-1 1,1-1,0 1,4 0,9 5,-2-2,2 0,0-1,-1 0,2-1,-2-1,19 2,114-2,-100-2,103-2,-120 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31646.02">15835 231,'0'4,"0"28,0 30,0 30,0 52,0 18,0 4,-5-8,-2-20,-3-28,-1-24,1-22,4-14,-3-10,1-8,0-6,3-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33540.99">1 1864,'117'1,"752"-26,22-67,-394 40,599-15,1561 70,32 0,-1019 41,-1 100,-1557-129,517 60,11-41,2102-41,-2535 7,-130 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34584.99">7191 2042,'0'5,"0"27,0 12,0 12,0 10,0 6,0 1,0 3,0-1,0-9,0-8,5-8,1-10,0-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36293">8617 2196,'-1'-1,"1"-1,0 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 1,0-1,0 1,0-1,-1 1,1 0,0 0,-1 0,1-1,-1 1,1 0,-4-1,-46-19,32 15,-124-42,124 43,0 0,-1 2,0 0,0 1,-33 0,46 3,1 1,0-1,0 1,-1 1,1-1,1 1,-1 0,1 0,-2 0,2 0,0 1,1 0,-1 0,1 0,-1 1,1-1,0 1,0 0,1 0,0 1,-5 7,0 5,0-1,1 1,0 2,1-2,-3 27,7-37,1 1,0-1,1 1,0-1,0 0,3 16,-3-23,1 2,0-1,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,0-1,0 0,1 1,-1-1,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,1-1,-1 1,0-1,7 1,28 1,1-1,1-1,-1-3,49-8,-52 6,-1 1,1 1,-1 1,2 3,46 5,-73-5,-1 0,-1 1,2-1,-2 2,0 0,0 0,1 0,-1 1,0 0,-1 0,1 0,-1 1,0 0,0 0,0 1,-1-1,0 1,0 0,4 8,-3-2,0 1,-2-1,1 1,-2 0,0 0,-1 0,1 1,-2-1,0 24,-1-7,0-14,0 2,-1-2,0 0,-8 25,8-35,-1-1,0-1,-1 1,1 0,-1 0,0 0,0-1,-1 0,0 0,0 1,0-1,0 0,0-1,0 0,-2 0,1 0,-9 5,1-3,1 0,-1-2,0 0,0 0,0 0,-1-1,-19 0,-103-5,58-1,57 4,5 1,0-1,0 0,1-1,-1-1,0 0,1 0,-1-2,2 0,-30-13,15 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8507,13 +8607,13 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 873,'6'-1,"0"-1,0 0,0 0,0-1,-1 1,1-1,-1-1,1 1,-1-1,0 0,4-5,8-4,48-32,20-13,-2-4,109-106,-185 160,15-13,-22 21,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,1 0,-1 0,1 0,-1 1,1-1,-1 0,0 1,1-1,-1 0,1 1,-1-1,0 0,0 1,1-1,-1 1,0-1,1 0,-1 1,0-1,0 1,0-1,0 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 1,-1 0,6 35,-2 1,-1-1,-7 66,2 1,22 240,-14-267,7 13,1 22,-12-88</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1014.99">1139 1376,'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3315.99">2356 212,'-8'1,"1"0,0 0,0 1,0 0,0 0,0 1,0-1,1 1,-1 1,1 0,0-1,-10 9,-8 8,-34 37,42-40,-6 5,-5 5,1 1,-34 47,54-66,0 1,0 1,1-1,0 1,1 0,0 0,1 0,0 1,1-1,0 1,0 0,1 17,3-9,-2 0,0 0,-2 0,0 0,-8 34,-2-12,-6 50,15-77,2 1,0 0,0 0,2-1,0 1,5 24,-4-35,0 0,0 1,0-2,1 1,-1 0,1 0,1-1,-1 0,1 1,-1-1,1-1,0 1,1 0,-1-1,1 0,-1 0,1 0,0-1,0 0,8 3,12 3,1 0,0-2,28 3,-2 0,128 40,-179-49,1 1,0-1,0 0,0 0,1 1,-1-1,0-1,0 1,0 0,0 0,0-1,0 1,0-1,0 1,-1-1,1 0,0 0,0 0,0 0,-1 0,1 0,-1-1,1 1,-1-1,1 1,-1-1,0 1,1-1,0-2,3-5,-1 0,0-1,0 1,3-19,3-6,-5 23,1-3,0-1,-1 0,-1 0,0-1,2-22,-5 34,-1 0,0 0,-1 0,1 0,-1 0,1 1,-1-1,0 0,-1 0,1 1,-1-1,1 1,-1-1,0 1,-1 0,1 0,0 0,-1 0,0 0,1 0,-1 1,0-1,-1 1,1 0,0 0,-1 0,-5-2,-121-42,99 35,0 1,0 2,-1 0,0 3,0 1,0 1,-57 2,67 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4151">3600 159,'-9'16,"-1"-1,0-1,-1 0,-23 24,-3 2,-182 237,168-197,48-75,0 1,1 0,-1 0,1 0,0 1,1-1,-1 0,1 1,1-1,-1 1,1 12,1-16,0 0,0-1,0 1,1 0,-1 0,1-1,-1 1,1-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1 0,1-1,0 1,3 1,59 20,-52-19,37 11,1-1,1-3,83 7,-96-15,-14-1,1-1,-1-1,37-4,-55 3,0 0,-1-1,1 1,-1-1,1-1,-1 1,0-1,0-1,0 1,0-1,-1 0,1 0,-1 0,0-1,0 0,-1 0,0 0,5-6,19-44,-5-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4829.99">4261 0,'-1'4,"0"0,-1-1,1 1,-1-1,1 1,-1-1,0 0,0 1,-1-1,1 0,0 0,-4 2,-5 8,-299 423,266-364,4 2,3 1,3 2,-34 115,48-124,-18 69,34-119,1 1,1 0,1 0,0 0,4 25,-3-41,0 0,1-1,-1 1,1-1,0 1,0-1,0 0,0 1,0-1,1 0,-1 1,0-1,3 2,9 7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6907.99">4817 265,'-1'1,"-1"-1,1 0,0 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,1 0,-1-1,0 1,0 0,0 0,1 0,-1 0,0-1,1 1,-1 2,-4 3,-48 67,4 2,3 2,-39 91,68-134,2 0,1 2,2-1,1 1,2 1,1 0,-3 48,7-38,-18 81,13-87,1 1,-1 52,9-86,0 0,0 0,1 0,0 0,1 0,0 0,0 0,1-1,-1 1,2-1,4 9,-6-13,0 1,1-1,0 0,-1 0,1 0,1 0,-1 0,0-1,0 1,1-1,0 0,-1 0,1 0,0-1,0 1,0-1,0 0,0 0,0 0,0-1,0 0,1 1,-1-1,5-1,10-2,1 0,-1-2,1 0,-1-1,-1-1,1-1,22-13,-25 12,-1 0,0-1,-1 0,0-1,0-1,-1 0,-1-1,18-24,-20 19,-1-1,-1 0,-1-1,0 1,-2-1,7-40,-8 35,1 0,1 0,19-45,-15 53,-2-1,0-1,-1 1,0-1,-2 0,0 0,-2-1,0 1,1-31,-5 9,2 4,-8-60,5 85,0 0,-1 0,-1 1,0-1,0 1,-1 0,0 0,-14-20,11 20,0 1,0 0,-1 1,0 0,-1 0,0 1,0 0,-1 1,0 0,0 0,0 2,-1-1,0 1,-13-3,-22-13,38 17,1 0,-1 0,1 1,-1 0,0 0,-13-2,18 6,10 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8537">6272 344,'-1'1,"1"-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 1,-1-1,0 0,0 0,1 0,-27 9,-95 1,-167-7,147-4,101 0,-131 8,166-7,-1 1,1 0,-1 0,0 1,1 0,0 0,-1 0,1 1,0-1,0 1,1 1,-1-1,1 1,-1-1,1 1,0 0,0 1,1-1,-5 7,6-7,0 1,0-1,0 1,1 0,-1 0,1 0,0 0,1-1,-1 1,1 0,0 1,0-1,1 0,-1-1,1 1,0 0,0 0,1 0,0 0,0-1,4 8,-3-7,0 0,1 0,-1-1,1 1,0-1,1 0,-1 0,1-1,0 1,0-1,0 0,0 0,0-1,0 1,1-1,-1-1,7 2,14 3,1-2,42 3,-6-1,-36-2,5 0,1 2,-1 1,36 13,-60-17,1 1,0 0,-1 0,0 1,0 0,0 0,-1 1,0 0,0 0,0 1,-1 0,0 0,0 0,-1 1,9 16,-3 2,-1 0,0 1,-2 0,-2 1,0 0,-2 0,0 0,-3 0,0 1,-1-1,-8 50,5-70,0 0,-1 1,0-1,0-1,-1 1,1 0,-2-1,1 0,-1-1,0 1,0-1,-1 0,0 0,0-1,-12 7,3-3,0 0,0 0,-1-2,0 0,-1-1,-28 6,4-7,0-1,-1-2,1-2,-47-6,75 5,1 0,-1-1,1 0,0-1,-1-1,1 0,1-1,-1 0,1-1,0 0,0-1,-16-11,12 3,0 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 836,'6'-1,"0"-1,1 0,-1 0,0 0,-1 0,2-1,-2-1,1 1,-1-1,1 0,3-4,9-5,49-30,22-12,-3-5,114-101,-193 154,16-13,-23 20,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,1 0,-1 0,1 0,-1 1,1-1,-1 0,0 1,1-1,-1 0,2 0,-2 0,0 0,0 1,1-1,-1 1,0-1,1 0,-1 1,0-1,0 1,0-1,0 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 1,-1 0,6 34,-2 0,-1-1,-7 64,2 1,22 229,-13-255,6 12,2 22,-13-85</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1014.99">1185 1318,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3315.99">2451 203,'-8'1,"1"0,-1 0,1 1,0 0,0 0,-1 1,1-2,1 2,-2 1,2 0,0-1,-11 8,-8 9,-35 34,43-38,-5 5,-7 5,2 1,-35 45,56-63,-1 0,1 2,1-2,0 2,1-1,-1 1,2-1,0 2,1-2,0 2,0-1,1 17,3-9,-2 0,0 1,-2-1,0 0,-9 33,-1-12,-7 48,16-74,2 2,0-1,0 0,2 0,0 0,5 23,-4-33,0 0,1 1,-1-2,1 0,-1 1,1 0,1-1,-1 0,1 0,0 0,0-1,0 1,1 0,-1-1,1-1,0 1,0 0,0-1,0 0,9 3,12 2,1 1,0-2,29 2,-2 1,133 38,-186-47,2 1,-1-1,0 0,0 0,1 1,-1-1,0-1,0 1,0 0,0 0,0-1,0 1,1-1,-1 1,-1-1,1 0,0 0,0 0,0 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1-1,0 1,2-1,-1-2,3-5,-1 1,0-2,0 2,4-19,2-6,-5 23,1-4,1 0,-2 0,-1-1,0 0,2-22,-5 34,-1-1,0 0,-1 0,1 0,-1 0,1 2,-1-2,0 0,-1 0,1 1,-1-1,1 2,-1-2,0 1,-1 0,1 0,0 0,-1 0,-1 0,2 1,-1 0,0-1,-1 1,1 0,0 0,-2 0,-4-2,-126-40,103 34,-1 0,1 2,-1 1,0 2,-1 1,1 1,-60 2,70 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4151">3746 152,'-10'16,"0"-2,0-1,-2 1,-23 22,-4 2,-189 228,175-190,50-71,0 1,1 0,-1-1,1 1,0 1,1-1,-1-1,0 2,2-1,-1 1,1 11,1-15,1-1,-1 0,0 1,1 0,-1 0,1-1,-1 1,1-1,0 1,0-2,0 1,0 0,0 0,0 0,2 0,-2 0,1-1,0 1,3 1,62 19,-55-18,39 10,1-1,1-2,87 6,-100-14,-15-1,1-1,-1-1,38-4,-57 3,1 0,-2-1,1 1,-1-1,2-1,-2 2,0-2,0-1,1 1,-1-1,-1 0,1 0,0 1,-1-2,0 0,-1 0,0 1,6-7,19-42,-5-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4829.99">4433 0,'-1'4,"0"0,-1-1,1 0,-1 0,1 1,-1-1,0 0,0 1,-1-1,1-1,0 1,-5 2,-4 8,-312 404,278-348,3 2,3 1,4 1,-36 111,51-119,-20 67,36-115,1 1,1 0,1 1,0-1,4 24,-3-39,0 0,1-1,-1 0,1 0,0 1,0-1,0 0,0 1,0-1,1 0,-1 1,0-1,3 1,10 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6907.99">5012 254,'-1'1,"-1"-1,1 0,0 0,0 1,0-1,0 1,0-1,0 1,-1-1,1 1,1 0,-1-1,0 1,0-1,0 1,1 0,-1 0,0-1,1 1,-1 2,-4 3,-50 64,4 2,3 1,-40 88,70-128,2-1,2 3,1-2,2 2,1 0,2 1,-3 45,6-36,-17 78,12-84,2 1,-1 50,9-82,0 0,0-1,1 1,0 0,1-1,0 1,0 0,1-2,-1 2,2-1,5 8,-7-12,0 1,1-1,0-1,-1 1,1 0,1 0,-1 0,1-1,-1 1,1-1,0 0,-1-1,1 1,0-1,1 1,-1-1,0 0,0 0,0 0,0-1,1 0,0 1,-1-1,5-1,11-2,1 0,-1-1,0-1,0-1,-1-1,1 0,22-13,-25 11,-1 0,-1 0,0-1,-1 0,1-2,-2 1,0-2,18-22,-20 17,-2 0,-1 0,0-1,-1 1,-2-1,8-39,-9 34,1 0,1 0,20-43,-15 51,-3-1,0-1,-1 0,1 0,-3 0,0 0,-2-1,0 0,2-29,-6 9,2 4,-9-58,6 81,0 1,-1-1,-1 2,0-2,0 2,-2-1,1 1,-15-20,12 20,0 0,-1 0,0 2,0-1,-2 1,1 0,-1 0,0 1,0 1,-1-1,1 2,-2 0,1 0,-14-3,-23-12,39 16,2 0,-1 1,0 0,0 0,0 0,-14-2,19 6,10 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8537">6526 329,'-1'1,"1"-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 1,-1-1,0 0,0 0,1 0,-28 9,-99 0,-174-6,154-4,104 0,-136 8,173-7,-1 1,0 0,0 0,0 1,1 0,0 0,-2 0,2 0,0 0,0 1,1 1,-2-1,2 1,-1-1,1 0,0 1,0 1,0-1,-4 6,6-6,0 1,0-1,0 1,1-1,-1 1,1 0,0 0,1-1,-2 0,2 1,0 1,0-1,2 0,-2-2,1 2,0 0,0 0,1 0,0-1,0 0,4 8,-3-8,0 1,2 0,-2-1,1 1,0-2,1 1,-1 0,2-1,-1 1,0-1,0 0,0-1,1 0,-1 1,1-1,-1-1,8 2,14 3,1-2,44 2,-7 0,-37-2,6 0,0 1,-1 2,38 12,-63-16,2 1,-1 0,-1 0,1 0,-1 1,0 0,0 1,-1-1,0 1,0 1,0 0,-1-1,0 1,-1 1,10 15,-4 2,0-1,-1 2,-1 0,-3 1,0 0,-2 0,0-1,-3 1,0 1,-1-1,-8 48,5-68,0 1,-1 1,0-2,-1 0,0 1,1-1,-2 0,1 0,-2-2,1 2,0-1,-1 0,-1-1,1 0,-13 7,4-4,-1 1,0-1,0-1,-1 0,-1-1,-29 5,5-6,-1-1,-1-2,1-2,-48-6,77 5,2 0,-2-1,2 0,-1-1,0-1,0 1,2-2,-2 0,2-1,-1 1,1-2,-18-10,14 2,-1 4</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8847,13 +8947,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7A3694-7BF9-49B8-BE95-175AC781497C}">
   <dimension ref="L1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:S7"/>
+    <sheetView topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="12:19" x14ac:dyDescent="0.3">
       <c r="M1">
         <v>0</v>
       </c>
@@ -8873,7 +8973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L2" t="s">
         <v>0</v>
       </c>
@@ -8899,7 +8999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L3" s="1">
         <v>0.8</v>
       </c>
@@ -8912,7 +9012,7 @@
         <v>20</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
+        <f>O2*POWER($L$3,O1)</f>
         <v>-128.00000000000003</v>
       </c>
       <c r="P3">
@@ -8932,7 +9032,7 @@
         <v>0.23199999999999932</v>
       </c>
     </row>
-    <row r="5" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
         <v>2</v>
       </c>
@@ -8940,7 +9040,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L6" t="s">
         <v>3</v>
       </c>
@@ -8948,7 +9048,7 @@
         <v>2.456</v>
       </c>
     </row>
-    <row r="7" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L7" t="s">
         <v>4</v>
       </c>
@@ -8970,9 +9070,9 @@
       <selection activeCell="L20" sqref="L20:L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:19" x14ac:dyDescent="0.3">
       <c r="M1">
         <v>0</v>
       </c>
@@ -8992,7 +9092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L2" t="s">
         <v>0</v>
       </c>
@@ -9018,7 +9118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L3" s="1">
         <v>0.6</v>
       </c>
@@ -9051,7 +9151,7 @@
         <v>3.4640000000000128</v>
       </c>
     </row>
-    <row r="5" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
         <v>2</v>
       </c>
@@ -9059,7 +9159,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L6" t="s">
         <v>5</v>
       </c>
@@ -9067,7 +9167,7 @@
         <v>1.288</v>
       </c>
     </row>
-    <row r="7" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L7" t="s">
         <v>3</v>
       </c>
@@ -9075,7 +9175,7 @@
         <v>2.456</v>
       </c>
     </row>
-    <row r="8" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L8" t="s">
         <v>6</v>
       </c>
@@ -9083,7 +9183,7 @@
         <v>3.464</v>
       </c>
     </row>
-    <row r="9" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L9" t="s">
         <v>4</v>
       </c>
@@ -9091,7 +9191,7 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="11" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L11" t="s">
         <v>7</v>
       </c>
@@ -9100,7 +9200,7 @@
         <v>0.14880000000000002</v>
       </c>
     </row>
-    <row r="12" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L12" t="s">
         <v>8</v>
       </c>
@@ -9109,7 +9209,7 @@
         <v>0.37440000000000001</v>
       </c>
     </row>
-    <row r="13" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L13" t="s">
         <v>9</v>
       </c>
@@ -9118,7 +9218,7 @@
         <v>0.59199999999999997</v>
       </c>
     </row>
-    <row r="14" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>14</v>
       </c>
@@ -9133,7 +9233,7 @@
         <v>0.36960000000000004</v>
       </c>
     </row>
-    <row r="15" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
         <v>15</v>
       </c>
@@ -9141,7 +9241,7 @@
         <v>1.4847999999999999</v>
       </c>
     </row>
-    <row r="16" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:19" x14ac:dyDescent="0.3">
       <c r="L16" t="s">
         <v>11</v>
       </c>
@@ -9150,7 +9250,7 @@
         <v>1.4847999999999999</v>
       </c>
     </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>16</v>
       </c>
@@ -9159,7 +9259,7 @@
         <v>0.13866666666666663</v>
       </c>
     </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>17</v>
       </c>
@@ -9168,7 +9268,7 @@
         <v>0.55466666666666653</v>
       </c>
     </row>
-    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:12" x14ac:dyDescent="0.3">
       <c r="K20" t="s">
         <v>12</v>
       </c>
@@ -9177,7 +9277,7 @@
         <v>1.3674666666666664</v>
       </c>
     </row>
-    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:12" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
         <v>13</v>
       </c>
@@ -9196,13 +9296,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43F7F71-6459-471E-9869-783D11A5D2B3}">
   <dimension ref="B31:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>18</v>
       </c>
@@ -9213,7 +9313,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>0.17280000000000001</v>
       </c>
@@ -9221,7 +9321,7 @@
         <v>1.3674666666666664</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1.0688</v>
       </c>
@@ -9229,9 +9329,219 @@
         <v>1.6234666666666664</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>1.4847999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD922335-4BEA-4886-84E5-472CBFE2E852}">
+  <dimension ref="J2:S17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>4</v>
+      </c>
+      <c r="R2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0.2</v>
+      </c>
+      <c r="N3">
+        <v>25</v>
+      </c>
+      <c r="O3">
+        <v>-200</v>
+      </c>
+      <c r="P3">
+        <v>675</v>
+      </c>
+      <c r="Q3">
+        <v>-900</v>
+      </c>
+      <c r="R3">
+        <v>400</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="L4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="M4">
+        <f>M3</f>
+        <v>0.2</v>
+      </c>
+      <c r="N4">
+        <f>N3*POWER($L$4,N2)</f>
+        <v>17.5</v>
+      </c>
+      <c r="O4">
+        <f>O3*POWER($L$4,O2)</f>
+        <v>-97.999999999999986</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:R4" si="0">P3*POWER($L$4,P2)</f>
+        <v>231.52499999999995</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>-216.08999999999992</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>67.22799999999998</v>
+      </c>
+      <c r="S4" s="2">
+        <f>SUM(M4:R4)</f>
+        <v>2.363000000000028</v>
+      </c>
+    </row>
+    <row r="7" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0.2</v>
+      </c>
+      <c r="N8">
+        <f>$J$9*(L8+L9)/2</f>
+        <v>7.4450000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>0.1</v>
+      </c>
+      <c r="L9">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="N9">
+        <f>$J$9*(L9+L10)/2</f>
+        <v>0.12884999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>0.2</v>
+      </c>
+      <c r="L10">
+        <v>1.288</v>
+      </c>
+      <c r="N10">
+        <f>$J$9*(L10+L11)/2</f>
+        <v>0.14475000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="L11">
+        <v>1.607</v>
+      </c>
+      <c r="N11">
+        <f>$J$9*(L11+L12)/2</f>
+        <v>0.20315</v>
+      </c>
+    </row>
+    <row r="12" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>0.4</v>
+      </c>
+      <c r="L12">
+        <v>2.456</v>
+      </c>
+      <c r="N12">
+        <f>$J$9*(L12+L13)/2</f>
+        <v>0.28905000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>0.5</v>
+      </c>
+      <c r="L13">
+        <v>3.3250000000000002</v>
+      </c>
+      <c r="N13">
+        <f>$J$9*(L13+L14)/2</f>
+        <v>0.33945000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>0.6</v>
+      </c>
+      <c r="L14">
+        <v>3.464</v>
+      </c>
+      <c r="N14">
+        <f>$J$9*(L14+L15)/2</f>
+        <v>0.29135</v>
+      </c>
+    </row>
+    <row r="15" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>0.7</v>
+      </c>
+      <c r="L15">
+        <v>2.363</v>
+      </c>
+      <c r="N15">
+        <f>$J$9*(L15+L16)/2</f>
+        <v>0.12975</v>
+      </c>
+    </row>
+    <row r="16" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>0.8</v>
+      </c>
+      <c r="L16">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <f>SUM(N8:N15)</f>
+        <v>1.6008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>